<commit_message>
Verification of all lines finished. Some lines are questionable and will be rerun.
</commit_message>
<xml_diff>
--- a/vrp_dss/Solve Times Summary.xlsx
+++ b/vrp_dss/Solve Times Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Aaron\Documents\Git Repositories\VRP-DSS\vrp_dss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\great\Documents\GitHub\VRP-DSS\vrp_dss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8369DE26-365A-4E68-AD82-DEA9C4168EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59BD14C-FA27-4769-98E0-B50078B9C5B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="196">
   <si>
     <t># Customers</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>CPLEX Generated Text File</t>
+  </si>
+  <si>
+    <t>Math Routes</t>
   </si>
   <si>
     <t>Math Objective (evaluated by meta)</t>
@@ -113,10 +116,13 @@
 Solve time: 641</t>
   </si>
   <si>
-    <t xml:space="preserve">11 metre (capacity 30):
+    <t>{0: [[(7, 5), (8, 2), (3, 2), (1, 5), (5, 3), (4, 6), (2, 1), (6, 6)]], 1: [[(9, 9)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+6 (6) -&gt; 9 (9)
+11 metre (capacity 30):
 7 (5) -&gt; 8 (2) -&gt; 3 (2) -&gt; 1 (5) -&gt; 5 (3) -&gt; 4 (6) -&gt; 2 (1)
-8 metre (capacity 22):
-6 (6) -&gt; 9 (9)
 </t>
   </si>
   <si>
@@ -149,6 +155,17 @@
 Solve time: 903</t>
   </si>
   <si>
+    <t>{0: [], 1: [[(6, 6), (1, 7), (2, 3)]], 2: [[(8, 8), (4, 2), (3, 6), (5, 3), (7, 8), (9, 1)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+11 metre (capacity 30):
+8 (8) -&gt; 4 (2) -&gt; 3 (6) -&gt; 5 (3) -&gt; 7 (8) -&gt; 9 (1)
+8 metre (capacity 22):
+2 (3) -&gt; 1 (7) -&gt; 6 (6)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 5 pallets demand and window 21-22 at (52.242025697, -37.558585418) and average unload time 0.060925028
 Customer 2 has 2 pallets demand and window 0-24 at (80.08666625, 89.79908273) and average unload time 0.060846624
@@ -176,6 +193,15 @@
 Vehicle SP2 travels from 8 to 3 to deliver 3 pallets. Expected unload start time is 5.264703289
 Objective value: 943.34840135
 Solve time: 630</t>
+  </si>
+  <si>
+    <t>{0: [[(6, 3), (9, 4), (1, 5)], [(2, 2), (5, 1), (8, 2), (3, 3), (7, 3), (4, 1)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+2 (2) -&gt; 5 (1) -&gt; 8 (2) -&gt; 3 (3) -&gt; 7 (3) -&gt; 4 (1) -&gt; 9 (4)
+6 (3) -&gt; 1 (5)
+</t>
   </si>
   <si>
     <t>Input:
@@ -208,6 +234,18 @@
 Solve time: 1531</t>
   </si>
   <si>
+    <t>{0: [[(2, 7), (4, 8)]], 1: [[(5, 5), (8, 8)]], 2: [[(6, 2), (1, 3), (7, 4), (3, 7), (9, 5)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+2 (7) -&gt; 4 (8)
+Rigid (capacity 16):
+8 (8) -&gt; 5 (5)
+8 metre (capacity 22):
+6 (2) -&gt; 1 (3) -&gt; 7 (4) -&gt; 3 (7) -&gt; 9 (5)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 7 pallets demand and window 21-22 at (-89.28625092, -19.528047969) and average unload time 0.088997757
 Customer 2 has 4 pallets demand and window 0-24 at (-79.777105548, -9.173939447) and average unload time 0.037538711
@@ -237,6 +275,17 @@
 Solve time: 2543</t>
   </si>
   <si>
+    <t>{0: [[(6, 5), (5, 4), (3, 7), (9, 4), (4, 2)], [(8, 5), (7, 3), (1, 7), (2, 4)]], 1: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+8 (5) -&gt; 7 (3)
+8 metre (capacity 22):
+9 (4) -&gt; 3 (7) -&gt; 5 (4) -&gt; 6 (5)
+4 (2) -&gt; 1 (7) -&gt; 2 (4)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 1 pallets demand and window 0-24 at (-28.036245659, -17.225052327) and average unload time 0.085209225
 Customer 2 has 2 pallets demand and window 0-24 at (6.541253413, 26.809224103) and average unload time 0.083426014
@@ -266,6 +315,16 @@
 Solve time: 3773</t>
   </si>
   <si>
+    <t>{0: [[(5, 8), (3, 8), (8, 3), (2, 2)]], 1: [], 2: [[(7, 8), (6, 3), (1, 1), (4, 2), (9, 2)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+9 (2) -&gt; 4 (2) -&gt; 1 (1) -&gt; 6 (3) -&gt; 7 (8)
+8 metre (capacity 22):
+5 (8) -&gt; 3 (8) -&gt; 8 (3) -&gt; 2 (2)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 7 pallets demand and window 0-24 at (-98.295543185, 28.838680271) and average unload time 0.083568028
 Customer 2 has 5 pallets demand and window 0-24 at (96.821349354, 63.117438185) and average unload time 0.154661074
@@ -293,6 +352,16 @@
 Vehicle SP2 travels from 7 to DepotReturn to deliver 0 pallets. Expected unload start time is 6.499013009
 Objective value: 883.239440793
 Solve time: 3816</t>
+  </si>
+  <si>
+    <t>{0: [[(2, 5), (9, 2), (3, 4), (8, 5), (6, 5)]], 1: [[(5, 4), (4, 1), (1, 7), (7, 4)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+6 (5) -&gt; 8 (5) -&gt; 3 (4) -&gt; 9 (2) -&gt; 2 (5)
+Rigid (capacity 16):
+7 (4) -&gt; 1 (7) -&gt; 4 (1) -&gt; 5 (4)
+</t>
   </si>
   <si>
     <t>Input:
@@ -326,6 +395,18 @@
 Solve time: 2016</t>
   </si>
   <si>
+    <t>{0: [[(7, 6), (6, 8)]], 1: [[(9, 3), (8, 8), (5, 7), (4, 8)]], 2: [[(2, 6), (1, 3), (3, 4), (7, 2)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+1 (3) -&gt; 3 (4) -&gt; 2 (6)
+Rigid (capacity 16):
+6 (8) -&gt; 7 (8)
+11 metre (capacity 30):
+9 (3) -&gt; 8 (8) -&gt; 5 (7) -&gt; 4 (8)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 1 pallets demand and window 0-24 at (11.834520083, -34.69497582) and average unload time 0.12405363
 Customer 2 has 3 pallets demand and window 0-24 at (41.605570864, -6.837804372) and average unload time 0.084174776
@@ -356,6 +437,17 @@
 Solve time: 1630</t>
   </si>
   <si>
+    <t>{0: [[(1, 1), (3, 2), (6, 7), (8, 4)], [(7, 2), (9, 2), (2, 3), (5, 6)]], 1: [[(4, 7)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+4 (7)
+Rigid (capacity 16):
+1 (1) -&gt; 3 (2) -&gt; 6 (7) -&gt; 8 (4)
+7 (2) -&gt; 9 (2) -&gt; 2 (3) -&gt; 5 (6)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 4 pallets demand and window 0-24 at (-99.384142277, 45.343950296) and average unload time 0.032665165
 Customer 2 has 6 pallets demand and window 17-18 at (26.906318094, 93.004308817) and average unload time 0.072299486
@@ -382,6 +474,16 @@
 Vehicle SP1 travels from 9 to 2 to deliver 6 pallets. Expected unload start time is 17.857478693
 Objective value: 566.836248779
 Solve time: 976</t>
+  </si>
+  <si>
+    <t>{0: [[(8, 1), (7, 1), (3, 3), (5, 4), (9, 4), (2, 6), (4, 1), (1, 4), (6, 5)]], 1: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+8 metre (capacity 22):
+4 (1) -&gt; 1 (4) -&gt; 6 (5)
+8 (1) -&gt; 7 (1) -&gt; 5 (4) -&gt; 9 (4) -&gt; 2 (6) -&gt; 3 (3)
+</t>
   </si>
   <si>
     <t>Input:
@@ -420,6 +522,16 @@
 Solve time: 2359</t>
   </si>
   <si>
+    <t>{0: [[(9, 3), (12, 3), (5, 4), (4, 5), (2, 7), (10, 7), (3, 1)]], 1: [[(7, 2), (1, 2), (11, 3), (8, 2), (6, 5), (9, 2)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+2 (7) -&gt; 10 (7) -&gt; 7 (2)
+11 metre (capacity 30):
+3 (1) -&gt; 4 (5) -&gt; 5 (4) -&gt; 12 (3) -&gt; 9 (5) -&gt; 6 (5) -&gt; 8 (2) -&gt; 11 (3) -&gt; 1 (2)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 2 pallets demand and window 0-24 at (86.117323523, 65.481263002) and average unload time 0.088372233
 Customer 2 has 1 pallets demand and window 0-24 at (11.386501748, 9.118109776) and average unload time 0.135651791
@@ -455,6 +567,16 @@
 Solve time: 8640</t>
   </si>
   <si>
+    <t>{0: [[(2, 1), (7, 3), (11, 2), (1, 2), (5, 4), (4, 4), (6, 3)]], 1: [[(3, 3), (12, 2), (10, 2), (8, 3), (9, 1)]], 2: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+3 (3) -&gt; 12 (2) -&gt; 10 (2) -&gt; 8 (3) -&gt; 9 (1)
+8 metre (capacity 22):
+2 (1) -&gt; 7 (3) -&gt; 11 (2) -&gt; 1 (2) -&gt; 5 (4) -&gt; 4 (4) -&gt; 6 (3)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 4 pallets demand and window 0-24 at (-95.616703662, -14.90802781) and average unload time 0.164037861
 Customer 2 has 1 pallets demand and window 0-24 at (60.574613574, 15.084761202) and average unload time 0.046722152
@@ -490,6 +612,16 @@
 Solve time: 1565</t>
   </si>
   <si>
+    <t>{0: [[(11, 4), (3, 5), (2, 1), (4, 1), (10, 3), (6, 2), (9, 3)]], 1: [], 2: [[(8, 2), (7, 1), (5, 3), (1, 4), (12, 5)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+11 (4) -&gt; 3 (5) -&gt; 2 (1) -&gt; 4 (1) -&gt; 10 (3) -&gt; 6 (2) -&gt; 9 (3)
+Rigid (capacity 16):
+8 (2) -&gt; 7 (1) -&gt; 5 (3) -&gt; 1 (4) -&gt; 12 (5)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 4 pallets demand and window 0-24 at (-75.904887286, -33.901246897) and average unload time 0.036907913
 Customer 2 has 6 pallets demand and window 0-24 at (35.865499648, 34.318194739) and average unload time 0.099555942
@@ -525,6 +657,15 @@
 Solve time: 5289</t>
   </si>
   <si>
+    <t>{0: [[(9, 3), (8, 5), (6, 7), (2, 6), (11, 8)], [(3, 1), (12, 1), (7, 4), (1, 4), (5, 8), (10, 5), (4, 5)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+9 (3) -&gt; 8 (5) -&gt; 6 (7) -&gt; 2 (6) -&gt; 11 (8)
+3 (1) -&gt; 12 (1) -&gt; 7 (4) -&gt; 1 (4) -&gt; 5 (8) -&gt; 10 (5) -&gt; 4 (5)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 4 pallets demand and window 0-24 at (92.548667144, -73.357619901) and average unload time 0.017126286
 Customer 2 has 5 pallets demand and window 0-24 at (-82.174744291, -40.392993107) and average unload time 0.039157449
@@ -558,6 +699,16 @@
 Vehicle SP2 travels from 12 to DepotReturn to deliver 0 pallets. Expected unload start time is 11.678149448
 Objective value: 909.070915683
 Solve time: 7905</t>
+  </si>
+  <si>
+    <t>{0: [[(4, 3), (5, 3)]], 1: [[(2, 5), (9, 1), (1, 4), (7, 2), (3, 1), (10, 5), (6, 1), (8, 3), (11, 2), (12, 4)]], 2: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+4 (3) -&gt; 6 (1) -&gt; 10 (5) -&gt; 3 (1) -&gt; 7 (2) -&gt; 1 (4) -&gt; 9 (1) -&gt; 2 (5)
+11 metre (capacity 30):
+12 (4) -&gt; 11 (2) -&gt; 8 (3) -&gt; 5 (3)
+</t>
   </si>
   <si>
     <t>Input:
@@ -596,6 +747,16 @@
 Solve time: 2023</t>
   </si>
   <si>
+    <t>{0: [[(10, 5), (8, 6), (5, 7), (3, 3), (2, 1)]], 1: [[(4, 6), (6, 2), (2, 5), (12, 5), (7, 3), (9, 3), (11, 3), (1, 3)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+10 (5) -&gt; 11 (3) -&gt; 9 (3) -&gt; 7 (3) -&gt; 1 (3) -&gt; 12 (5)
+11 metre (capacity 30):
+4 (6) -&gt; 6 (2) -&gt; 2 (6) -&gt; 3 (3) -&gt; 5 (7) -&gt; 8 (6)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 1 pallets demand and window 14-15 at (-60.507168905, -25.526932952) and average unload time 0.037034357
 Customer 2 has 1 pallets demand and window 0-24 at (-38.189779923, -94.309764347) and average unload time 0.115327914
@@ -629,6 +790,16 @@
 Vehicle SP2 travels from 10 to 8 to deliver 2 pallets. Expected unload start time is 3.82719613
 Objective value: 683.459790607
 Solve time: 3644</t>
+  </si>
+  <si>
+    <t>{0: [[(1, 1), (3, 4), (12, 2), (2, 1), (9, 3), (11, 5), (6, 5), (7, 6)]], 1: [[(10, 5), (8, 2), (5, 3), (4, 4)]], 2: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+10 (5) -&gt; 8 (2) -&gt; 5 (3) -&gt; 4 (4)
+11 metre (capacity 30):
+7 (6) -&gt; 6 (5) -&gt; 11 (5) -&gt; 9 (3) -&gt; 2 (1) -&gt; 12 (2) -&gt; 3 (4) -&gt; 1 (1)
+</t>
   </si>
   <si>
     <t>Input:
@@ -667,6 +838,17 @@
 Solve time: 11599</t>
   </si>
   <si>
+    <t>{0: [[(1, 7), (6, 7), (8, 5)], [(11, 5), (10, 7), (12, 7)]], 1: [[(3, 4), (2, 5), (9, 7), (4, 2), (7, 5), (5, 5)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+3 (4) -&gt; 2 (5) -&gt; 9 (7) -&gt; 4 (2) -&gt; 7 (5) -&gt; 5 (5)
+8 metre (capacity 22):
+12 (7) -&gt; 10 (7) -&gt; 11 (5)
+8 (5) -&gt; 6 (7) -&gt; 1 (7)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 3 pallets demand and window 0-24 at (-35.450068632, -1.394236418) and average unload time 0.166319408
 Customer 2 has 5 pallets demand and window 0-24 at (63.063748607, 33.189197656) and average unload time 0.063055616
@@ -700,6 +882,15 @@
 Vehicle SP3 travels from 12 to 6 to deliver 6 pallets. Expected unload start time is 6.556042746
 Objective value: 952.746718211
 Solve time: 66931</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [[(10, 5), (2, 5), (3, 2), (7, 6)], [(1, 3), (12, 3), (6, 6), (5, 1), (4, 2), (9, 4), (8, 7), (11, 2)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+10 (5) -&gt; 2 (5) -&gt; 3 (2) -&gt; 7 (6)
+11 (2) -&gt; 8 (7) -&gt; 9 (4) -&gt; 4 (2) -&gt; 5 (1) -&gt; 6 (6) -&gt; 12 (3) -&gt; 1 (3)
+</t>
   </si>
   <si>
     <t>Input:
@@ -740,6 +931,16 @@
 Vehicle SP3 travels from 12 to 7 to deliver 0 pallets. Expected unload start time is 19
 Objective value: 1604.457014441
 Solve time: 32942</t>
+  </si>
+  <si>
+    <t>{0: [[(6, 3), (7, 1), (10, 0), (2, 3), (9, 2)]], 1: [[(1, 2), (8, 5), (4, 4), (5, 4), (3, 1), (7, 0), (10, 1)], [(12, 2), (7, 0), (10, 0), (11, 3)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+3 (1) -&gt; 7 (1) -&gt; 12 (2) -&gt; 6 (3) -&gt; 2 (3) -&gt; 10 (1) -&gt; 11 (3)
+11 metre (capacity 30):
+5 (4) -&gt; 4 (4) -&gt; 8 (5) -&gt; 1 (2) -&gt; 9 (2)
+</t>
   </si>
   <si>
     <t>Input:
@@ -784,6 +985,16 @@
 Solve time: 202664</t>
   </si>
   <si>
+    <t>{0: [[(2, 4), (13, 5), (11, 4), (12, 1)], [(14, 5), (6, 5), (3, 2), (10, 4), (5, 3)], [(8, 1), (9, 2), (15, 3), (4, 5), (1, 2), (7, 3)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+14 (5) -&gt; 6 (5) -&gt; 3 (2) -&gt; 10 (4) -&gt; 5 (3)
+8 (1) -&gt; 9 (2) -&gt; 15 (3) -&gt; 4 (5) -&gt; 1 (2) -&gt; 7 (3)
+2 (4) -&gt; 13 (5) -&gt; 11 (4) -&gt; 12 (1)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 4 pallets demand and window 0-24 at (-87.579150258, -89.783731753) and average unload time 0.088865326
 Customer 2 has 1 pallets demand and window 0-24 at (-21.265605804, -5.062985601) and average unload time 0.051322487
@@ -826,6 +1037,17 @@
 Solve time: 35184</t>
   </si>
   <si>
+    <t>{0: [[(15, 1), (1, 4), (4, 4), (9, 2), (2, 1)], [(3, 1), (10, 4), (6, 1), (5, 3), (13, 4)]], 1: [[(11, 2), (14, 3), (7, 3), (12, 3), (8, 4)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+13 (4) -&gt; 5 (3) -&gt; 6 (1) -&gt; 10 (4) -&gt; 3 (1)
+2 (1) -&gt; 9 (2) -&gt; 4 (4) -&gt; 1 (4) -&gt; 15 (1)
+8 metre (capacity 22):
+8 (4) -&gt; 12 (3) -&gt; 7 (3) -&gt; 14 (3) -&gt; 11 (2)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 3 pallets demand and window 0-24 at (69.091565718, 78.959259142) and average unload time 0.09181663
 Customer 2 has 4 pallets demand and window 0-24 at (47.254550552, 82.887779312) and average unload time 0.054112947
@@ -868,6 +1090,17 @@
 Solve time: 380729</t>
   </si>
   <si>
+    <t>{0: [[(6, 3)], [(15, 4), (4, 3), (12, 2), (8, 2), (3, 3), (13, 2)]], 1: [[(7, 2), (5, 2), (2, 4), (1, 3), (14, 1), (11, 1), (10, 4), (9, 4)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+7 (2) -&gt; 5 (2) -&gt; 2 (4) -&gt; 1 (3) -&gt; 14 (1) -&gt; 11 (1) -&gt; 10 (4) -&gt; 9 (4)
+Rigid (capacity 16):
+6 (3)
+15 (4) -&gt; 4 (3) -&gt; 12 (2) -&gt; 8 (2) -&gt; 3 (3) -&gt; 13 (2)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 5 pallets demand and window 0-24 at (-41.430511728, 67.190069284) and average unload time 0.131760763
 Customer 2 has 3 pallets demand and window 0-24 at (-0.576573004, -72.615105011) and average unload time 0.121328391
@@ -907,6 +1140,16 @@
 Vehicle SP2 travels from 13 to DepotReturn to deliver 0 pallets. Expected unload start time is 7.991377995
 Objective value: 1003.760132766
 Solve time: 520620</t>
+  </si>
+  <si>
+    <t>{0: [[(14, 3), (9, 5), (3, 1), (12, 1), (1, 5), (6, 4), (10, 4), (7, 5), (15, 1)]], 1: [[(5, 4), (2, 3), (4, 1), (11, 3), (8, 5), (13, 2)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+15 (1) -&gt; 7 (5) -&gt; 10 (4) -&gt; 6 (4) -&gt; 1 (5) -&gt; 12 (1) -&gt; 3 (1) -&gt; 9 (5) -&gt; 14 (3)
+8 metre (capacity 22):
+13 (2) -&gt; 8 (5) -&gt; 11 (3) -&gt; 4 (1) -&gt; 2 (3) -&gt; 5 (4)
+</t>
   </si>
   <si>
     <t>Input:
@@ -951,6 +1194,16 @@
 Solve time: 79067</t>
   </si>
   <si>
+    <t>{0: [[(13, 2), (15, 2), (7, 3), (4, 3)], [(8, 3), (5, 2), (12, 3), (9, 4), (3, 3)], [(11, 3), (14, 2), (6, 3), (2, 2), (10, 2), (1, 4)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+8 (3) -&gt; 5 (2) -&gt; 12 (3) -&gt; 9 (4) -&gt; 3 (3)
+4 (3) -&gt; 7 (3) -&gt; 15 (2) -&gt; 13 (2)
+11 (3) -&gt; 14 (2) -&gt; 6 (3) -&gt; 2 (2) -&gt; 10 (2) -&gt; 1 (4)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 3 pallets demand and window 0-24 at (-84.386511464, 41.028512923) and average unload time 0.02664974
 Customer 2 has 1 pallets demand and window 0-24 at (12.051179729, -94.371117561) and average unload time 0.076220267
@@ -991,6 +1244,18 @@
 Vehicle SP3 travels from 8 to DepotReturn to deliver 0 pallets. Expected unload start time is 2.151403282
 Objective value: 1067.862157347
 Solve time: 15668</t>
+  </si>
+  <si>
+    <t>{0: [[(14, 1), (7, 2), (11, 5), (10, 3), (13, 3), (4, 4), (2, 1), (5, 1)]], 1: [[(12, 1), (3, 5), (6, 1), (9, 3), (15, 3), (1, 3)]], 2: [[(8, 4)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+1 (3) -&gt; 15 (3) -&gt; 9 (3) -&gt; 6 (1) -&gt; 3 (5) -&gt; 12 (1)
+11 metre (capacity 30):
+8 (4)
+8 metre (capacity 22):
+14 (1) -&gt; 7 (2) -&gt; 11 (5) -&gt; 10 (3) -&gt; 13 (3) -&gt; 4 (4) -&gt; 2 (1) -&gt; 5 (1)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1036,6 +1301,16 @@
 Solve time: 72924</t>
   </si>
   <si>
+    <t>{0: [[(2, 2), (1, 2), (8, 4), (15, 1), (14, 4), (10, 3)], [(3, 2), (13, 4), (12, 4), (5, 4), (11, 2)], [(4, 3), (9, 3), (7, 4), (6, 4), (2, 2)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+10 (3) -&gt; 14 (4) -&gt; 15 (1) -&gt; 6 (4) -&gt; 2 (4)
+11 (2) -&gt; 5 (4) -&gt; 12 (4) -&gt; 13 (4) -&gt; 3 (2)
+4 (3) -&gt; 7 (4) -&gt; 9 (3) -&gt; 1 (2) -&gt; 8 (4)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 1 pallets demand and window 0-24 at (27.223585357, 95.572274447) and average unload time 0.16093088
 Customer 2 has 1 pallets demand and window 0-24 at (-23.113715798, 63.159264089) and average unload time 0.113434344
@@ -1077,6 +1352,16 @@
 Solve time: 7998</t>
   </si>
   <si>
+    <t>{0: [], 1: [[(10, 1), (12, 3), (13, 2), (15, 1), (8, 3), (4, 2), (5, 1), (7, 3), (11, 3), (1, 1), (2, 1)], [(9, 1), (14, 4), (6, 2), (3, 2)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+8 metre (capacity 22):
+9 (1) -&gt; 14 (4) -&gt; 6 (2) -&gt; 3 (2) -&gt; 12 (3) -&gt; 15 (1) -&gt; 13 (2) -&gt; 10 (1)
+8 (3) -&gt; 4 (2) -&gt; 5 (1) -&gt; 7 (3) -&gt; 11 (3) -&gt; 1 (1) -&gt; 2 (1)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 3 pallets demand and window 18-19 at (86.128283791, -71.338412168) and average unload time 0.096117568
 Customer 2 has 1 pallets demand and window 0-24 at (-26.120167839, -22.867441357) and average unload time 0.134962108
@@ -1118,6 +1403,16 @@
 Solve time: 18387</t>
   </si>
   <si>
+    <t>{0: [[(11, 2), (8, 4), (4, 2), (12, 2), (3, 2), (15, 3), (9, 6), (2, 1)]], 1: [[(14, 1), (5, 5), (10, 4), (7, 6), (13, 3), (6, 6), (1, 3)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+13 (3) -&gt; 6 (6) -&gt; 1 (3) -&gt; 8 (4) -&gt; 4 (2) -&gt; 12 (2) -&gt; 11 (2)
+11 metre (capacity 30):
+14 (1) -&gt; 10 (4) -&gt; 7 (6) -&gt; 5 (5) -&gt; 9 (6) -&gt; 3 (2) -&gt; 15 (3) -&gt; 2 (1)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 1 pallets demand and window 0-24 at (-24.529968069, 38.399091166) and average unload time 0.066972794
 Customer 2 has 4 pallets demand and window 0-24 at (51.690777233, -76.603520474) and average unload time 0.020191499
@@ -1159,6 +1454,16 @@
 Solve time: 81641</t>
   </si>
   <si>
+    <t>{0: [[(6, 1), (15, 1), (1, 1), (12, 1), (10, 2), (5, 3), (11, 1), (7, 4), (14, 2), (9, 1)]], 1: [[(4, 4), (13, 3), (3, 3), (2, 4), (8, 1)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+6 (1) -&gt; 15 (1) -&gt; 1 (1) -&gt; 12 (1) -&gt; 10 (2) -&gt; 5 (3) -&gt; 11 (1) -&gt; 7 (4) -&gt; 14 (2) -&gt; 9 (1)
+Rigid (capacity 16):
+8 (1) -&gt; 2 (4) -&gt; 3 (3) -&gt; 13 (3) -&gt; 4 (4)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 7 pallets demand and window 0-24 at (25.507139791, 34.12404121) and average unload time 0.032989452
 Customer 2 has 9 pallets demand and window 0-24 at (20.418426913, -15.534208616) and average unload time 0.028418584
@@ -1192,6 +1497,17 @@
 Solve time: 13318</t>
   </si>
   <si>
+    <t>{0: [[(7, 3), (5, 12), (1, 7)], [(7, 4), (3, 5), (9, 3), (8, 4), (6, 5)], [(2, 9), (4, 8)]], 1: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+8 metre (capacity 22):
+7 (7) -&gt; 3 (5) -&gt; 9 (3) -&gt; 8 (4)
+1 (7) -&gt; 5 (12)
+6 (5) -&gt; 4 (8) -&gt; 2 (9)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 4 pallets demand and window 0-24 at (-93.346452798, 32.406838113) and average unload time 0.125621569
 Customer 2 has 5 pallets demand and window 12-13 at (-89.57070554, 30.845985663) and average unload time 0.084441489
@@ -1221,6 +1537,9 @@
 Vehicle SP5 travels from 8 to 3 to deliver 5 pallets. Expected unload start time is 10.250352275
 Objective value: 845.523454536
 Solve time: 1909</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [[(7, 7), (9, 11), (1, 4), (2, 5), (6, 2)], [(5, 8), (4, 9), (8, 8), (3, 5)]], 2: []}</t>
   </si>
   <si>
     <t>Input:
@@ -1257,6 +1576,18 @@
 Solve time: 26248</t>
   </si>
   <si>
+    <t>{0: [[(7, 15)]], 1: [], 2: [[(9, 9), (1, 7), (8, 5), (5, 9)], [(3, 15), (6, 14)], [(9, 5), (4, 14), (2, 5)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+9 (14)
+11 metre (capacity 30):
+6 (14) -&gt; 7 (15)
+2 (5) -&gt; 4 (14) -&gt; 1 (7)
+5 (9) -&gt; 8 (5) -&gt; 3 (15)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 2 pallets demand and window 21-22 at (90.005022837, -95.337592023) and average unload time 0.062945357
 Customer 2 has 2 pallets demand and window 0-24 at (-33.815013292, -77.865289496) and average unload time 0.076961625
@@ -1287,6 +1618,16 @@
 Vehicle SP5 travels from 9 to 4 to deliver 3 pallets. Expected unload start time is 10.497281846
 Objective value: 694.665149453
 Solve time: 2249</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [[(3, 8), (1, 2), (8, 6)]], 2: [[(8, 2), (7, 3), (2, 2), (6, 5), (5, 4), (9, 6), (4, 3)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+8 (8) -&gt; 3 (8)
+11 metre (capacity 30):
+9 (6) -&gt; 5 (4) -&gt; 6 (5) -&gt; 4 (3) -&gt; 7 (3) -&gt; 2 (2) -&gt; 1 (2)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1331,6 +1672,18 @@
 Solve time: 5946</t>
   </si>
   <si>
+    <t>{0: [[(7, 3), (3, 3), (9, 0), (1, 3), (6, 13)], [(9, 1), (1, 1), (4, 9), (2, 10)], [(8, 10), (9, 0), (1, 3)]], 1: [[(9, 2), (1, 0)]], 2: [[(9, 0), (1, 3), (5, 13)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+1 (10) -&gt; 6 (13)
+8 metre (capacity 22):
+8 (10) -&gt; 9 (3) -&gt; 3 (3) -&gt; 7 (3)
+4 (9) -&gt; 2 (10)
+5 (13)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 12 pallets demand and window 0-24 at (-30.968215885, -75.574032689) and average unload time 0.150709065
 Customer 2 has 9 pallets demand and window 0-24 at (-23.291709414, 19.405698648) and average unload time 0.12843052
@@ -1364,6 +1717,18 @@
 Solve time: 10698</t>
   </si>
   <si>
+    <t>{0: [[(3, 10), (8, 16)], [(5, 12), (1, 12)], [(4, 8), (9, 3), (7, 16)]], 1: [[(6, 11), (2, 9)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+2 (9) -&gt; 4 (8) -&gt; 9 (3)
+11 metre (capacity 30):
+7 (16) -&gt; 6 (11)
+3 (10) -&gt; 8 (16)
+5 (12) -&gt; 1 (12)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 11 pallets demand and window 0-24 at (-45.764791583, 86.137379344) and average unload time 0.027180512
 Customer 2 has 1 pallets demand and window 0-24 at (98.382227775, 83.751952147) and average unload time 0.020148877
@@ -1393,6 +1758,9 @@
 Vehicle SP4 travels from 9 to 7 to deliver 2 pallets. Expected unload start time is 22.934633274
 Objective value: 484.162097897
 Solve time: 6631</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [[(5, 1), (2, 1), (3, 12), (6, 4)], [(1, 11), (8, 4), (9, 7), (7, 2), (4, 4)]], 2: []}</t>
   </si>
   <si>
     <t>Input:
@@ -1425,6 +1793,16 @@
 Vehicle SP5 travels from 5 to DepotReturn to deliver 0 pallets. Expected unload start time is 4.885529631
 Objective value: 892.847354116
 Solve time: 23010</t>
+  </si>
+  <si>
+    <t>{0: [[(3, 3), (9, 8), (6, 5)], [(4, 1), (1, 2), (5, 1)]], 1: [[(2, 4), (8, 10), (7, 4)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+3 (3) -&gt; 9 (8) -&gt; 6 (5)
+11 metre (capacity 30):
+7 (4) -&gt; 8 (10) -&gt; 2 (4) -&gt; 1 (2) -&gt; 5 (1) -&gt; 4 (1)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1460,6 +1838,19 @@
 Solve time: 12555</t>
   </si>
   <si>
+    <t>{0: [[(2, 7), (5, 10), (6, 5)], [(1, 11), (8, 7)]], 1: [], 2: [[(3, 5), (4, 12), (7, 7), (9, 5), (2, 1)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+2 (8) -&gt; 5 (10)
+Rigid (capacity 16):
+6 (5) -&gt; 1 (11)
+8 (7)
+11 metre (capacity 30):
+9 (5) -&gt; 7 (7) -&gt; 4 (12) -&gt; 3 (5)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 3 pallets demand and window 0-24 at (43.877999052, -67.22643211) and average unload time 0.162624943
 Customer 2 has 14 pallets demand and window 0-24 at (3.321852729, -43.388160642) and average unload time 0.042911884
@@ -1490,6 +1881,17 @@
 Vehicle SP5 travels from 9 to 4 to deliver 4 pallets. Expected unload start time is 23.021242584
 Objective value: 1059.49309779
 Solve time: 6468</t>
+  </si>
+  <si>
+    <t>{0: [[(6, 13), (5, 4), (8, 4)], [(9, 5), (4, 4), (3, 12)]], 1: [[(1, 3), (2, 14), (7, 11)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+3 (12)
+11 metre (capacity 30):
+5 (4) -&gt; 6 (13) -&gt; 7 (11)
+2 (14) -&gt; 1 (3) -&gt; 4 (4) -&gt; 9 (5) -&gt; 8 (4)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1544,6 +1946,16 @@
 Solve time: 95015</t>
   </si>
   <si>
+    <t>{0: [[(5, 8), (2, 7), (7, 0), (9, 2), (4, 1)], [(8, 3), (11, 7), (12, 9), (7, 2), (9, 0), (4, 0)], [(1, 2), (10, 5), (3, 2), (6, 1), (7, 0), (9, 0), (4, 0)], [(7, 5), (9, 0), (4, 2)]], 1: [[(7, 0), (9, 0), (4, 0)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+8 (3) -&gt; 11 (7) -&gt; 12 (9) -&gt; 4 (3)
+5 (8) -&gt; 2 (7) -&gt; 9 (2) -&gt; 1 (2)
+10 (5) -&gt; 3 (2) -&gt; 6 (1) -&gt; 7 (7)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 7 pallets demand and window 0-24 at (88.586330366, 26.747218425) and average unload time 0.079463013
 Customer 2 has 6 pallets demand and window 0-24 at (-32.739209063, -16.604833265) and average unload time 0.063886353
@@ -1583,6 +1995,18 @@
 Solve time: 30046</t>
   </si>
   <si>
+    <t>{0: [[(3, 4), (1, 7), (7, 4), (5, 7)]], 1: [[(8, 1), (11, 1), (6, 5), (5, 1), (9, 8)]], 2: [[(2, 6), (10, 10), (4, 4), (12, 9)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+11 (1) -&gt; 6 (5) -&gt; 5 (8) -&gt; 7 (4) -&gt; 3 (4)
+Rigid (capacity 16):
+9 (8) -&gt; 1 (7) -&gt; 8 (1)
+11 metre (capacity 30):
+2 (6) -&gt; 10 (10) -&gt; 4 (4) -&gt; 12 (9)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 10 pallets demand and window 0-24 at (-55.665073856, 71.674487895) and average unload time 0.162205203
 Customer 2 has 1 pallets demand and window 0-24 at (-52.917721724, -77.845332262) and average unload time 0.065456515
@@ -1621,6 +2045,16 @@
 Solve time: 176437</t>
   </si>
   <si>
+    <t>{0: [[(2, 1), (6, 8), (11, 6), (4, 1)], [(9, 1), (10, 1), (8, 3), (1, 10), (3, 8)], [(7, 2), (12, 11), (5, 5)]], 1: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+5 (5) -&gt; 12 (11) -&gt; 7 (2)
+3 (8) -&gt; 1 (10) -&gt; 8 (3) -&gt; 10 (1) -&gt; 9 (1)
+2 (1) -&gt; 6 (8) -&gt; 11 (6) -&gt; 4 (1)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 9 pallets demand and window 0-24 at (-41.465726331, 1.091471707) and average unload time 0.086859822
 Customer 2 has 7 pallets demand and window 0-24 at (-17.356206415, 19.906737897) and average unload time 0.064942136
@@ -1657,6 +2091,17 @@
 Vehicle SP5 travels from 12 to 6 to deliver 1 pallets. Expected unload start time is 12.239680951
 Objective value: 835.715151055
 Solve time: 75019</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [[(3, 5), (5, 4), (4, 7), (7, 5)]], 2: [[(2, 7), (1, 9), (9, 3), (11, 9)], [(10, 7), (8, 10), (12, 9), (6, 1)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+11 (9) -&gt; 9 (3) -&gt; 1 (9) -&gt; 2 (7)
+10 (7) -&gt; 8 (10) -&gt; 12 (9) -&gt; 6 (1)
+8 metre (capacity 22):
+3 (5) -&gt; 5 (4) -&gt; 4 (7) -&gt; 7 (5)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1699,6 +2144,17 @@
 Solve time: 40203</t>
   </si>
   <si>
+    <t>{0: [[(1, 5), (2, 6), (8, 4), (3, 6)], [(7, 2)], [(10, 3), (9, 4)]], 1: [[(10, 3), (5, 10), (12, 7), (11, 2), (6, 6), (4, 2)]], 2: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+1 (5) -&gt; 6 (6) -&gt; 11 (2) -&gt; 12 (7) -&gt; 5 (10)
+8 metre (capacity 22):
+4 (2) -&gt; 3 (6) -&gt; 8 (4) -&gt; 2 (6) -&gt; 7 (2)
+10 (6) -&gt; 9 (4)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 2 pallets demand and window 23-24 at (-51.428372932, -11.553882867) and average unload time 0.047898656
 Customer 2 has 9 pallets demand and window 0-24 at (47.55052979, -19.215770402) and average unload time 0.157660311
@@ -1734,6 +2190,17 @@
 Vehicle SP4 travels from 12 to 3 to deliver 2 pallets. Expected unload start time is 5.524910415
 Objective value: 597.194187645
 Solve time: 13732</t>
+  </si>
+  <si>
+    <t>{0: [[(9, 1), (7, 7), (4, 8), (6, 1), (11, 5), (8, 3), (1, 2)], [(2, 9), (12, 8), (3, 2), (10, 2), (5, 9)]], 1: [], 2: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+8 metre (capacity 22):
+11 metre (capacity 30):
+9 (1) -&gt; 7 (7) -&gt; 4 (8) -&gt; 6 (1) -&gt; 11 (5) -&gt; 8 (3) -&gt; 1 (2)
+2 (9) -&gt; 12 (8) -&gt; 3 (2) -&gt; 10 (2) -&gt; 5 (9)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1772,6 +2239,17 @@
 Vehicle SP4 travels from 12 to DepotReturn to deliver 0 pallets. Expected unload start time is 25.255179469
 Objective value: 663.316536328
 Solve time: 17221</t>
+  </si>
+  <si>
+    <t>{0: [[(5, 6), (11, 3), (4, 2), (9, 7), (8, 10)], [(2, 8), (3, 8), (6, 4)]], 1: [], 2: [[(10, 6), (7, 2), (1, 9), (12, 3)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+6 (4) -&gt; 3 (8) -&gt; 2 (8)
+11 metre (capacity 30):
+5 (6) -&gt; 11 (3) -&gt; 4 (2) -&gt; 9 (7) -&gt; 8 (10)
+10 (6) -&gt; 7 (2) -&gt; 1 (9) -&gt; 12 (3)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1813,6 +2291,19 @@
 Solve time: 26318</t>
   </si>
   <si>
+    <t>{0: [[(3, 8), (10, 8), (6, 1), (2, 5)]], 1: [[(11, 10)]], 2: [[(4, 5), (9, 8), (12, 10)], [(8, 6), (7, 9), (1, 7), (5, 8)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+11 (10)
+11 metre (capacity 30):
+5 (8) -&gt; 1 (7) -&gt; 7 (9) -&gt; 8 (6)
+4 (5) -&gt; 9 (8) -&gt; 12 (10)
+8 metre (capacity 22):
+3 (8) -&gt; 10 (8) -&gt; 6 (1) -&gt; 2 (5)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 9 pallets demand and window 0-24 at (-36.4603162, 86.224088672) and average unload time 0.134912375
 Customer 2 has 6 pallets demand and window 0-24 at (-96.619193336, -88.002849108) and average unload time 0.147846307
@@ -1848,6 +2339,16 @@
 Vehicle SP4 travels from 12 to 11 to deliver 3 pallets. Expected unload start time is 7.869715692
 Objective value: 958.651706322
 Solve time: 64992</t>
+  </si>
+  <si>
+    <t>{0: [[(4, 1), (1, 9), (6, 4), (9, 1), (3, 2)]], 1: [[(8, 1), (10, 9), (2, 6), (12, 2), (11, 3), (7, 2), (5, 4)]], 2: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+8 (1) -&gt; 2 (6) -&gt; 3 (2) -&gt; 9 (1) -&gt; 6 (4) -&gt; 1 (9) -&gt; 4 (1)
+8 metre (capacity 22):
+5 (4) -&gt; 7 (2) -&gt; 11 (3) -&gt; 12 (2) -&gt; 10 (9)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1887,6 +2388,19 @@
 Vehicle SP5 travels from 9 to DepotReturn to deliver 0 pallets. Expected unload start time is 10.713855308
 Objective value: 1054.082647881
 Solve time: 327067</t>
+  </si>
+  <si>
+    <t>{0: [[(8, 9), (12, 9), (10, 9), (5, 3)]], 1: [[(4, 10), (1, 8), (2, 4)], [(3, 8), (9, 8)]], 2: [[(6, 2), (11, 9), (7, 4)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+7 (4) -&gt; 11 (9) -&gt; 6 (2)
+11 metre (capacity 30):
+5 (3) -&gt; 10 (9) -&gt; 12 (9) -&gt; 8 (9)
+8 metre (capacity 22):
+4 (10) -&gt; 1 (8) -&gt; 2 (4)
+9 (8) -&gt; 3 (8)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1931,6 +2445,18 @@
 Vehicle SP5 travels from 15 to 11 to deliver 1 pallets. Expected unload start time is 22.475678314
 Objective value: 810.905975236
 Solve time: 178811</t>
+  </si>
+  <si>
+    <t>{0: [[(1, 3), (5, 2), (2, 5), (8, 5)]], 1: [[(6, 8), (7, 2), (13, 4), (12, 3)]], 2: [[(10, 5), (9, 5), (3, 3), (15, 6), (11, 1), (4, 7), (14, 3)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+10 (5) -&gt; 9 (5) -&gt; 3 (3) -&gt; 15 (6) -&gt; 11 (1) -&gt; 4 (7) -&gt; 14 (3)
+Rigid (capacity 16):
+8 (5) -&gt; 2 (5) -&gt; 5 (2) -&gt; 1 (3)
+8 metre (capacity 22):
+6 (8) -&gt; 7 (2) -&gt; 13 (4) -&gt; 12 (3)
+</t>
   </si>
   <si>
     <t>Input:
@@ -1978,6 +2504,19 @@
 Solve time: 181385</t>
   </si>
   <si>
+    <t>{0: [[(12, 2), (1, 6), (4, 3), (11, 3), (10, 5), (2, 2)], [(7, 8), (6, 3), (14, 6), (13, 1), (5, 2)]], 1: [[(3, 7), (15, 5), (8, 4)]], 2: [[(9, 4)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+13 (1) -&gt; 14 (6) -&gt; 6 (3) -&gt; 8 (4) -&gt; 7 (8)
+9 (4) -&gt; 1 (6) -&gt; 4 (3) -&gt; 11 (3) -&gt; 10 (5)
+Rigid (capacity 16):
+2 (2) -&gt; 3 (7) -&gt; 15 (5)
+11 metre (capacity 30):
+12 (2) -&gt; 5 (2)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 4 pallets demand and window 0-24 at (-18.420588435, 1.956733413) and average unload time 0.019041122
 Customer 2 has 1 pallets demand and window 0-24 at (54.455425874, 89.224318758) and average unload time 0.071461774
@@ -2019,6 +2558,15 @@
 Vehicle SP4 travels from 15 to 13 to deliver 2 pallets. Expected unload start time is 20.946620699
 Objective value: 816.442220013
 Solve time: 13830</t>
+  </si>
+  <si>
+    <t>{0: [], 1: [[(12, 6), (2, 1), (6, 3), (8, 3), (3, 2), (1, 4)], [(7, 2), (4, 2), (14, 1), (15, 2), (13, 2), (5, 1), (11, 7), (10, 2), (9, 1)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+12 (6) -&gt; 2 (1) -&gt; 6 (3) -&gt; 3 (2) -&gt; 8 (3) -&gt; 1 (4)
+9 (1) -&gt; 10 (2) -&gt; 11 (7) -&gt; 5 (1) -&gt; 13 (2) -&gt; 15 (2) -&gt; 14 (1) -&gt; 4 (2) -&gt; 7 (2)
+</t>
   </si>
   <si>
     <t>Input:
@@ -2066,6 +2614,18 @@
 Solve time: 1908806</t>
   </si>
   <si>
+    <t>{0: [[(6, 8), (1, 5), (2, 5), (4, 6)], [(11, 9), (3, 8)], [(13, 8), (5, 7), (15, 1), (8, 1), (12, 8), (14, 4)]], 1: [[(9, 8), (10, 6), (7, 7)]], 2: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+4 (6) -&gt; 1 (5)
+11 metre (capacity 30):
+5 (7) -&gt; 11 (9) -&gt; 3 (8)
+13 (8) -&gt; 14 (4) -&gt; 15 (1) -&gt; 8 (1) -&gt; 12 (8) -&gt; 7 (7)
+2 (5) -&gt; 10 (6) -&gt; 9 (8) -&gt; 6 (8)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 3 pallets demand and window 0-24 at (-47.49489985, 6.706850446) and average unload time 0.076132654
 Customer 2 has 1 pallets demand and window 19-20 at (-68.405715588, -30.841255547) and average unload time 0.035494192
@@ -2110,6 +2670,17 @@
 Solve time: 382633</t>
   </si>
   <si>
+    <t>{0: [[(10, 5), (12, 1), (9, 6), (15, 4)], [(3, 1), (8, 5), (4, 1), (14, 9)]], 1: [[(1, 3), (7, 3), (2, 1), (11, 3), (6, 7), (5, 1), (13, 3)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+10 (5) -&gt; 12 (1) -&gt; 9 (6) -&gt; 15 (4)
+2 (1) -&gt; 11 (3) -&gt; 6 (7) -&gt; 5 (1) -&gt; 13 (3)
+11 metre (capacity 30):
+1 (3) -&gt; 7 (3) -&gt; 4 (1) -&gt; 14 (9) -&gt; 8 (5) -&gt; 3 (1)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 7 pallets demand and window 0-24 at (6.811752096, 11.842209262) and average unload time 0.086289929
 Customer 2 has 5 pallets demand and window 16-17 at (-37.502668453, 13.289004958) and average unload time 0.046515297
@@ -2154,6 +2725,17 @@
 Solve time: 715637</t>
   </si>
   <si>
+    <t>{0: [[(3, 6), (14, 2), (12, 7), (4, 5), (11, 3), (1, 7)]], 1: [], 2: [[(5, 6), (9, 2), (15, 4), (7, 2), (6, 2)], [(13, 5), (10, 2), (2, 5), (8, 3)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+5 (6) -&gt; 9 (2) -&gt; 15 (4) -&gt; 7 (2) -&gt; 6 (2)
+3 (6) -&gt; 14 (2) -&gt; 10 (2) -&gt; 13 (5)
+11 metre (capacity 30):
+8 (3) -&gt; 1 (7) -&gt; 11 (3) -&gt; 2 (5) -&gt; 4 (5) -&gt; 12 (7)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 3 pallets demand and window 0-24 at (43.819632519, 96.540563072) and average unload time 0.030967713
 Customer 2 has 6 pallets demand and window 0-24 at (33.639335364, 12.125825756) and average unload time 0.069759681
@@ -2196,6 +2778,17 @@
 Vehicle SP5 travels from 11 to 7 to deliver 6 pallets. Expected unload start time is 22
 Objective value: 1042.983796971
 Solve time: 48352</t>
+  </si>
+  <si>
+    <t>{0: [[(14, 3), (8, 3), (2, 6)], [(5, 2), (4, 3), (10, 4), (3, 1), (11, 4), (7, 6)]], 1: [], 2: [[(13, 8), (9, 8), (12, 1), (15, 3), (1, 3), (6, 4)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+2 (6) -&gt; 8 (3) -&gt; 11 (4) -&gt; 14 (3)
+5 (2) -&gt; 4 (3) -&gt; 10 (4) -&gt; 3 (1) -&gt; 7 (6)
+11 metre (capacity 30):
+13 (8) -&gt; 9 (8) -&gt; 12 (1) -&gt; 15 (3) -&gt; 1 (3) -&gt; 6 (4)
+</t>
   </si>
   <si>
     <t>Input:
@@ -2252,6 +2845,18 @@
 Solve time: 1251752</t>
   </si>
   <si>
+    <t>{0: [[(7, 5), (6, 0)], [(7, 1), (6, 0)]], 1: [[(9, 7), (8, 2), (11, 3), (14, 2), (7, 0), (6, 0), (10, 1), (5, 5)], [(3, 2), (4, 7), (13, 1), (12, 4), (1, 3), (7, 0), (6, 1), (2, 3)]], 2: [[(15, 6), (7, 0), (6, 0)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+Rigid (capacity 16):
+9 (7) -&gt; 5 (5)
+8 metre (capacity 22):
+3 (2) -&gt; 13 (1) -&gt; 4 (7) -&gt; 10 (1) -&gt; 6 (1) -&gt; 2 (3) -&gt; 15 (6)
+8 (2) -&gt; 14 (2) -&gt; 7 (6) -&gt; 11 (3) -&gt; 1 (3) -&gt; 12 (4)
+</t>
+  </si>
+  <si>
     <t>Input:
 Customer 1 has 3 pallets demand and window 0-24 at (-56.895399211, 29.052689043) and average unload time 0.143475865
 Customer 2 has 6 pallets demand and window 0-24 at (-38.554318701, -99.205204961) and average unload time 0.097478595
@@ -2297,7 +2902,15 @@
 Solve time: 831002</t>
   </si>
   <si>
-    <t>Math Routes</t>
+    <t>{0: [[(13, 9), (9, 5), (14, 7)]], 1: [[(2, 6), (10, 5), (4, 6), (5, 2), (11, 8), (6, 3)], [(12, 6), (1, 3), (6, 1), (3, 5), (7, 8), (15, 6), (8, 1)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+14 (7) -&gt; 9 (5) -&gt; 13 (9)
+11 metre (capacity 30):
+8 (1) -&gt; 15 (6) -&gt; 7 (8) -&gt; 3 (5) -&gt; 2 (6) -&gt; 6 (4)
+12 (6) -&gt; 1 (3) -&gt; 11 (8) -&gt; 5 (2) -&gt; 4 (6) -&gt; 10 (5)
+</t>
   </si>
   <si>
     <t>Input:
@@ -2345,6 +2958,19 @@
 Vehicle SP4 travels from 15 to DepotReturn to deliver 0 pallets. Expected unload start time is 11.473228587
 Objective value: 1036.060760446
 Solve time: 27788201</t>
+  </si>
+  <si>
+    <t>{0: [[(15, 5), (10, 5), (9, 2), (8, 4)], [(13, 2), (2, 6), (5, 8)]], 1: [[(4, 4), (1, 5), (7, 6), (3, 6)]], 2: [[(13, 4), (11, 4), (14, 7), (6, 6), (12, 8), (15, 1)]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 metre (capacity 30):
+10 (5) -&gt; 12 (8) -&gt; 6 (6) -&gt; 14 (7) -&gt; 11 (4)
+3 (6) -&gt; 7 (6) -&gt; 1 (5) -&gt; 4 (4) -&gt; 2 (6)
+8 metre (capacity 22):
+Rigid (capacity 16):
+5 (8) -&gt; 8 (4) -&gt; 9 (2)
+15 (6) -&gt; 13 (6)
+</t>
   </si>
 </sst>
 </file>
@@ -2394,7 +3020,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2402,11 +3028,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2520,7 +3146,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0FD1-40CB-9EAD-A6AB7805499F}"/>
+              <c16:uniqueId val="{00000000-9338-4886-9421-C7416FC28C74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2593,7 +3219,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0FD1-40CB-9EAD-A6AB7805499F}"/>
+              <c16:uniqueId val="{00000001-9338-4886-9421-C7416FC28C74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3188,11 +3814,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3460,28 +4086,28 @@
   <dimension ref="A1:N209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="4" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="150.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="100.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="150.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="100.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3507,22 +4133,22 @@
         <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3547,24 +4173,27 @@
         <v>641</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="7"/>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
       <c r="J2">
-        <v>681.47077530873207</v>
+        <v>681.64705556381671</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L2">
-        <v>214.0572899</v>
+        <v>262.46966379999998</v>
       </c>
       <c r="M2">
         <v>737.89099450163053</v>
       </c>
-      <c r="N2" s="5">
-        <f>(M2-J2)/J2</f>
-        <v>8.2791839704847159E-2</v>
+      <c r="N2" s="4">
+        <f t="shared" ref="N2:N33" si="2">(M2-J2)/J2</f>
+        <v>8.2511819685470916E-2</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3589,9 +4218,28 @@
         <v>903</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H3" s="7"/>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3">
+        <v>662.80451167813396</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3">
+        <v>278.01979510000001</v>
+      </c>
+      <c r="M3">
+        <v>662.80451167813396</v>
+      </c>
+      <c r="N3" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3615,9 +4263,28 @@
         <v>630</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H4" s="7"/>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>1121.506775041001</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4">
+        <v>278.10329050000013</v>
+      </c>
+      <c r="M4">
+        <v>1017.840597157414</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" si="2"/>
+        <v>-9.2434731729371042E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3641,9 +4308,28 @@
         <v>1531</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H5" s="7"/>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5">
+        <v>648.77828901133626</v>
+      </c>
+      <c r="K5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5">
+        <v>277.54593849999998</v>
+      </c>
+      <c r="M5">
+        <v>648.77828901133626</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -3667,9 +4353,28 @@
         <v>2543</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="H6" s="7"/>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6">
+        <v>1096.3601690856599</v>
+      </c>
+      <c r="K6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6">
+        <v>260.34920179999989</v>
+      </c>
+      <c r="M6">
+        <v>1077.6947002346831</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="2"/>
+        <v>-1.7024942511860323E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -3693,9 +4398,28 @@
         <v>3773</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H7" s="7"/>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7">
+        <v>520.34549815358832</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7">
+        <v>317.7635937</v>
+      </c>
+      <c r="M7">
+        <v>520.34549815358832</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -3719,9 +4443,28 @@
         <v>3816</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H8" s="7"/>
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8">
+        <v>996.8146493389404</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8">
+        <v>270.72479270000002</v>
+      </c>
+      <c r="M8">
+        <v>996.81464933894028</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="2"/>
+        <v>-1.1405012737022871E-16</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -3745,9 +4488,28 @@
         <v>2016</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="H9" s="7"/>
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9">
+        <v>849.7955585238285</v>
+      </c>
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9">
+        <v>304.02424980000001</v>
+      </c>
+      <c r="M9">
+        <v>775.21553639218246</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="2"/>
+        <v>-8.7762311044786198E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -3771,9 +4533,28 @@
         <v>1630</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="H10" s="7"/>
+      <c r="I10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10">
+        <v>732.72108410107626</v>
+      </c>
+      <c r="K10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10">
+        <v>294.104108</v>
+      </c>
+      <c r="M10">
+        <v>732.72108410107626</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -3797,9 +4578,28 @@
         <v>976</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="H11" s="7"/>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11">
+        <v>675.31814202394798</v>
+      </c>
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11">
+        <v>268.09872009999998</v>
+      </c>
+      <c r="M11">
+        <v>695.40386535206767</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="2"/>
+        <v>2.9742608821261916E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -3823,9 +4623,28 @@
         <v>2359</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="H12" s="7"/>
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12">
+        <v>913.45865950850782</v>
+      </c>
+      <c r="K12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12">
+        <v>464.70780339999988</v>
+      </c>
+      <c r="M12">
+        <v>914.85828521333269</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="2"/>
+        <v>1.5322266533418691E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -3849,9 +4668,28 @@
         <v>8640</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="H13" s="7"/>
+      <c r="I13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13">
+        <v>723.75913134411178</v>
+      </c>
+      <c r="K13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13">
+        <v>406.5890359</v>
+      </c>
+      <c r="M13">
+        <v>723.75913134411178</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -3875,9 +4713,28 @@
         <v>1565</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="H14" s="7"/>
+      <c r="I14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14">
+        <v>869.73014524941982</v>
+      </c>
+      <c r="K14" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14">
+        <v>419.66426040000027</v>
+      </c>
+      <c r="M14">
+        <v>869.73014524941982</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -3901,9 +4758,28 @@
         <v>5289</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="H15" s="7"/>
+      <c r="I15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15">
+        <v>894.78810796327741</v>
+      </c>
+      <c r="K15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15">
+        <v>422.64755399999967</v>
+      </c>
+      <c r="M15">
+        <v>894.78810796327741</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -3927,11 +4803,30 @@
         <v>7905</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16">
+        <v>1027.364256635447</v>
+      </c>
+      <c r="K16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L16">
+        <v>442.34885850000001</v>
+      </c>
+      <c r="M16">
+        <v>1018.647370722324</v>
+      </c>
+      <c r="N16" s="4">
+        <f t="shared" si="2"/>
+        <v>-8.484708180981692E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -3953,11 +4848,30 @@
         <v>2023</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17">
+        <v>999.21410672612376</v>
+      </c>
+      <c r="K17" t="s">
+        <v>65</v>
+      </c>
+      <c r="L17">
+        <v>426.36255859999977</v>
+      </c>
+      <c r="M17">
+        <v>900.14586449837202</v>
+      </c>
+      <c r="N17" s="4">
+        <f t="shared" si="2"/>
+        <v>-9.914616052844169E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -3979,11 +4893,30 @@
         <v>3644</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18">
+        <v>782.003935883964</v>
+      </c>
+      <c r="K18" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18">
+        <v>370.22184800000008</v>
+      </c>
+      <c r="M18">
+        <v>782.003935883964</v>
+      </c>
+      <c r="N18" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -4005,11 +4938,30 @@
         <v>11599</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19">
+        <v>1219.039143534927</v>
+      </c>
+      <c r="K19" t="s">
+        <v>71</v>
+      </c>
+      <c r="L19">
+        <v>438.19959239999929</v>
+      </c>
+      <c r="M19">
+        <v>1219.039143534927</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -4031,11 +4983,30 @@
         <v>66931</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20">
+        <v>1095.786848590677</v>
+      </c>
+      <c r="K20" t="s">
+        <v>74</v>
+      </c>
+      <c r="L20">
+        <v>395.94870300000002</v>
+      </c>
+      <c r="M20">
+        <v>1095.786848590677</v>
+      </c>
+      <c r="N20" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -4057,11 +5028,30 @@
         <v>32942</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21">
+        <v>1783.3204562016881</v>
+      </c>
+      <c r="K21" t="s">
+        <v>77</v>
+      </c>
+      <c r="L21">
+        <v>409.07242740000038</v>
+      </c>
+      <c r="M21">
+        <v>1037.0643622155451</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.41846438277033016</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
@@ -4083,11 +5073,30 @@
         <v>202664</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22">
+        <v>1281.2391705977</v>
+      </c>
+      <c r="K22" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22">
+        <v>672.47080480000022</v>
+      </c>
+      <c r="M22">
+        <v>1281.2391705977</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
@@ -4109,11 +5118,30 @@
         <v>35184</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>82</v>
+      </c>
+      <c r="J23">
+        <v>977.46652415438575</v>
+      </c>
+      <c r="K23" t="s">
+        <v>83</v>
+      </c>
+      <c r="L23">
+        <v>699.79639490000045</v>
+      </c>
+      <c r="M23">
+        <v>977.46652415438575</v>
+      </c>
+      <c r="N23" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -4135,11 +5163,30 @@
         <v>380729</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>85</v>
+      </c>
+      <c r="J24">
+        <v>916.32674868129936</v>
+      </c>
+      <c r="K24" t="s">
+        <v>86</v>
+      </c>
+      <c r="L24">
+        <v>701.53700339999978</v>
+      </c>
+      <c r="M24">
+        <v>916.32674868129936</v>
+      </c>
+      <c r="N24" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>15</v>
       </c>
@@ -4161,11 +5208,30 @@
         <v>520620</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25">
+        <v>1139.100511867154</v>
+      </c>
+      <c r="K25" t="s">
+        <v>89</v>
+      </c>
+      <c r="L25">
+        <v>583.48621159999948</v>
+      </c>
+      <c r="M25">
+        <v>1139.100511867154</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>15</v>
       </c>
@@ -4187,11 +5253,30 @@
         <v>79067</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26">
+        <v>1026.542152900709</v>
+      </c>
+      <c r="K26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L26">
+        <v>892.96981309999865</v>
+      </c>
+      <c r="M26">
+        <v>1026.542152900709</v>
+      </c>
+      <c r="N26" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15</v>
       </c>
@@ -4213,11 +5298,30 @@
         <v>15668</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>94</v>
+      </c>
+      <c r="J27">
+        <v>1204.045683633422</v>
+      </c>
+      <c r="K27" t="s">
+        <v>95</v>
+      </c>
+      <c r="L27">
+        <v>630.24923900000067</v>
+      </c>
+      <c r="M27">
+        <v>1204.045683633422</v>
+      </c>
+      <c r="N27" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>15</v>
       </c>
@@ -4239,11 +5343,30 @@
         <v>72924</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>97</v>
+      </c>
+      <c r="J28">
+        <v>1102.417321416543</v>
+      </c>
+      <c r="K28" t="s">
+        <v>98</v>
+      </c>
+      <c r="L28">
+        <v>1224.071597600001</v>
+      </c>
+      <c r="M28">
+        <v>1175.4004660916421</v>
+      </c>
+      <c r="N28" s="4">
+        <f t="shared" si="2"/>
+        <v>6.6202828327588253E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
@@ -4265,11 +5388,30 @@
         <v>7998</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>100</v>
+      </c>
+      <c r="J29">
+        <v>1053.1063034427791</v>
+      </c>
+      <c r="K29" t="s">
+        <v>101</v>
+      </c>
+      <c r="L29">
+        <v>544.41398100000151</v>
+      </c>
+      <c r="M29">
+        <v>841.42993112169711</v>
+      </c>
+      <c r="N29" s="4">
+        <f t="shared" si="2"/>
+        <v>-0.20100190420385564</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>15</v>
       </c>
@@ -4291,11 +5433,30 @@
         <v>18387</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>103</v>
+      </c>
+      <c r="J30">
+        <v>1286.4102607775251</v>
+      </c>
+      <c r="K30" t="s">
+        <v>104</v>
+      </c>
+      <c r="L30">
+        <v>868.00867970000036</v>
+      </c>
+      <c r="M30">
+        <v>1323.487054912182</v>
+      </c>
+      <c r="N30" s="4">
+        <f t="shared" si="2"/>
+        <v>2.8821904850360212E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>15</v>
       </c>
@@ -4317,11 +5478,30 @@
         <v>81641</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>47</v>
+        <v>105</v>
       </c>
       <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>106</v>
+      </c>
+      <c r="J31">
+        <v>856.80458072890463</v>
+      </c>
+      <c r="K31" t="s">
+        <v>107</v>
+      </c>
+      <c r="L31">
+        <v>463.10816349999908</v>
+      </c>
+      <c r="M31">
+        <v>856.80458072890463</v>
+      </c>
+      <c r="N31" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
@@ -4343,11 +5523,30 @@
         <v>13318</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>109</v>
+      </c>
+      <c r="J32">
+        <v>724.48723782131583</v>
+      </c>
+      <c r="K32" t="s">
+        <v>110</v>
+      </c>
+      <c r="L32">
+        <v>317.03553440000002</v>
+      </c>
+      <c r="M32">
+        <v>753.23582552852463</v>
+      </c>
+      <c r="N32" s="4">
+        <f t="shared" si="2"/>
+        <v>3.9681289340115632E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
@@ -4369,11 +5568,27 @@
         <v>1909</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>112</v>
+      </c>
+      <c r="J33">
+        <v>1024.350870524725</v>
+      </c>
+      <c r="L33">
+        <v>297.15786459999981</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>9</v>
       </c>
@@ -4384,22 +5599,41 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D61" si="2">E34/60</f>
+        <f t="shared" ref="D34:D65" si="3">E34/60</f>
         <v>0.43746666666666667</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E61" si="3">F34/1000</f>
+        <f t="shared" ref="E34:E65" si="4">F34/1000</f>
         <v>26.248000000000001</v>
       </c>
       <c r="F34">
         <v>26248</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>114</v>
+      </c>
+      <c r="J34">
+        <v>866.88826321288798</v>
+      </c>
+      <c r="K34" t="s">
+        <v>115</v>
+      </c>
+      <c r="L34">
+        <v>420.53963870000013</v>
+      </c>
+      <c r="M34">
+        <v>883.13909655706368</v>
+      </c>
+      <c r="N34" s="4">
+        <f t="shared" ref="N34:N65" si="5">(M34-J34)/J34</f>
+        <v>1.8746168374625772E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
@@ -4410,22 +5644,41 @@
         <v>4</v>
       </c>
       <c r="D35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7483333333333334E-2</v>
       </c>
       <c r="E35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2490000000000001</v>
       </c>
       <c r="F35">
         <v>2249</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>117</v>
+      </c>
+      <c r="J35">
+        <v>931.91447117107839</v>
+      </c>
+      <c r="K35" t="s">
+        <v>118</v>
+      </c>
+      <c r="L35">
+        <v>305.86990820000028</v>
+      </c>
+      <c r="M35">
+        <v>854.4762539967021</v>
+      </c>
+      <c r="N35" s="4">
+        <f t="shared" si="5"/>
+        <v>-8.3095841485393548E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9</v>
       </c>
@@ -4436,22 +5689,41 @@
         <v>5</v>
       </c>
       <c r="D36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.9099999999999994E-2</v>
       </c>
       <c r="E36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.9459999999999997</v>
       </c>
       <c r="F36">
         <v>5946</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>120</v>
+      </c>
+      <c r="J36">
+        <v>2241.807068141215</v>
+      </c>
+      <c r="K36" t="s">
+        <v>121</v>
+      </c>
+      <c r="L36">
+        <v>316.42438950000002</v>
+      </c>
+      <c r="M36">
+        <v>1133.0187938159579</v>
+      </c>
+      <c r="N36" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.49459576164357638</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9</v>
       </c>
@@ -4462,22 +5734,41 @@
         <v>6</v>
       </c>
       <c r="D37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.17830000000000001</v>
       </c>
       <c r="E37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.698</v>
       </c>
       <c r="F37">
         <v>10698</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="H37" s="7"/>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>123</v>
+      </c>
+      <c r="J37">
+        <v>1326.10584170281</v>
+      </c>
+      <c r="K37" t="s">
+        <v>124</v>
+      </c>
+      <c r="L37">
+        <v>388.58196549999963</v>
+      </c>
+      <c r="M37">
+        <v>1401.748026361061</v>
+      </c>
+      <c r="N37" s="4">
+        <f t="shared" si="5"/>
+        <v>5.7040835112468262E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9</v>
       </c>
@@ -4488,22 +5779,38 @@
         <v>7</v>
       </c>
       <c r="D38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.11051666666666667</v>
       </c>
       <c r="E38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.6310000000000002</v>
       </c>
       <c r="F38">
         <v>6631</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>126</v>
+      </c>
+      <c r="J38">
+        <v>622.21807644280557</v>
+      </c>
+      <c r="L38">
+        <v>399.54162879999973</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38" s="4">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9</v>
       </c>
@@ -4514,22 +5821,41 @@
         <v>8</v>
       </c>
       <c r="D39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.38350000000000001</v>
       </c>
       <c r="E39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.01</v>
       </c>
       <c r="F39">
         <v>23010</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>128</v>
+      </c>
+      <c r="J39">
+        <v>988.08515815373653</v>
+      </c>
+      <c r="K39" t="s">
+        <v>129</v>
+      </c>
+      <c r="L39">
+        <v>276.81299589999981</v>
+      </c>
+      <c r="M39">
+        <v>987.84311063723396</v>
+      </c>
+      <c r="N39" s="4">
+        <f t="shared" si="5"/>
+        <v>-2.4496625063657329E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9</v>
       </c>
@@ -4540,22 +5866,41 @@
         <v>9</v>
       </c>
       <c r="D40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.20924999999999999</v>
       </c>
       <c r="E40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12.555</v>
       </c>
       <c r="F40">
         <v>12555</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>131</v>
+      </c>
+      <c r="J40">
+        <v>1367.2770599111541</v>
+      </c>
+      <c r="K40" t="s">
+        <v>132</v>
+      </c>
+      <c r="L40">
+        <v>297.8125940000009</v>
+      </c>
+      <c r="M40">
+        <v>1175.4149018879809</v>
+      </c>
+      <c r="N40" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.14032427197721023</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9</v>
       </c>
@@ -4566,22 +5911,41 @@
         <v>10</v>
       </c>
       <c r="D41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.10779999999999999</v>
       </c>
       <c r="E41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.468</v>
       </c>
       <c r="F41">
         <v>6468</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>134</v>
+      </c>
+      <c r="J41">
+        <v>1198.896614545255</v>
+      </c>
+      <c r="K41" t="s">
+        <v>135</v>
+      </c>
+      <c r="L41">
+        <v>293.25066800000059</v>
+      </c>
+      <c r="M41">
+        <v>1171.163514436588</v>
+      </c>
+      <c r="N41" s="4">
+        <f t="shared" si="5"/>
+        <v>-2.3132186522343529E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>12</v>
       </c>
@@ -4592,22 +5956,41 @@
         <v>1</v>
       </c>
       <c r="D42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5835833333333333</v>
       </c>
       <c r="E42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95.015000000000001</v>
       </c>
       <c r="F42">
         <v>95015</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
       <c r="H42" s="7"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>137</v>
+      </c>
+      <c r="J42">
+        <v>3155.4945885752991</v>
+      </c>
+      <c r="K42" t="s">
+        <v>138</v>
+      </c>
+      <c r="L42">
+        <v>418.98603239999829</v>
+      </c>
+      <c r="M42">
+        <v>1035.407331022036</v>
+      </c>
+      <c r="N42" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.67187161886735458</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12</v>
       </c>
@@ -4618,22 +6001,41 @@
         <v>2</v>
       </c>
       <c r="D43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.50076666666666669</v>
       </c>
       <c r="E43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30.045999999999999</v>
       </c>
       <c r="F43">
         <v>30046</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
       <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>140</v>
+      </c>
+      <c r="J43">
+        <v>1013.155546866768</v>
+      </c>
+      <c r="K43" t="s">
+        <v>141</v>
+      </c>
+      <c r="L43">
+        <v>446.54841970000052</v>
+      </c>
+      <c r="M43">
+        <v>1105.841482055037</v>
+      </c>
+      <c r="N43" s="4">
+        <f t="shared" si="5"/>
+        <v>9.1482433743668198E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>12</v>
       </c>
@@ -4644,22 +6046,41 @@
         <v>3</v>
       </c>
       <c r="D44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9406166666666667</v>
       </c>
       <c r="E44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>176.43700000000001</v>
       </c>
       <c r="F44">
         <v>176437</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="H44" s="7"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>143</v>
+      </c>
+      <c r="J44">
+        <v>977.17357619100812</v>
+      </c>
+      <c r="K44" t="s">
+        <v>144</v>
+      </c>
+      <c r="L44">
+        <v>415.29174580000108</v>
+      </c>
+      <c r="M44">
+        <v>977.17357619100812</v>
+      </c>
+      <c r="N44" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>12</v>
       </c>
@@ -4670,22 +6091,41 @@
         <v>4</v>
       </c>
       <c r="D45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2503166666666667</v>
       </c>
       <c r="E45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75.019000000000005</v>
       </c>
       <c r="F45">
         <v>75019</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
       <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>146</v>
+      </c>
+      <c r="J45">
+        <v>1012.611449136446</v>
+      </c>
+      <c r="K45" t="s">
+        <v>147</v>
+      </c>
+      <c r="L45">
+        <v>640.17047660000026</v>
+      </c>
+      <c r="M45">
+        <v>1012.611449136445</v>
+      </c>
+      <c r="N45" s="4">
+        <f t="shared" si="5"/>
+        <v>-1.0104384464219839E-15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>12</v>
       </c>
@@ -4696,22 +6136,41 @@
         <v>5</v>
       </c>
       <c r="D46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.67005000000000003</v>
       </c>
       <c r="E46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40.203000000000003</v>
       </c>
       <c r="F46">
         <v>40203</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>62</v>
+        <v>148</v>
       </c>
       <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>149</v>
+      </c>
+      <c r="J46">
+        <v>1401.6565058130111</v>
+      </c>
+      <c r="K46" t="s">
+        <v>150</v>
+      </c>
+      <c r="L46">
+        <v>729.52997780000078</v>
+      </c>
+      <c r="M46">
+        <v>1207.078493999617</v>
+      </c>
+      <c r="N46" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.13882003972188028</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>12</v>
       </c>
@@ -4722,22 +6181,41 @@
         <v>6</v>
       </c>
       <c r="D47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.22886666666666666</v>
       </c>
       <c r="E47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.731999999999999</v>
       </c>
       <c r="F47">
         <v>13732</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>63</v>
+        <v>151</v>
       </c>
       <c r="H47" s="7"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>152</v>
+      </c>
+      <c r="J47">
+        <v>799.14062349535777</v>
+      </c>
+      <c r="K47" t="s">
+        <v>153</v>
+      </c>
+      <c r="L47">
+        <v>405.30707930000062</v>
+      </c>
+      <c r="M47">
+        <v>799.14062349535777</v>
+      </c>
+      <c r="N47" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>12</v>
       </c>
@@ -4748,22 +6226,41 @@
         <v>7</v>
       </c>
       <c r="D48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28701666666666664</v>
       </c>
       <c r="E48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17.221</v>
       </c>
       <c r="F48">
         <v>17221</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>64</v>
+        <v>154</v>
       </c>
       <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>155</v>
+      </c>
+      <c r="J48">
+        <v>873.69244502127435</v>
+      </c>
+      <c r="K48" t="s">
+        <v>156</v>
+      </c>
+      <c r="L48">
+        <v>679.35048359999928</v>
+      </c>
+      <c r="M48">
+        <v>873.05605380381769</v>
+      </c>
+      <c r="N48" s="4">
+        <f t="shared" si="5"/>
+        <v>-7.2839272112644406E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>12</v>
       </c>
@@ -4774,22 +6271,41 @@
         <v>8</v>
       </c>
       <c r="D49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.43863333333333338</v>
       </c>
       <c r="E49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>26.318000000000001</v>
       </c>
       <c r="F49">
         <v>26318</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>158</v>
+      </c>
+      <c r="J49">
+        <v>1289.1298271084211</v>
+      </c>
+      <c r="K49" t="s">
+        <v>159</v>
+      </c>
+      <c r="L49">
+        <v>449.06065099999978</v>
+      </c>
+      <c r="M49">
+        <v>1289.1298271084211</v>
+      </c>
+      <c r="N49" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>12</v>
       </c>
@@ -4800,22 +6316,41 @@
         <v>9</v>
       </c>
       <c r="D50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0832000000000002</v>
       </c>
       <c r="E50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64.992000000000004</v>
       </c>
       <c r="F50">
         <v>64992</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="H50" s="7"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>161</v>
+      </c>
+      <c r="J50">
+        <v>1088.708858004286</v>
+      </c>
+      <c r="K50" t="s">
+        <v>162</v>
+      </c>
+      <c r="L50">
+        <v>400.13931310000038</v>
+      </c>
+      <c r="M50">
+        <v>1132.2410789061589</v>
+      </c>
+      <c r="N50" s="4">
+        <f t="shared" si="5"/>
+        <v>3.9985181145372466E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>12</v>
       </c>
@@ -4826,22 +6361,41 @@
         <v>10</v>
       </c>
       <c r="D51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.4511166666666666</v>
       </c>
       <c r="E51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>327.06700000000001</v>
       </c>
       <c r="F51">
         <v>327067</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>67</v>
+        <v>163</v>
       </c>
       <c r="H51" s="7"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>164</v>
+      </c>
+      <c r="J51">
+        <v>1230.788478416772</v>
+      </c>
+      <c r="K51" t="s">
+        <v>165</v>
+      </c>
+      <c r="L51">
+        <v>462.89721049999929</v>
+      </c>
+      <c r="M51">
+        <v>1230.7884784167711</v>
+      </c>
+      <c r="N51" s="4">
+        <f t="shared" si="5"/>
+        <v>-7.3895288891789039E-16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>15</v>
       </c>
@@ -4852,22 +6406,41 @@
         <v>1</v>
       </c>
       <c r="D52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9801833333333336</v>
       </c>
       <c r="E52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>178.81100000000001</v>
       </c>
       <c r="F52">
         <v>178811</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" t="s">
+        <v>167</v>
+      </c>
+      <c r="J52">
+        <v>962.34315919796416</v>
+      </c>
+      <c r="K52" t="s">
+        <v>168</v>
+      </c>
+      <c r="L52">
+        <v>641.09922839999854</v>
+      </c>
+      <c r="M52">
+        <v>962.34315919796416</v>
+      </c>
+      <c r="N52" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>15</v>
       </c>
@@ -4878,22 +6451,41 @@
         <v>2</v>
       </c>
       <c r="D53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.0230833333333331</v>
       </c>
       <c r="E53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>181.38499999999999</v>
       </c>
       <c r="F53">
         <v>181385</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>69</v>
+        <v>169</v>
       </c>
       <c r="H53" s="7"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>170</v>
+      </c>
+      <c r="J53">
+        <v>1153.558670195504</v>
+      </c>
+      <c r="K53" t="s">
+        <v>171</v>
+      </c>
+      <c r="L53">
+        <v>1800.0106947999991</v>
+      </c>
+      <c r="M53">
+        <v>1167.912269342434</v>
+      </c>
+      <c r="N53" s="4">
+        <f t="shared" si="5"/>
+        <v>1.2442886103484796E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>15</v>
       </c>
@@ -4904,22 +6496,41 @@
         <v>3</v>
       </c>
       <c r="D54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23050000000000001</v>
       </c>
       <c r="E54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.83</v>
       </c>
       <c r="F54">
         <v>13830</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>70</v>
+        <v>172</v>
       </c>
       <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>173</v>
+      </c>
+      <c r="J54">
+        <v>975.46261747594792</v>
+      </c>
+      <c r="K54" t="s">
+        <v>174</v>
+      </c>
+      <c r="L54">
+        <v>589.63765830000193</v>
+      </c>
+      <c r="M54">
+        <v>986.5123038407138</v>
+      </c>
+      <c r="N54" s="4">
+        <f t="shared" si="5"/>
+        <v>1.1327636925090395E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>15</v>
       </c>
@@ -4930,22 +6541,41 @@
         <v>4</v>
       </c>
       <c r="D55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31.813433333333332</v>
       </c>
       <c r="E55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1908.806</v>
       </c>
       <c r="F55">
         <v>1908806</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>176</v>
+      </c>
+      <c r="J55">
+        <v>1734.233114828321</v>
+      </c>
+      <c r="K55" t="s">
+        <v>177</v>
+      </c>
+      <c r="L55">
+        <v>722.65049179999914</v>
+      </c>
+      <c r="M55">
+        <v>1479.107828259258</v>
+      </c>
+      <c r="N55" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.1471112991602164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>15</v>
       </c>
@@ -4956,22 +6586,41 @@
         <v>5</v>
       </c>
       <c r="D56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3772166666666665</v>
       </c>
       <c r="E56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>382.63299999999998</v>
       </c>
       <c r="F56">
         <v>382633</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>72</v>
+        <v>178</v>
       </c>
       <c r="H56" s="7"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>179</v>
+      </c>
+      <c r="J56">
+        <v>1490.656141002366</v>
+      </c>
+      <c r="K56" t="s">
+        <v>180</v>
+      </c>
+      <c r="L56">
+        <v>754.21830090000003</v>
+      </c>
+      <c r="M56">
+        <v>1454.7840481513599</v>
+      </c>
+      <c r="N56" s="4">
+        <f t="shared" si="5"/>
+        <v>-2.406463292525968E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>15</v>
       </c>
@@ -4982,22 +6631,41 @@
         <v>6</v>
       </c>
       <c r="D57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.927283333333332</v>
       </c>
       <c r="E57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>715.63699999999994</v>
       </c>
       <c r="F57">
         <v>715637</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>73</v>
+        <v>181</v>
       </c>
       <c r="H57" s="7"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>182</v>
+      </c>
+      <c r="J57">
+        <v>875.64538242702918</v>
+      </c>
+      <c r="K57" t="s">
+        <v>183</v>
+      </c>
+      <c r="L57">
+        <v>843.49386729999969</v>
+      </c>
+      <c r="M57">
+        <v>834.37760121061604</v>
+      </c>
+      <c r="N57" s="4">
+        <f t="shared" si="5"/>
+        <v>-4.7128417558750892E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>15</v>
       </c>
@@ -5008,22 +6676,41 @@
         <v>7</v>
       </c>
       <c r="D58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.80586666666666662</v>
       </c>
       <c r="E58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48.351999999999997</v>
       </c>
       <c r="F58">
         <v>48352</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>74</v>
+        <v>184</v>
       </c>
       <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>185</v>
+      </c>
+      <c r="J58">
+        <v>1287.259466421646</v>
+      </c>
+      <c r="K58" t="s">
+        <v>186</v>
+      </c>
+      <c r="L58">
+        <v>858.84702300000208</v>
+      </c>
+      <c r="M58">
+        <v>1275.382289345094</v>
+      </c>
+      <c r="N58" s="4">
+        <f t="shared" si="5"/>
+        <v>-9.226715659406623E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>15</v>
       </c>
@@ -5034,22 +6721,41 @@
         <v>8</v>
       </c>
       <c r="D59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20.862533333333332</v>
       </c>
       <c r="E59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1251.752</v>
       </c>
       <c r="F59">
         <v>1251752</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>75</v>
+        <v>187</v>
       </c>
       <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>188</v>
+      </c>
+      <c r="J59">
+        <v>2656.0957601557811</v>
+      </c>
+      <c r="K59" t="s">
+        <v>189</v>
+      </c>
+      <c r="L59">
+        <v>1312.5918292000019</v>
+      </c>
+      <c r="M59">
+        <v>933.66048774492606</v>
+      </c>
+      <c r="N59" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.64848387556246601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>15</v>
       </c>
@@ -5060,22 +6766,41 @@
         <v>9</v>
       </c>
       <c r="D60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.850033333333332</v>
       </c>
       <c r="E60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>831.00199999999995</v>
       </c>
       <c r="F60">
         <v>831002</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>76</v>
+        <v>190</v>
       </c>
       <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>191</v>
+      </c>
+      <c r="J60">
+        <v>928.10921743592348</v>
+      </c>
+      <c r="K60" t="s">
+        <v>192</v>
+      </c>
+      <c r="L60">
+        <v>676.07068479999725</v>
+      </c>
+      <c r="M60">
+        <v>948.70542409475468</v>
+      </c>
+      <c r="N60" s="4">
+        <f t="shared" si="5"/>
+        <v>2.2191576456628771E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>15</v>
       </c>
@@ -5086,30 +6811,49 @@
         <v>10</v>
       </c>
       <c r="D61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>463.13668333333334</v>
       </c>
       <c r="E61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27788.201000000001</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61">
         <v>27788201</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>78</v>
+        <v>193</v>
       </c>
       <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" t="s">
+        <v>194</v>
+      </c>
+      <c r="J61">
+        <v>1172.042609135658</v>
+      </c>
+      <c r="K61" t="s">
+        <v>195</v>
+      </c>
+      <c r="L61">
+        <v>741.70262700000239</v>
+      </c>
+      <c r="M61">
+        <v>1212.417268828427</v>
+      </c>
+      <c r="N61" s="4">
+        <f t="shared" si="5"/>
+        <v>3.4448115945668524E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G62" s="6"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G63" s="6"/>
       <c r="H63" s="7"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G64" s="6"/>
       <c r="H64" s="7"/>
     </row>

</xml_diff>

<commit_message>
Fixed bug that allows the metaheurstic to sometimes generate blank children. Will rerun verification on tests that had questionable results.
</commit_message>
<xml_diff>
--- a/vrp_dss/Solve Times Summary.xlsx
+++ b/vrp_dss/Solve Times Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\great\Documents\GitHub\VRP-DSS\vrp_dss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59BD14C-FA27-4769-98E0-B50078B9C5B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FE66DA-6620-4966-BF98-033B9ED749C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="197">
   <si>
     <t># Customers</t>
   </si>
@@ -1500,11 +1500,10 @@
     <t>{0: [[(7, 3), (5, 12), (1, 7)], [(7, 4), (3, 5), (9, 3), (8, 4), (6, 5)], [(2, 9), (4, 8)]], 1: []}</t>
   </si>
   <si>
-    <t xml:space="preserve">11 metre (capacity 30):
-8 metre (capacity 22):
+    <t xml:space="preserve">8 metre (capacity 22):
+5 (12) -&gt; 1 (7)
+6 (5) -&gt; 4 (8) -&gt; 2 (9)
 7 (7) -&gt; 3 (5) -&gt; 9 (3) -&gt; 8 (4)
-1 (7) -&gt; 5 (12)
-6 (5) -&gt; 4 (8) -&gt; 2 (9)
 </t>
   </si>
   <si>
@@ -1540,6 +1539,14 @@
   </si>
   <si>
     <t>{0: [], 1: [[(7, 7), (9, 11), (1, 4), (2, 5), (6, 2)], [(5, 8), (4, 9), (8, 8), (3, 5)]], 2: []}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 metre (capacity 22):
+11 metre (capacity 30):
+7 (7) -&gt; 9 (11) -&gt; 1 (4) -&gt; 2 (5) -&gt; 6 (2)
+5 (8) -&gt; 4 (9) -&gt; 8 (8) -&gt; 3 (5)
+Rigid (capacity 16):
+</t>
   </si>
   <si>
     <t>Input:
@@ -3146,7 +3153,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9338-4886-9421-C7416FC28C74}"/>
+              <c16:uniqueId val="{00000000-0D5E-46CD-90E0-0D8AC78099AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3219,7 +3226,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9338-4886-9421-C7416FC28C74}"/>
+              <c16:uniqueId val="{00000001-0D5E-46CD-90E0-0D8AC78099AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4086,10 +4093,10 @@
   <dimension ref="A1:N209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M45" sqref="M45"/>
+      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5530,20 +5537,20 @@
         <v>109</v>
       </c>
       <c r="J32">
-        <v>724.48723782131583</v>
+        <v>724.48711326831585</v>
       </c>
       <c r="K32" t="s">
         <v>110</v>
       </c>
       <c r="L32">
-        <v>317.03553440000002</v>
+        <v>309.14720440000002</v>
       </c>
       <c r="M32">
         <v>753.23582552852463</v>
       </c>
       <c r="N32" s="4">
         <f t="shared" si="2"/>
-        <v>3.9681289340115632E-2</v>
+        <v>3.9681468080939641E-2</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5577,15 +5584,18 @@
       <c r="J33">
         <v>1024.350870524725</v>
       </c>
+      <c r="K33" t="s">
+        <v>113</v>
+      </c>
       <c r="L33">
-        <v>297.15786459999981</v>
+        <v>270.34894500000001</v>
       </c>
       <c r="M33">
-        <v>0</v>
+        <v>1024.350870524725</v>
       </c>
       <c r="N33" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5610,17 +5620,17 @@
         <v>26248</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J34">
         <v>866.88826321288798</v>
       </c>
       <c r="K34" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L34">
         <v>420.53963870000013</v>
@@ -5655,17 +5665,17 @@
         <v>2249</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J35">
         <v>931.91447117107839</v>
       </c>
       <c r="K35" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L35">
         <v>305.86990820000028</v>
@@ -5700,17 +5710,17 @@
         <v>5946</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J36">
         <v>2241.807068141215</v>
       </c>
       <c r="K36" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L36">
         <v>316.42438950000002</v>
@@ -5745,17 +5755,17 @@
         <v>10698</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J37">
         <v>1326.10584170281</v>
       </c>
       <c r="K37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L37">
         <v>388.58196549999963</v>
@@ -5790,11 +5800,11 @@
         <v>6631</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J38">
         <v>622.21807644280557</v>
@@ -5832,17 +5842,17 @@
         <v>23010</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J39">
         <v>988.08515815373653</v>
       </c>
       <c r="K39" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L39">
         <v>276.81299589999981</v>
@@ -5877,17 +5887,17 @@
         <v>12555</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J40">
         <v>1367.2770599111541</v>
       </c>
       <c r="K40" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L40">
         <v>297.8125940000009</v>
@@ -5922,17 +5932,17 @@
         <v>6468</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H41" s="7"/>
       <c r="I41" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J41">
         <v>1198.896614545255</v>
       </c>
       <c r="K41" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L41">
         <v>293.25066800000059</v>
@@ -5967,17 +5977,17 @@
         <v>95015</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H42" s="7"/>
       <c r="I42" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J42">
         <v>3155.4945885752991</v>
       </c>
       <c r="K42" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L42">
         <v>418.98603239999829</v>
@@ -6012,17 +6022,17 @@
         <v>30046</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J43">
         <v>1013.155546866768</v>
       </c>
       <c r="K43" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L43">
         <v>446.54841970000052</v>
@@ -6057,17 +6067,17 @@
         <v>176437</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J44">
         <v>977.17357619100812</v>
       </c>
       <c r="K44" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L44">
         <v>415.29174580000108</v>
@@ -6102,17 +6112,17 @@
         <v>75019</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J45">
         <v>1012.611449136446</v>
       </c>
       <c r="K45" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L45">
         <v>640.17047660000026</v>
@@ -6147,17 +6157,17 @@
         <v>40203</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J46">
         <v>1401.6565058130111</v>
       </c>
       <c r="K46" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="L46">
         <v>729.52997780000078</v>
@@ -6192,17 +6202,17 @@
         <v>13732</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J47">
         <v>799.14062349535777</v>
       </c>
       <c r="K47" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="L47">
         <v>405.30707930000062</v>
@@ -6237,17 +6247,17 @@
         <v>17221</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J48">
         <v>873.69244502127435</v>
       </c>
       <c r="K48" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L48">
         <v>679.35048359999928</v>
@@ -6282,17 +6292,17 @@
         <v>26318</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J49">
         <v>1289.1298271084211</v>
       </c>
       <c r="K49" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L49">
         <v>449.06065099999978</v>
@@ -6327,17 +6337,17 @@
         <v>64992</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H50" s="7"/>
       <c r="I50" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J50">
         <v>1088.708858004286</v>
       </c>
       <c r="K50" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L50">
         <v>400.13931310000038</v>
@@ -6372,17 +6382,17 @@
         <v>327067</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H51" s="7"/>
       <c r="I51" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="J51">
         <v>1230.788478416772</v>
       </c>
       <c r="K51" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L51">
         <v>462.89721049999929</v>
@@ -6417,17 +6427,17 @@
         <v>178811</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H52" s="7"/>
       <c r="I52" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J52">
         <v>962.34315919796416</v>
       </c>
       <c r="K52" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L52">
         <v>641.09922839999854</v>
@@ -6462,17 +6472,17 @@
         <v>181385</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H53" s="7"/>
       <c r="I53" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J53">
         <v>1153.558670195504</v>
       </c>
       <c r="K53" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="L53">
         <v>1800.0106947999991</v>
@@ -6507,17 +6517,17 @@
         <v>13830</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H54" s="7"/>
       <c r="I54" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J54">
         <v>975.46261747594792</v>
       </c>
       <c r="K54" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L54">
         <v>589.63765830000193</v>
@@ -6552,17 +6562,17 @@
         <v>1908806</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H55" s="7"/>
       <c r="I55" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J55">
         <v>1734.233114828321</v>
       </c>
       <c r="K55" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="L55">
         <v>722.65049179999914</v>
@@ -6597,17 +6607,17 @@
         <v>382633</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H56" s="7"/>
       <c r="I56" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J56">
         <v>1490.656141002366</v>
       </c>
       <c r="K56" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L56">
         <v>754.21830090000003</v>
@@ -6642,17 +6652,17 @@
         <v>715637</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H57" s="7"/>
       <c r="I57" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J57">
         <v>875.64538242702918</v>
       </c>
       <c r="K57" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="L57">
         <v>843.49386729999969</v>
@@ -6687,17 +6697,17 @@
         <v>48352</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J58">
         <v>1287.259466421646</v>
       </c>
       <c r="K58" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="L58">
         <v>858.84702300000208</v>
@@ -6732,17 +6742,17 @@
         <v>1251752</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H59" s="7"/>
       <c r="I59" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J59">
         <v>2656.0957601557811</v>
       </c>
       <c r="K59" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="L59">
         <v>1312.5918292000019</v>
@@ -6777,17 +6787,17 @@
         <v>831002</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J60">
         <v>928.10921743592348</v>
       </c>
       <c r="K60" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="L60">
         <v>676.07068479999725</v>
@@ -6822,17 +6832,17 @@
         <v>27788201</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H61" s="7"/>
       <c r="I61" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J61">
         <v>1172.042609135658</v>
       </c>
       <c r="K61" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L61">
         <v>741.70262700000239</v>
@@ -7439,6 +7449,190 @@
     </row>
   </sheetData>
   <mergeCells count="208">
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G206:H206"/>
+    <mergeCell ref="G207:H207"/>
+    <mergeCell ref="G208:H208"/>
+    <mergeCell ref="G209:H209"/>
+    <mergeCell ref="G179:H179"/>
+    <mergeCell ref="G180:H180"/>
+    <mergeCell ref="G181:H181"/>
+    <mergeCell ref="G200:H200"/>
+    <mergeCell ref="G201:H201"/>
+    <mergeCell ref="G202:H202"/>
+    <mergeCell ref="G203:H203"/>
+    <mergeCell ref="G204:H204"/>
+    <mergeCell ref="G205:H205"/>
+    <mergeCell ref="G185:H185"/>
+    <mergeCell ref="G186:H186"/>
+    <mergeCell ref="G187:H187"/>
+    <mergeCell ref="G188:H188"/>
+    <mergeCell ref="G189:H189"/>
+    <mergeCell ref="G190:H190"/>
+    <mergeCell ref="G191:H191"/>
+    <mergeCell ref="G192:H192"/>
+    <mergeCell ref="G193:H193"/>
+    <mergeCell ref="G194:H194"/>
+    <mergeCell ref="G195:H195"/>
+    <mergeCell ref="G175:H175"/>
+    <mergeCell ref="G176:H176"/>
+    <mergeCell ref="G177:H177"/>
+    <mergeCell ref="G178:H178"/>
+    <mergeCell ref="G174:H174"/>
+    <mergeCell ref="G131:H131"/>
+    <mergeCell ref="G171:H171"/>
+    <mergeCell ref="G172:H172"/>
+    <mergeCell ref="G173:H173"/>
+    <mergeCell ref="G138:H138"/>
+    <mergeCell ref="G139:H139"/>
+    <mergeCell ref="G140:H140"/>
+    <mergeCell ref="G159:H159"/>
+    <mergeCell ref="G160:H160"/>
+    <mergeCell ref="G161:H161"/>
+    <mergeCell ref="G162:H162"/>
+    <mergeCell ref="G163:H163"/>
+    <mergeCell ref="G150:H150"/>
+    <mergeCell ref="G151:H151"/>
+    <mergeCell ref="G156:H156"/>
+    <mergeCell ref="G157:H157"/>
+    <mergeCell ref="G158:H158"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G121:H121"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="G118:H118"/>
+    <mergeCell ref="G119:H119"/>
+    <mergeCell ref="G120:H120"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G126:H126"/>
+    <mergeCell ref="G127:H127"/>
+    <mergeCell ref="G128:H128"/>
+    <mergeCell ref="G129:H129"/>
+    <mergeCell ref="G130:H130"/>
+    <mergeCell ref="G122:H122"/>
+    <mergeCell ref="G123:H123"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="G125:H125"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G102:H102"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="G104:H104"/>
+    <mergeCell ref="G106:H106"/>
+    <mergeCell ref="G107:H107"/>
+    <mergeCell ref="G108:H108"/>
+    <mergeCell ref="G109:H109"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G105:H105"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G153:H153"/>
+    <mergeCell ref="G154:H154"/>
+    <mergeCell ref="G155:H155"/>
+    <mergeCell ref="G141:H141"/>
+    <mergeCell ref="G142:H142"/>
+    <mergeCell ref="G143:H143"/>
+    <mergeCell ref="G144:H144"/>
+    <mergeCell ref="G145:H145"/>
+    <mergeCell ref="G146:H146"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="G98:H98"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="G81:H81"/>
     <mergeCell ref="G196:H196"/>
     <mergeCell ref="G197:H197"/>
     <mergeCell ref="G198:H198"/>
@@ -7463,190 +7657,6 @@
     <mergeCell ref="G148:H148"/>
     <mergeCell ref="G149:H149"/>
     <mergeCell ref="G152:H152"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G75:H75"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G153:H153"/>
-    <mergeCell ref="G154:H154"/>
-    <mergeCell ref="G155:H155"/>
-    <mergeCell ref="G141:H141"/>
-    <mergeCell ref="G142:H142"/>
-    <mergeCell ref="G143:H143"/>
-    <mergeCell ref="G144:H144"/>
-    <mergeCell ref="G145:H145"/>
-    <mergeCell ref="G146:H146"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="G95:H95"/>
-    <mergeCell ref="G96:H96"/>
-    <mergeCell ref="G97:H97"/>
-    <mergeCell ref="G98:H98"/>
-    <mergeCell ref="G99:H99"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G102:H102"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="G104:H104"/>
-    <mergeCell ref="G106:H106"/>
-    <mergeCell ref="G107:H107"/>
-    <mergeCell ref="G108:H108"/>
-    <mergeCell ref="G109:H109"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G105:H105"/>
-    <mergeCell ref="G126:H126"/>
-    <mergeCell ref="G127:H127"/>
-    <mergeCell ref="G128:H128"/>
-    <mergeCell ref="G129:H129"/>
-    <mergeCell ref="G130:H130"/>
-    <mergeCell ref="G122:H122"/>
-    <mergeCell ref="G123:H123"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="G125:H125"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G121:H121"/>
-    <mergeCell ref="G82:H82"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="G100:H100"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="G118:H118"/>
-    <mergeCell ref="G119:H119"/>
-    <mergeCell ref="G120:H120"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G175:H175"/>
-    <mergeCell ref="G176:H176"/>
-    <mergeCell ref="G177:H177"/>
-    <mergeCell ref="G178:H178"/>
-    <mergeCell ref="G174:H174"/>
-    <mergeCell ref="G131:H131"/>
-    <mergeCell ref="G171:H171"/>
-    <mergeCell ref="G172:H172"/>
-    <mergeCell ref="G173:H173"/>
-    <mergeCell ref="G138:H138"/>
-    <mergeCell ref="G139:H139"/>
-    <mergeCell ref="G140:H140"/>
-    <mergeCell ref="G159:H159"/>
-    <mergeCell ref="G160:H160"/>
-    <mergeCell ref="G161:H161"/>
-    <mergeCell ref="G162:H162"/>
-    <mergeCell ref="G163:H163"/>
-    <mergeCell ref="G150:H150"/>
-    <mergeCell ref="G151:H151"/>
-    <mergeCell ref="G156:H156"/>
-    <mergeCell ref="G157:H157"/>
-    <mergeCell ref="G158:H158"/>
-    <mergeCell ref="G206:H206"/>
-    <mergeCell ref="G207:H207"/>
-    <mergeCell ref="G208:H208"/>
-    <mergeCell ref="G209:H209"/>
-    <mergeCell ref="G179:H179"/>
-    <mergeCell ref="G180:H180"/>
-    <mergeCell ref="G181:H181"/>
-    <mergeCell ref="G200:H200"/>
-    <mergeCell ref="G201:H201"/>
-    <mergeCell ref="G202:H202"/>
-    <mergeCell ref="G203:H203"/>
-    <mergeCell ref="G204:H204"/>
-    <mergeCell ref="G205:H205"/>
-    <mergeCell ref="G185:H185"/>
-    <mergeCell ref="G186:H186"/>
-    <mergeCell ref="G187:H187"/>
-    <mergeCell ref="G188:H188"/>
-    <mergeCell ref="G189:H189"/>
-    <mergeCell ref="G190:H190"/>
-    <mergeCell ref="G191:H191"/>
-    <mergeCell ref="G192:H192"/>
-    <mergeCell ref="G193:H193"/>
-    <mergeCell ref="G194:H194"/>
-    <mergeCell ref="G195:H195"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Case study functions seem to be working. Time to see if the algorithm can generate a feasible solution.
</commit_message>
<xml_diff>
--- a/vrp_dss/Solve Times Summary.xlsx
+++ b/vrp_dss/Solve Times Summary.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Aaron\Documents\Git Repositories\VRP-DSS\vrp_dss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342C1D9D-9D3A-4864-B666-0B689BFFC2D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A211E6D-BCD9-459F-BA7B-42897A076F81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="3615" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="3615" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="1" r:id="rId1"/>
     <sheet name="Run Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Case Study" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="211">
   <si>
     <t># Customers</t>
   </si>
@@ -2982,6 +2983,15 @@
 5 (8) -&gt; 8 (4) -&gt; 9 (2)
 15 (6) -&gt; 13 (6)
 </t>
+  </si>
+  <si>
+    <t>Archive Routes</t>
+  </si>
+  <si>
+    <t>Archive Objective</t>
+  </si>
+  <si>
+    <t>Archive Date</t>
   </si>
 </sst>
 </file>
@@ -3037,7 +3047,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3061,6 +3071,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6255,7 +6266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -6622,7 +6633,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6634,7 +6646,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11368,4 +11380,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38517884-779F-4BC7-B6B1-F5D7B406D059}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>43745</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>43768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>43775</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First archive day solved and compared.
</commit_message>
<xml_diff>
--- a/vrp_dss/Solve Times Summary.xlsx
+++ b/vrp_dss/Solve Times Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\great\Documents\GitHub\VRP-DSS\vrp_dss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4466D013-5D62-4460-889D-92D08F0AC57D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8638591-238D-4163-BD8B-82EA98589399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="220">
   <si>
     <t># Customers</t>
   </si>
@@ -2985,12 +2985,12 @@
 </t>
   </si>
   <si>
+    <t>Archive Date</t>
+  </si>
+  <si>
     <t>Archive Routes</t>
   </si>
   <si>
-    <t>Archive Date</t>
-  </si>
-  <si>
     <t>Archive Cost</t>
   </si>
   <si>
@@ -3001,6 +3001,93 @@
   </si>
   <si>
     <t>Meta Penalty</t>
+  </si>
+  <si>
+    <t>{"2": [[[17, 24], [164, 4]], [[44, 30]], [[111, 3], [77, 27]], [[149, 28], [148, 2]], [[165, 30]], [[159, 19], [194, 11]], [[41, 30]], [[172, 30]], [[79, 30]], [[104, 30]], [[6, 23], [187, 7]], [[176, 30]], [[153, 30]], [[208, 30]], [[35, 30]], [[100, 30]], [[83, 20]], [[40, 30]], [[117, 7], [126, 14], [125, 9]], [[121, 12], [143, 11], [193, 7]], [[80, 20], [168, 9]], [[135, 5], [182, 15], [95, 10]], [[81, 30]], [[193, 12], [143, 18]], [[121, 19], [135, 10]]], "1": [[[75, 18]], [[149, 22]], [[24, 8], [25, 14]], [[207, 21]], [[72, 22]], [[119, 10], [2, 12]], [[157, 22]], [[46, 20]], [[188, 22]], [[186, 9], [53, 12]], [[130, 22]], [[83, 20]], [[116, 10], [177, 11], [203, 1]], [[27, 22]]], "0": [[[194, 16]], [[16, 10], [165, 4]], [[156, 16]], [[77, 11]], [[120, 11], [198, 5]], [[151, 16]], [[196, 8], [48, 5]], [[34, 14]], [[9, 15]], [[154, 13]], [[8, 16]], [[108, 11]], [[152, 15]], [[120, 12]], [[199, 1], [91, 6], [81, 6]], [[197, 14]], [[131, 16]], [[151, 9], [173, 7]], [[144, 12]], [[166, 6], [28, 2], [3, 8]], [[97, 13]], [[66, 15]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+81-H (16)
+186-V (9)
+8-B (16)
+121-O (16)
+135-P (15)
+173-T (7)
+130-P (16)
+208-Z (16)
+80-H (16)
+164-S (4) -&gt; 168-S (9)
+9-B (15)
+25-C (14)
+156-S (16)
+2-A (12)
+151-R (3) -&gt; 198-W (5) -&gt; 48-D (5)
+188-V (6) -&gt; 80-H (4) -&gt; 199-W (1)
+3-A (8) -&gt; 91-K (6)
+188-V (16)
+131-P (16)
+144-Q (12)
+148-R (2) -&gt; 111-M (3) -&gt; 77-H (8)
+8 Metre (capacity 22):
+66-G (15)
+119-O (10) -&gt; 83-H (10)
+151-R (22)
+120-O (1) -&gt; 97-K (13)
+75-H (18)
+120-O (22)
+72-G (22)
+108-M (11)
+152-R (15)
+34-C (14)
+121-O (15)
+193-V (19)
+19-B (10)
+196-W (8) -&gt; 53-E (12)
+11 Metre (capacity 30):
+194-V (27)
+166-S (6) -&gt; 17-B (24)
+28-C (2) -&gt; 95-K (10) -&gt; 197-W (14)
+35-C (30)
+40-C (30)
+104-M (30)
+100-L (30)
+153-S (30)
+159-S (19)
+6-B (23)
+157-S (22)
+126-P (14) -&gt; 154-S (13)
+83-H (30)
+176-T (30)
+187-V (7) -&gt; 27-C (22)
+149-R (30)
+44-D (30)
+149-R (20) -&gt; 165-S (4)
+41-C (30)
+79-H (30)
+24-B (8) -&gt; 16-B (10)
+165-S (30)
+172-S (30)
+125-P (9) -&gt; 117-N (7)
+207-Y (21) -&gt; 130-P (6)
+143-P (29)
+77-H (30)
+46-D (20) -&gt; 101-L (6)
+81-H (20)
+208-Z (14) -&gt; 182-U (15)
+203-W (1) -&gt; 177-T (11) -&gt; 116-N (10)
+</t>
+  </si>
+  <si>
+    <t>Difference (R)</t>
+  </si>
+  <si>
+    <t>Difference (%)</t>
+  </si>
+  <si>
+    <t>Meta Routes (Pretty)</t>
+  </si>
+  <si>
+    <t>Meta Routes (JSON)</t>
   </si>
 </sst>
 </file>
@@ -3071,10 +3158,10 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3290,7 +3377,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0F4E-487F-9991-AC940FA40B35}"/>
+              <c16:uniqueId val="{00000000-E5EE-4ECD-9B2B-E397DADBAD47}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3363,7 +3450,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0F4E-487F-9991-AC940FA40B35}"/>
+              <c16:uniqueId val="{00000001-E5EE-4ECD-9B2B-E397DADBAD47}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3701,7 +3788,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AD33-4D06-A575-B235B0844F42}"/>
+              <c16:uniqueId val="{00000000-3906-4646-9E1E-39ADFADFE9CA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3774,7 +3861,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AD33-4D06-A575-B235B0844F42}"/>
+              <c16:uniqueId val="{00000001-3906-4646-9E1E-39ADFADFE9CA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4113,7 +4200,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-64C9-4E63-8DDD-F9557DD28953}"/>
+              <c16:uniqueId val="{00000000-0549-4629-AF31-D85C03267BAC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4186,7 +4273,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-64C9-4E63-8DDD-F9557DD28953}"/>
+              <c16:uniqueId val="{00000001-0549-4629-AF31-D85C03267BAC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4510,7 +4597,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5392-47FD-BEA4-48B1DDEA6CFF}"/>
+              <c16:uniqueId val="{00000000-64DE-4EE5-8210-051E0268A9B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4569,7 +4656,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5392-47FD-BEA4-48B1DDEA6CFF}"/>
+              <c16:uniqueId val="{00000001-64DE-4EE5-8210-051E0268A9B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4906,7 +4993,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-447A-41F6-904C-33E19B6B06F4}"/>
+              <c16:uniqueId val="{00000000-AE02-4F69-ADBF-1A10BEB2200F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4979,7 +5066,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-447A-41F6-904C-33E19B6B06F4}"/>
+              <c16:uniqueId val="{00000001-AE02-4F69-ADBF-1A10BEB2200F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5316,7 +5403,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-138E-47DC-B035-B7165B7982A8}"/>
+              <c16:uniqueId val="{00000000-BF70-42AC-8F7D-D9D3AEB59EA7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5389,7 +5476,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-138E-47DC-B035-B7165B7982A8}"/>
+              <c16:uniqueId val="{00000001-BF70-42AC-8F7D-D9D3AEB59EA7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5443,7 +5530,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-138E-47DC-B035-B7165B7982A8}"/>
+              <c16:uniqueId val="{00000002-BF70-42AC-8F7D-D9D3AEB59EA7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5497,7 +5584,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-138E-47DC-B035-B7165B7982A8}"/>
+              <c16:uniqueId val="{00000003-BF70-42AC-8F7D-D9D3AEB59EA7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6642,8 +6729,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6667,9 +6754,9 @@
     <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="150.7109375" style="12" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="12" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="150.7109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" style="4" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" style="2" customWidth="1"/>
@@ -8773,11 +8860,11 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D61" si="6">E34/60</f>
+        <f t="shared" ref="D34:D65" si="6">E34/60</f>
         <v>0.43746666666666667</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E61" si="7">F34/1000</f>
+        <f t="shared" ref="E34:E65" si="7">F34/1000</f>
         <v>26.248000000000001</v>
       </c>
       <c r="F34">
@@ -8813,7 +8900,7 @@
         <v>883.13909655706368</v>
       </c>
       <c r="Q34" s="4">
-        <f t="shared" ref="Q34:Q61" si="9">(P34-G34)/G34</f>
+        <f t="shared" ref="Q34:Q65" si="9">(P34-G34)/G34</f>
         <v>0.21471932406368316</v>
       </c>
       <c r="R34" s="8">
@@ -8821,7 +8908,7 @@
         <v>1.8746168374625772E-2</v>
       </c>
       <c r="S34" s="8">
-        <f t="shared" ref="S34:S61" si="11">ROUND(R34,5)</f>
+        <f t="shared" ref="S34:S65" si="11">ROUND(R34,5)</f>
         <v>1.8749999999999999E-2</v>
       </c>
     </row>
@@ -11392,31 +11479,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38517884-779F-4BC7-B6B1-F5D7B406D059}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>210</v>
@@ -11425,30 +11515,62 @@
         <v>211</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>23</v>
+        <v>219</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="J1" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>43745</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="B2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2">
+        <v>469154.88979999977</v>
+      </c>
+      <c r="F2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G2">
+        <v>3603.7618333999999</v>
+      </c>
+      <c r="H2">
+        <v>455532.2174666666</v>
+      </c>
+      <c r="J2">
+        <f>C2-H2</f>
+        <v>13622.672333333176</v>
+      </c>
+      <c r="K2" s="4">
+        <f>J2/C2</f>
+        <v>2.9036620164271349E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
         <v>43768</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
         <v>43775</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Algorithm running too slow. Will profile it and try make optimisations.
</commit_message>
<xml_diff>
--- a/vrp_dss/Solve Times Summary.xlsx
+++ b/vrp_dss/Solve Times Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\great\Documents\GitHub\VRP-DSS\vrp_dss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8638591-238D-4163-BD8B-82EA98589399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04E67B4-2506-4683-BC9F-909ABCF06236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="223">
   <si>
     <t># Customers</t>
   </si>
@@ -2997,10 +2997,22 @@
     <t>Archive Penalty</t>
   </si>
   <si>
+    <t>Meta Routes (JSON)</t>
+  </si>
+  <si>
+    <t>Meta Routes (Pretty)</t>
+  </si>
+  <si>
     <t>Meta Cost</t>
   </si>
   <si>
     <t>Meta Penalty</t>
+  </si>
+  <si>
+    <t>Difference (R)</t>
+  </si>
+  <si>
+    <t>Difference (%)</t>
   </si>
   <si>
     <t>{"2": [[[17, 24], [164, 4]], [[44, 30]], [[111, 3], [77, 27]], [[149, 28], [148, 2]], [[165, 30]], [[159, 19], [194, 11]], [[41, 30]], [[172, 30]], [[79, 30]], [[104, 30]], [[6, 23], [187, 7]], [[176, 30]], [[153, 30]], [[208, 30]], [[35, 30]], [[100, 30]], [[83, 20]], [[40, 30]], [[117, 7], [126, 14], [125, 9]], [[121, 12], [143, 11], [193, 7]], [[80, 20], [168, 9]], [[135, 5], [182, 15], [95, 10]], [[81, 30]], [[193, 12], [143, 18]], [[121, 19], [135, 10]]], "1": [[[75, 18]], [[149, 22]], [[24, 8], [25, 14]], [[207, 21]], [[72, 22]], [[119, 10], [2, 12]], [[157, 22]], [[46, 20]], [[188, 22]], [[186, 9], [53, 12]], [[130, 22]], [[83, 20]], [[116, 10], [177, 11], [203, 1]], [[27, 22]]], "0": [[[194, 16]], [[16, 10], [165, 4]], [[156, 16]], [[77, 11]], [[120, 11], [198, 5]], [[151, 16]], [[196, 8], [48, 5]], [[34, 14]], [[9, 15]], [[154, 13]], [[8, 16]], [[108, 11]], [[152, 15]], [[120, 12]], [[199, 1], [91, 6], [81, 6]], [[197, 14]], [[131, 16]], [[151, 9], [173, 7]], [[144, 12]], [[166, 6], [28, 2], [3, 8]], [[97, 13]], [[66, 15]]]}</t>
@@ -3078,16 +3090,22 @@
 </t>
   </si>
   <si>
-    <t>Difference (R)</t>
-  </si>
-  <si>
-    <t>Difference (%)</t>
-  </si>
-  <si>
-    <t>Meta Routes (Pretty)</t>
-  </si>
-  <si>
-    <t>Meta Routes (JSON)</t>
+    <t>{"0": [[[37, 10], [123, 1]], [[9, 10], [48, 4]], [[196, 13], [157, 3]], [[154, 14]], [[144, 3], [49, 3]], [[34, 16]], [[63, 16]], [[108, 9], [120, 7]], [[199, 10], [74, 5]], [[93, 9], [70, 7]], [[186, 14], [151, 1]], [[91, 13], [81, 2]], [[53, 13], [95, 3]], [[197, 16]], [[131, 12], [8, 4]], [[66, 12]], [[83, 13]], [[79, 7], [77, 7]], [[120, 9], [198, 7]], [[96, 16]], [[46, 15]], [[188, 15], [39, 1]], [[151, 14], [123, 1]], [[17, 16]], [[42, 12]], [[134, 10], [171, 2]], [[62, 1], [57, 15]], [[191, 2], [94, 5]]], "1": [[[192, 21]], [[38, 22]], [[33, 9], [4, 11]], [[88, 22]], [[82, 22]], [[68, 10], [1, 4], [18, 8]], [[207, 20]], [[83, 18], [2, 4]], [[119, 12], [2, 10]], [[18, 7], [200, 15]], [[3, 22]], [[157, 21]], [[163, 17], [3, 5]], [[66, 22]]], "2": [[[33, 30]], [[4, 30]], [[32, 27]], [[81, 30]], [[8, 30]], [[55, 30]], [[44, 30]], [[77, 30]], [[159, 24], [41, 6]], [[150, 8], [172, 20]], [[98, 16], [153, 14]], [[149, 24], [148, 6]], [[149, 30]], [[165, 30]], [[172, 30]], [[15, 28]], [[6, 14], [187, 8], [194, 8]], [[176, 16], [35, 5], [209, 9]], [[153, 30]], [[104, 30]], [[100, 30]], [[110, 19], [174, 5], [104, 6]], [[16, 30]], [[156, 12], [168, 8], [132, 10]], [[72, 30]], [[29, 29]], [[35, 30]], [[41, 30]], [[194, 30]], [[79, 30]], [[208, 24], [152, 4]], [[24, 25], [25, 5]], [[25, 30]], [[117, 6], [126, 10], [125, 14]], [[40, 30]], [[59, 28]], [[92, 30]], [[139, 15], [40, 15]], [[121, 6], [143, 5], [193, 3], [19, 6], [97, 10]], [[97, 27]], [[186, 1], [95, 12], [182, 7], [101, 10]], [[49, 21], [197, 9]], [[140, 30]]]}</t>
+  </si>
+  <si>
+    <t>{"0": [[[42, 12]], [[200, 15]], [[96, 16]], [[151, 15]]], "1": [[[156, 12], [46, 15], [192, 21], [1, 4], [68, 10], [18, 15], [72, 22], [199, 10], [134, 10], [120, 16], [72, 8], [108, 9], [207, 20], [98, 16], [194, 22], [187, 8], [41, 22], [6, 14], [194, 16], [40, 22], [41, 14], [95, 15], [152, 4], [53, 13], [2, 14], [121, 6], [19, 6], [81, 22]]], "2": [[[63, 16], [17, 16], [49, 24], [132, 10], [97, 30], [9, 10], [33, 30], [74, 5], [39, 1], [188, 15], [66, 30], [25, 30], [79, 30], [148, 6], [79, 7], [165, 30], [172, 30], [16, 30], [150, 8], [24, 25], [48, 4], [149, 24], [77, 7], [168, 8], [88, 22], [8, 4], [81, 10], [66, 4], [172, 20], [38, 22], [55, 30], [25, 5], [97, 7], [143, 5], [28, 6], [157, 24], [104, 30], [153, 30], [100, 30], [197, 25], [35, 5], [144, 3], [125, 14], [126, 10], [117, 6], [149, 30], [77, 30], [44, 30], [140, 30], [3, 27], [8, 30], [4, 30], [186, 15], [37, 10], [4, 11], [123, 2], [57, 15], [94, 5], [62, 1], [93, 9], [154, 14], [29, 29], [70, 7], [193, 3], [101, 10], [75, 7], [33, 9], [135, 5], [32, 27], [196, 13], [35, 30], [176, 16], [153, 14], [159, 24], [139, 15], [82, 22], [15, 28], [40, 23], [209, 9], [208, 24], [92, 30], [59, 28], [163, 17], [131, 12], [119, 12], [83, 1], [198, 7], [171, 2], [104, 6], [174, 5], [83, 30], [91, 13], [110, 19], [34, 16], [191, 2], [182, 7]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+42-C (12)
+200-W (15)
+96-K (16)
+151-R (15)
+8 Metre (capacity 22):
+156-S (12) -&gt; 46-D (15) -&gt; 192-V (21) -&gt; 1-A (4) -&gt; 68-G (10) -&gt; 18-B (15) -&gt; 72-G (22) -&gt; 199-W (10) -&gt; 134-P (10) -&gt; 120-O (16) -&gt; 72-G (8) -&gt; 108-M (9) -&gt; 207-Y (20) -&gt; 98-L (16) -&gt; 194-V (22) -&gt; 187-V (8) -&gt; 41-C (22) -&gt; 6-B (14) -&gt; 194-V (16) -&gt; 40-C (22) -&gt; 41-C (14) -&gt; 95-K (15) -&gt; 152-R (4) -&gt; 53-E (13) -&gt; 2-A (14) -&gt; 121-O (6) -&gt; 19-B (6) -&gt; 81-H (22)
+11 Metre (capacity 30):
+63-G (16) -&gt; 17-B (16) -&gt; 49-D (24) -&gt; 132-P (10) -&gt; 97-K (30) -&gt; 9-B (10) -&gt; 33-C (30) -&gt; 74-G (5) -&gt; 39-C (1) -&gt; 188-V (15) -&gt; 66-G (30) -&gt; 25-C (30) -&gt; 79-H (30) -&gt; 148-R (6) -&gt; 79-H (7) -&gt; 165-S (30) -&gt; 172-S (30) -&gt; 16-B (30) -&gt; 150-R (8) -&gt; 24-B (25) -&gt; 48-D (4) -&gt; 149-R (24) -&gt; 77-H (7) -&gt; 168-S (8) -&gt; 88-K (22) -&gt; 8-B (4) -&gt; 81-H (10) -&gt; 66-G (4) -&gt; 172-S (20) -&gt; 38-C (22) -&gt; 55-E (30) -&gt; 25-C (5) -&gt; 97-K (7) -&gt; 143-P (5) -&gt; 28-C (6) -&gt; 157-S (24) -&gt; 104-M (30) -&gt; 153-S (30) -&gt; 100-L (30) -&gt; 197-W (25) -&gt; 35-C (5) -&gt; 144-Q (3) -&gt; 125-P (14) -&gt; 126-P (10) -&gt; 117-N (6) -&gt; 149-R (30) -&gt; 77-H (30) -&gt; 44-D (30) -&gt; 140-P (30) -&gt; 3-A (27) -&gt; 8-B (30) -&gt; 4-A (30) -&gt; 186-V (15) -&gt; 37-C (10) -&gt; 4-A (11) -&gt; 123-O (2) -&gt; 57-F (15) -&gt; 94-K (5) -&gt; 62-G (1) -&gt; 93-K (9) -&gt; 154-S (14) -&gt; 29-C (29) -&gt; 70-G (7) -&gt; 193-V (3) -&gt; 101-L (10) -&gt; 75-H (7) -&gt; 33-C (9) -&gt; 135-P (5) -&gt; 32-C (27) -&gt; 196-W (13) -&gt; 35-C (30) -&gt; 176-T (16) -&gt; 153-S (14) -&gt; 159-S (24) -&gt; 139-P (15) -&gt; 82-H (22) -&gt; 15-B (28) -&gt; 40-C (23) -&gt; 209-Z (9) -&gt; 208-Z (24) -&gt; 92-K (30) -&gt; 59-G (28) -&gt; 163-S (17) -&gt; 131-P (12) -&gt; 119-O (12) -&gt; 83-H (1) -&gt; 198-W (7) -&gt; 171-S (2) -&gt; 104-M (6) -&gt; 174-T (5) -&gt; 83-H (30) -&gt; 91-K (13) -&gt; 110-M (19) -&gt; 34-C (16) -&gt; 191-V (2) -&gt; 182-U (7)
+</t>
   </si>
 </sst>
 </file>
@@ -3377,7 +3395,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E5EE-4ECD-9B2B-E397DADBAD47}"/>
+              <c16:uniqueId val="{00000000-80EB-4E21-A3C9-EEC1972388FD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3450,7 +3468,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E5EE-4ECD-9B2B-E397DADBAD47}"/>
+              <c16:uniqueId val="{00000001-80EB-4E21-A3C9-EEC1972388FD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3788,7 +3806,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3906-4646-9E1E-39ADFADFE9CA}"/>
+              <c16:uniqueId val="{00000000-D5E5-4DF1-887D-FE288AA9C341}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3861,7 +3879,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3906-4646-9E1E-39ADFADFE9CA}"/>
+              <c16:uniqueId val="{00000001-D5E5-4DF1-887D-FE288AA9C341}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4200,7 +4218,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0549-4629-AF31-D85C03267BAC}"/>
+              <c16:uniqueId val="{00000000-05EA-4BD6-B13D-DB25E32032DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4273,7 +4291,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0549-4629-AF31-D85C03267BAC}"/>
+              <c16:uniqueId val="{00000001-05EA-4BD6-B13D-DB25E32032DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4597,7 +4615,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-64DE-4EE5-8210-051E0268A9B9}"/>
+              <c16:uniqueId val="{00000000-8757-4B64-8CE4-8F44098BBEFF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4656,7 +4674,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-64DE-4EE5-8210-051E0268A9B9}"/>
+              <c16:uniqueId val="{00000001-8757-4B64-8CE4-8F44098BBEFF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4993,7 +5011,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AE02-4F69-ADBF-1A10BEB2200F}"/>
+              <c16:uniqueId val="{00000000-AAF9-427E-B7EA-3FE51A89D5A3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5066,7 +5084,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AE02-4F69-ADBF-1A10BEB2200F}"/>
+              <c16:uniqueId val="{00000001-AAF9-427E-B7EA-3FE51A89D5A3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5403,7 +5421,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BF70-42AC-8F7D-D9D3AEB59EA7}"/>
+              <c16:uniqueId val="{00000000-2D6F-46E4-BA41-AB9837C74F60}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5476,7 +5494,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BF70-42AC-8F7D-D9D3AEB59EA7}"/>
+              <c16:uniqueId val="{00000001-2D6F-46E4-BA41-AB9837C74F60}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5530,7 +5548,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-BF70-42AC-8F7D-D9D3AEB59EA7}"/>
+              <c16:uniqueId val="{00000002-2D6F-46E4-BA41-AB9837C74F60}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5584,7 +5602,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-BF70-42AC-8F7D-D9D3AEB59EA7}"/>
+              <c16:uniqueId val="{00000003-2D6F-46E4-BA41-AB9837C74F60}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11483,7 +11501,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11497,8 +11515,8 @@
     <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -11515,19 +11533,19 @@
         <v>211</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>216</v>
@@ -11541,13 +11559,13 @@
         <v>43745</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C2">
         <v>469154.88979999977</v>
       </c>
       <c r="F2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="G2">
         <v>3603.7618333999999</v>
@@ -11567,6 +11585,35 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>43768</v>
+      </c>
+      <c r="B3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3">
+        <v>536358.08533333312</v>
+      </c>
+      <c r="E3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G3">
+        <v>3603.2390693000002</v>
+      </c>
+      <c r="H3">
+        <v>234205.035</v>
+      </c>
+      <c r="I3">
+        <v>46576.329196977233</v>
+      </c>
+      <c r="J3" s="2">
+        <f>C3-(H3+I3*10)</f>
+        <v>-163610.24163643923</v>
+      </c>
+      <c r="K3" s="4">
+        <f>J3/C3</f>
+        <v>-0.30503920069510942</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Minor bug fixes. More live data validation.
</commit_message>
<xml_diff>
--- a/vrp_dss/Solve Times Summary.xlsx
+++ b/vrp_dss/Solve Times Summary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -44,13 +44,49 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF9C5700"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,11 +98,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -80,7 +119,9 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -90,10 +131,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="15" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="15" fontId="5" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
   </cellStyles>
   <dxfs count="19">
     <dxf>
@@ -801,13 +848,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>281.1203354</v>
+                  <v>248.36392408</v>
                 </pt>
                 <pt idx="1">
-                  <v>417.3269438799999</v>
+                  <v>371.6756806900001</v>
                 </pt>
                 <pt idx="2">
-                  <v>724.82864351</v>
+                  <v>537.5725834300001</v>
                 </pt>
               </numCache>
             </numRef>
@@ -869,13 +916,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>313.6798690800001</v>
+                  <v>259.5535755800001</v>
                 </pt>
                 <pt idx="1">
-                  <v>483.74806733</v>
+                  <v>393.3559107399998</v>
                 </pt>
                 <pt idx="2">
-                  <v>724.0348672500002</v>
+                  <v>642.3157155900002</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1196,13 +1243,13 @@
                 <formatCode>0.00%</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>-0.008496755677928482</v>
+                  <v>-0.01156526716209559</v>
                 </pt>
                 <pt idx="1">
-                  <v>-0.01060986420560815</v>
+                  <v>-0.01060943282509886</v>
                 </pt>
                 <pt idx="2">
-                  <v>-0.01059784314491593</v>
+                  <v>3.002299032413779</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1264,13 +1311,13 @@
                 <formatCode>0.00%</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>-0.01448237860497617</v>
+                  <v>-0.01122460091527198</v>
                 </pt>
                 <pt idx="1">
-                  <v>-0.0008080817553967817</v>
+                  <v>0.01322179491490654</v>
                 </pt>
                 <pt idx="2">
-                  <v>-0.02014286014801766</v>
+                  <v>-0.00821107375936006</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1577,13 +1624,13 @@
                 <formatCode>0</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>5</v>
+                  <v>6</v>
                 </pt>
                 <pt idx="1">
                   <v>7</v>
                 </pt>
                 <pt idx="2">
-                  <v>7</v>
+                  <v>6</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1634,7 +1681,7 @@
                   <v>2</v>
                 </pt>
                 <pt idx="1">
-                  <v>6</v>
+                  <v>3</v>
                 </pt>
                 <pt idx="2">
                   <v>1</v>
@@ -1955,13 +2002,13 @@
                 <formatCode>0.00%</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>-0.008496755677928482</v>
+                  <v>-0.01156526716209559</v>
                 </pt>
                 <pt idx="1">
-                  <v>-0.01060986420560815</v>
+                  <v>-0.01060943282509886</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.01055830368643872</v>
+                  <v>3.358221276541197</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2023,13 +2070,13 @@
                 <formatCode>0.00%</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>-0.0004885318303873518</v>
+                  <v>0.00060018667944594</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.01452658024087916</v>
+                  <v>0.03011533209677175</v>
                 </pt>
                 <pt idx="2">
-                  <v>-0.006035948649591364</v>
+                  <v>0.006668596132344186</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2348,13 +2395,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>281.1203354</v>
+                  <v>248.36392408</v>
                 </pt>
                 <pt idx="1">
-                  <v>417.3269438799999</v>
+                  <v>371.6756806900001</v>
                 </pt>
                 <pt idx="2">
-                  <v>724.82864351</v>
+                  <v>537.5725834300001</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2416,13 +2463,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>313.6798690800001</v>
+                  <v>259.5535755800001</v>
                 </pt>
                 <pt idx="1">
-                  <v>483.74806733</v>
+                  <v>393.3559107399998</v>
                 </pt>
                 <pt idx="2">
-                  <v>724.0348672500002</v>
+                  <v>642.3157155900002</v>
                 </pt>
               </numCache>
             </numRef>
@@ -3660,11 +3707,11 @@
   </sheetPr>
   <dimension ref="A1:V208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O61" sqref="O61"/>
+      <selection pane="bottomRight" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3844,7 +3891,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>681.6470555638167</v>
+        <v>681.3944735908287</v>
       </c>
       <c r="L2" s="4" t="n">
         <v>0.1894691799941965</v>
@@ -3855,18 +3902,18 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 metre (capacity 22):
-6 (6) -&gt; 9 (9)
-11 metre (capacity 30):
-7 (5) -&gt; 8 (2) -&gt; 3 (2) -&gt; 1 (5) -&gt; 5 (3) -&gt; 4 (6) -&gt; 2 (1)
+          <t xml:space="preserve">11 metre (capacity 30):
+6 (6) -&gt; 2 (1) -&gt; 4 (6) -&gt; 5 (3) -&gt; 1 (5) -&gt; 3 (2) -&gt; 8 (2) -&gt; 7 (5)
+8 metre (capacity 22):
+9 (9)
 </t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>262.4696638</v>
+        <v>233.5733909</v>
       </c>
       <c r="P2" t="n">
-        <v>737.8909945016305</v>
+        <v>681.3944735908287</v>
       </c>
       <c r="Q2" s="4">
         <f>(P2-G2)/G2</f>
@@ -3954,15 +4001,15 @@
       <c r="N3" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
+8 metre (capacity 22):
+6 (6) -&gt; 1 (7) -&gt; 2 (3)
 11 metre (capacity 30):
-8 (8) -&gt; 4 (2) -&gt; 3 (6) -&gt; 5 (3) -&gt; 7 (8) -&gt; 9 (1)
-8 metre (capacity 22):
-2 (3) -&gt; 1 (7) -&gt; 6 (6)
+9 (1) -&gt; 7 (8) -&gt; 5 (3) -&gt; 3 (6) -&gt; 4 (2) -&gt; 8 (8)
 </t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>278.0197951</v>
+        <v>237.247164</v>
       </c>
       <c r="P3" t="n">
         <v>662.804511678134</v>
@@ -4049,7 +4096,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>1121.506775041001</v>
+        <v>1121.506653578627</v>
       </c>
       <c r="L4" s="4" t="n">
         <v>0.1888574501594993</v>
@@ -4061,16 +4108,16 @@
       <c r="N4" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
-2 (2) -&gt; 5 (1) -&gt; 8 (2) -&gt; 3 (3) -&gt; 7 (3) -&gt; 4 (1) -&gt; 9 (4)
-6 (3) -&gt; 1 (5)
+2 (2) -&gt; 5 (1) -&gt; 8 (2) -&gt; 3 (3) -&gt; 7 (3) -&gt; 4 (1)
+9 (4) -&gt; 6 (3) -&gt; 1 (5)
 </t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>278.1032905000001</v>
+        <v>248.9852562</v>
       </c>
       <c r="P4" t="n">
-        <v>1017.840597157414</v>
+        <v>1064.39489829658</v>
       </c>
       <c r="Q4" s="4">
         <f>(P4-G4)/G4</f>
@@ -4168,7 +4215,7 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>277.5459385</v>
+        <v>246.7568436</v>
       </c>
       <c r="P5" t="n">
         <v>648.7782890113363</v>
@@ -4247,7 +4294,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>1096.36016908566</v>
+        <v>1096.360166127857</v>
       </c>
       <c r="L6" s="4" t="n">
         <v>0.1192523719444274</v>
@@ -4258,16 +4305,16 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
-8 (5) -&gt; 7 (3)
-8 metre (capacity 22):
+          <t xml:space="preserve">8 metre (capacity 22):
 9 (4) -&gt; 3 (7) -&gt; 5 (4) -&gt; 6 (5)
 4 (2) -&gt; 1 (7) -&gt; 2 (4)
+Rigid (capacity 16):
+8 (5) -&gt; 7 (3)
 </t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>260.3492017999999</v>
+        <v>274.5532626</v>
       </c>
       <c r="P6" t="n">
         <v>1077.694700234683</v>
@@ -4357,15 +4404,16 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
+          <t xml:space="preserve">8 metre (capacity 22):
+5 (8) -&gt; 3 (8) -&gt; 8 (3) -&gt; 2 (2)
+11 metre (capacity 30):
+Rigid (capacity 16):
 9 (2) -&gt; 4 (2) -&gt; 1 (1) -&gt; 6 (3) -&gt; 7 (8)
-8 metre (capacity 22):
-5 (8) -&gt; 3 (8) -&gt; 8 (3) -&gt; 2 (2)
 </t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>317.7635937</v>
+        <v>242.1010329000001</v>
       </c>
       <c r="P7" t="n">
         <v>520.3454981535883</v>
@@ -4463,7 +4511,7 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>270.7247927</v>
+        <v>234.060618</v>
       </c>
       <c r="P8" t="n">
         <v>996.8146493389403</v>
@@ -4555,20 +4603,20 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 metre (capacity 22):
-1 (3) -&gt; 3 (4) -&gt; 2 (6)
-Rigid (capacity 16):
+          <t xml:space="preserve">Rigid (capacity 16):
 6 (8) -&gt; 7 (8)
 11 metre (capacity 30):
 9 (3) -&gt; 8 (8) -&gt; 5 (7) -&gt; 4 (8)
+8 metre (capacity 22):
+1 (3) -&gt; 3 (4) -&gt; 2 (6)
 </t>
         </is>
       </c>
       <c r="O9" t="n">
-        <v>304.0242498</v>
+        <v>273.31324</v>
       </c>
       <c r="P9" t="n">
-        <v>775.2155363921825</v>
+        <v>775.2155363921826</v>
       </c>
       <c r="Q9" s="4">
         <f>(P9-G9)/G9</f>
@@ -4656,16 +4704,16 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 metre (capacity 30):
+          <t xml:space="preserve">Rigid (capacity 16):
+8 (4) -&gt; 6 (7) -&gt; 3 (2) -&gt; 1 (1)
+5 (6) -&gt; 2 (3) -&gt; 9 (2) -&gt; 7 (2)
+11 metre (capacity 30):
 4 (7)
-Rigid (capacity 16):
-1 (1) -&gt; 3 (2) -&gt; 6 (7) -&gt; 8 (4)
-7 (2) -&gt; 9 (2) -&gt; 2 (3) -&gt; 5 (6)
 </t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>294.104108</v>
+        <v>234.5970427999999</v>
       </c>
       <c r="P10" t="n">
         <v>732.7210841010763</v>
@@ -4743,7 +4791,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>675.318142023948</v>
+        <v>675.3177456547439</v>
       </c>
       <c r="L11" s="4" t="n">
         <v>0.1913813618635446</v>
@@ -4755,17 +4803,17 @@
       <c r="N11" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
+3 (3) -&gt; 5 (4) -&gt; 9 (4) -&gt; 2 (6) -&gt; 4 (1) -&gt; 1 (4) -&gt; 6 (5)
 8 metre (capacity 22):
-4 (1) -&gt; 1 (4) -&gt; 6 (5)
-8 (1) -&gt; 7 (1) -&gt; 5 (4) -&gt; 9 (4) -&gt; 2 (6) -&gt; 3 (3)
+7 (1) -&gt; 8 (1)
 </t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>268.0987201</v>
+        <v>258.4513898</v>
       </c>
       <c r="P11" t="n">
-        <v>695.4038653520677</v>
+        <v>702.370105707741</v>
       </c>
       <c r="Q11" s="4">
         <f>(P11-G11)/G11</f>
@@ -4859,15 +4907,15 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
-2 (7) -&gt; 10 (7) -&gt; 7 (2)
-11 metre (capacity 30):
+          <t xml:space="preserve">11 metre (capacity 30):
 3 (1) -&gt; 4 (5) -&gt; 5 (4) -&gt; 12 (3) -&gt; 9 (5) -&gt; 6 (5) -&gt; 8 (2) -&gt; 11 (3) -&gt; 1 (2)
+Rigid (capacity 16):
+7 (2) -&gt; 10 (7) -&gt; 2 (7)
 </t>
         </is>
       </c>
       <c r="O12" t="n">
-        <v>464.7078033999999</v>
+        <v>411.7896006000001</v>
       </c>
       <c r="P12" t="n">
         <v>914.8582852133327</v>
@@ -4963,15 +5011,16 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
-3 (3) -&gt; 12 (2) -&gt; 10 (2) -&gt; 8 (3) -&gt; 9 (1)
-8 metre (capacity 22):
+          <t xml:space="preserve">8 metre (capacity 22):
 2 (1) -&gt; 7 (3) -&gt; 11 (2) -&gt; 1 (2) -&gt; 5 (4) -&gt; 4 (4) -&gt; 6 (3)
+Rigid (capacity 16):
+9 (1) -&gt; 8 (3) -&gt; 10 (2) -&gt; 12 (2) -&gt; 3 (3)
+11 metre (capacity 30):
 </t>
         </is>
       </c>
       <c r="O13" t="n">
-        <v>406.5890359</v>
+        <v>428.6970002000003</v>
       </c>
       <c r="P13" t="n">
         <v>723.7591313441118</v>
@@ -5069,13 +5118,14 @@
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
 11 (4) -&gt; 3 (5) -&gt; 2 (1) -&gt; 4 (1) -&gt; 10 (3) -&gt; 6 (2) -&gt; 9 (3)
+8 metre (capacity 22):
 Rigid (capacity 16):
-8 (2) -&gt; 7 (1) -&gt; 5 (3) -&gt; 1 (4) -&gt; 12 (5)
+12 (5) -&gt; 1 (4) -&gt; 5 (3) -&gt; 7 (1) -&gt; 8 (2)
 </t>
         </is>
       </c>
       <c r="O14" t="n">
-        <v>419.6642604000003</v>
+        <v>359.7548925000001</v>
       </c>
       <c r="P14" t="n">
         <v>869.7301452494198</v>
@@ -5172,13 +5222,13 @@
       <c r="N15" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-9 (3) -&gt; 8 (5) -&gt; 6 (7) -&gt; 2 (6) -&gt; 11 (8)
-3 (1) -&gt; 12 (1) -&gt; 7 (4) -&gt; 1 (4) -&gt; 5 (8) -&gt; 10 (5) -&gt; 4 (5)
+11 (8) -&gt; 2 (6) -&gt; 6 (7) -&gt; 8 (5) -&gt; 9 (3)
+4 (5) -&gt; 10 (5) -&gt; 5 (8) -&gt; 1 (4) -&gt; 7 (4) -&gt; 12 (1) -&gt; 3 (1)
 </t>
         </is>
       </c>
       <c r="O15" t="n">
-        <v>422.6475539999997</v>
+        <v>154.5560035</v>
       </c>
       <c r="P15" t="n">
         <v>894.7881079632774</v>
@@ -5263,7 +5313,7 @@
         </is>
       </c>
       <c r="K16" t="n">
-        <v>1027.364256635447</v>
+        <v>1027.361501897991</v>
       </c>
       <c r="L16" s="4" t="n">
         <v>0.1301255368659235</v>
@@ -5277,12 +5327,13 @@
           <t xml:space="preserve">8 metre (capacity 22):
 4 (3) -&gt; 6 (1) -&gt; 10 (5) -&gt; 3 (1) -&gt; 7 (2) -&gt; 1 (4) -&gt; 9 (1) -&gt; 2 (5)
 11 metre (capacity 30):
-12 (4) -&gt; 11 (2) -&gt; 8 (3) -&gt; 5 (3)
+5 (3) -&gt; 8 (3) -&gt; 11 (2) -&gt; 12 (4)
+Rigid (capacity 16):
 </t>
         </is>
       </c>
       <c r="O16" t="n">
-        <v>442.3488585</v>
+        <v>452.9247354000004</v>
       </c>
       <c r="P16" t="n">
         <v>1018.647370722324</v>
@@ -5368,7 +5419,7 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>999.2141067261238</v>
+        <v>999.2122708225403</v>
       </c>
       <c r="L17" s="4" t="n">
         <v>0.2401357380254352</v>
@@ -5382,12 +5433,12 @@
           <t xml:space="preserve">8 metre (capacity 22):
 10 (5) -&gt; 11 (3) -&gt; 9 (3) -&gt; 7 (3) -&gt; 1 (3) -&gt; 12 (5)
 11 metre (capacity 30):
-4 (6) -&gt; 6 (2) -&gt; 2 (6) -&gt; 3 (3) -&gt; 5 (7) -&gt; 8 (6)
+8 (6) -&gt; 5 (7) -&gt; 3 (3) -&gt; 2 (6) -&gt; 6 (2) -&gt; 4 (6)
 </t>
         </is>
       </c>
       <c r="O17" t="n">
-        <v>426.3625585999998</v>
+        <v>314.9303991000006</v>
       </c>
       <c r="P17" t="n">
         <v>900.145864498372</v>
@@ -5483,15 +5534,16 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
-10 (5) -&gt; 8 (2) -&gt; 5 (3) -&gt; 4 (4)
-11 metre (capacity 30):
+          <t xml:space="preserve">11 metre (capacity 30):
 7 (6) -&gt; 6 (5) -&gt; 11 (5) -&gt; 9 (3) -&gt; 2 (1) -&gt; 12 (2) -&gt; 3 (4) -&gt; 1 (1)
+Rigid (capacity 16):
+4 (4) -&gt; 5 (3) -&gt; 8 (2) -&gt; 10 (5)
+8 metre (capacity 22):
 </t>
         </is>
       </c>
       <c r="O18" t="n">
-        <v>370.2218480000001</v>
+        <v>315.9241723000005</v>
       </c>
       <c r="P18" t="n">
         <v>782.003935883964</v>
@@ -5588,16 +5640,16 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 metre (capacity 30):
-3 (4) -&gt; 2 (5) -&gt; 9 (7) -&gt; 4 (2) -&gt; 7 (5) -&gt; 5 (5)
-8 metre (capacity 22):
+          <t xml:space="preserve">8 metre (capacity 22):
 12 (7) -&gt; 10 (7) -&gt; 11 (5)
-8 (5) -&gt; 6 (7) -&gt; 1 (7)
+1 (7) -&gt; 6 (7) -&gt; 8 (5)
+11 metre (capacity 30):
+5 (5) -&gt; 7 (5) -&gt; 4 (2) -&gt; 9 (7) -&gt; 2 (5) -&gt; 3 (4)
 </t>
         </is>
       </c>
       <c r="O19" t="n">
-        <v>438.1995923999993</v>
+        <v>472.7646245</v>
       </c>
       <c r="P19" t="n">
         <v>1219.039143534927</v>
@@ -5693,14 +5745,15 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 metre (capacity 30):
-10 (5) -&gt; 2 (5) -&gt; 3 (2) -&gt; 7 (6)
+          <t xml:space="preserve">8 metre (capacity 22):
+11 metre (capacity 30):
+7 (6) -&gt; 3 (2) -&gt; 2 (5) -&gt; 10 (5)
 11 (2) -&gt; 8 (7) -&gt; 9 (4) -&gt; 4 (2) -&gt; 5 (1) -&gt; 6 (6) -&gt; 12 (3) -&gt; 1 (3)
 </t>
         </is>
       </c>
       <c r="O20" t="n">
-        <v>395.948703</v>
+        <v>437.1781145</v>
       </c>
       <c r="P20" t="n">
         <v>1095.786848590677</v>
@@ -5799,12 +5852,12 @@
           <t xml:space="preserve">Rigid (capacity 16):
 3 (1) -&gt; 9 (2) -&gt; 1 (2) -&gt; 12 (1) -&gt; 8 (1) -&gt; 2 (1) -&gt; 4 (3) -&gt; 7 (2) -&gt; 10 (2)
 8 metre (capacity 22):
-6 (3) -&gt; 5 (4) -&gt; 11 (5)
+11 (5) -&gt; 5 (4) -&gt; 6 (3)
 </t>
         </is>
       </c>
       <c r="O21" t="n">
-        <v>386.5792246</v>
+        <v>368.2372643</v>
       </c>
       <c r="P21" t="n">
         <v>735.0974435515864</v>
@@ -5908,14 +5961,14 @@
       <c r="N22" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
-14 (5) -&gt; 6 (5) -&gt; 3 (2) -&gt; 10 (4) -&gt; 5 (3)
+5 (3) -&gt; 10 (4) -&gt; 3 (2) -&gt; 6 (5) -&gt; 14 (5)
+2 (4) -&gt; 13 (5) -&gt; 11 (4) -&gt; 12 (1)
 8 (1) -&gt; 9 (2) -&gt; 15 (3) -&gt; 4 (5) -&gt; 1 (2) -&gt; 7 (3)
-2 (4) -&gt; 13 (5) -&gt; 11 (4) -&gt; 12 (1)
 </t>
         </is>
       </c>
       <c r="O22" t="n">
-        <v>672.4708048000002</v>
+        <v>238.2298800999999</v>
       </c>
       <c r="P22" t="n">
         <v>1281.2391705977</v>
@@ -6019,15 +6072,15 @@
       <c r="N23" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
+2 (1) -&gt; 9 (2) -&gt; 4 (4) -&gt; 1 (4) -&gt; 15 (1)
 13 (4) -&gt; 5 (3) -&gt; 6 (1) -&gt; 10 (4) -&gt; 3 (1)
-2 (1) -&gt; 9 (2) -&gt; 4 (4) -&gt; 1 (4) -&gt; 15 (1)
 8 metre (capacity 22):
-8 (4) -&gt; 12 (3) -&gt; 7 (3) -&gt; 14 (3) -&gt; 11 (2)
+11 (2) -&gt; 14 (3) -&gt; 7 (3) -&gt; 12 (3) -&gt; 8 (4)
 </t>
         </is>
       </c>
       <c r="O23" t="n">
-        <v>699.7963949000005</v>
+        <v>503.3568825</v>
       </c>
       <c r="P23" t="n">
         <v>977.4665241543858</v>
@@ -6130,19 +6183,19 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 metre (capacity 22):
+          <t xml:space="preserve">Rigid (capacity 16):
+3 (3) -&gt; 8 (2) -&gt; 12 (2) -&gt; 4 (3) -&gt; 15 (4)
+6 (3) -&gt; 13 (2)
+8 metre (capacity 22):
 7 (2) -&gt; 5 (2) -&gt; 2 (4) -&gt; 1 (3) -&gt; 14 (1) -&gt; 11 (1) -&gt; 10 (4) -&gt; 9 (4)
-Rigid (capacity 16):
-6 (3)
-15 (4) -&gt; 4 (3) -&gt; 12 (2) -&gt; 8 (2) -&gt; 3 (3) -&gt; 13 (2)
 </t>
         </is>
       </c>
       <c r="O24" t="n">
-        <v>701.5370033999998</v>
+        <v>551.2556817999998</v>
       </c>
       <c r="P24" t="n">
-        <v>916.3267486812994</v>
+        <v>941.029672863207</v>
       </c>
       <c r="Q24" s="4">
         <f>(P24-G24)/G24</f>
@@ -6242,14 +6295,14 @@
       <c r="N25" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-15 (1) -&gt; 7 (5) -&gt; 10 (4) -&gt; 6 (4) -&gt; 1 (5) -&gt; 12 (1) -&gt; 3 (1) -&gt; 9 (5) -&gt; 14 (3)
+14 (3) -&gt; 9 (5) -&gt; 3 (1) -&gt; 12 (1) -&gt; 1 (5) -&gt; 6 (4) -&gt; 10 (4) -&gt; 7 (5) -&gt; 15 (1)
 8 metre (capacity 22):
 13 (2) -&gt; 8 (5) -&gt; 11 (3) -&gt; 4 (1) -&gt; 2 (3) -&gt; 5 (4)
 </t>
         </is>
       </c>
       <c r="O25" t="n">
-        <v>583.4862115999995</v>
+        <v>491.1873168999999</v>
       </c>
       <c r="P25" t="n">
         <v>1139.100511867154</v>
@@ -6353,17 +6406,17 @@
       <c r="N26" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
+10 (2) -&gt; 2 (2) -&gt; 6 (3) -&gt; 14 (2) -&gt; 11 (3)
 8 (3) -&gt; 5 (2) -&gt; 12 (3) -&gt; 9 (4) -&gt; 3 (3)
-4 (3) -&gt; 7 (3) -&gt; 15 (2) -&gt; 13 (2)
-11 (3) -&gt; 14 (2) -&gt; 6 (3) -&gt; 2 (2) -&gt; 10 (2) -&gt; 1 (4)
+13 (2) -&gt; 15 (2) -&gt; 7 (3) -&gt; 4 (3) -&gt; 1 (4)
 </t>
         </is>
       </c>
       <c r="O26" t="n">
-        <v>892.9698130999986</v>
+        <v>677.3077531000001</v>
       </c>
       <c r="P26" t="n">
-        <v>1026.542152900709</v>
+        <v>1050.73661222106</v>
       </c>
       <c r="Q26" s="4">
         <f>(P26-G26)/G26</f>
@@ -6463,17 +6516,17 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
-1 (3) -&gt; 15 (3) -&gt; 9 (3) -&gt; 6 (1) -&gt; 3 (5) -&gt; 12 (1)
+          <t xml:space="preserve">8 metre (capacity 22):
+14 (1) -&gt; 7 (2) -&gt; 11 (5) -&gt; 10 (3) -&gt; 13 (3) -&gt; 4 (4) -&gt; 2 (1) -&gt; 5 (1)
+Rigid (capacity 16):
+12 (1) -&gt; 3 (5) -&gt; 6 (1) -&gt; 9 (3) -&gt; 15 (3) -&gt; 1 (3)
 11 metre (capacity 30):
 8 (4)
-8 metre (capacity 22):
-14 (1) -&gt; 7 (2) -&gt; 11 (5) -&gt; 10 (3) -&gt; 13 (3) -&gt; 4 (4) -&gt; 2 (1) -&gt; 5 (1)
 </t>
         </is>
       </c>
       <c r="O27" t="n">
-        <v>630.2492390000007</v>
+        <v>808.7153081000001</v>
       </c>
       <c r="P27" t="n">
         <v>1204.045683633422</v>
@@ -6578,17 +6631,15 @@
       <c r="N28" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
-10 (3) -&gt; 14 (4) -&gt; 15 (1) -&gt; 6 (4) -&gt; 2 (4)
-11 (2) -&gt; 5 (4) -&gt; 12 (4) -&gt; 13 (4) -&gt; 3 (2)
-4 (3) -&gt; 7 (4) -&gt; 9 (3) -&gt; 1 (2) -&gt; 8 (4)
+12 (4) -&gt; 15 (1) -&gt; 1 (2) -&gt; 13 (4) -&gt; 11 (2) -&gt; 4 (3) -&gt; 3 (2) -&gt; 5 (4) -&gt; 9 (3) -&gt; 6 (4) -&gt; 7 (4) -&gt; 10 (3) -&gt; 2 (4) -&gt; 14 (4) -&gt; 8 (4)
 </t>
         </is>
       </c>
       <c r="O28" t="n">
-        <v>1224.071597600001</v>
+        <v>558.2765410000002</v>
       </c>
       <c r="P28" t="n">
-        <v>1175.400466091642</v>
+        <v>34366.16663506354</v>
       </c>
       <c r="Q28" s="4">
         <f>(P28-G28)/G28</f>
@@ -6676,7 +6727,7 @@
         </is>
       </c>
       <c r="K29" t="n">
-        <v>1053.107964725544</v>
+        <v>1053.105328796254</v>
       </c>
       <c r="L29" s="4" t="n">
         <v>0.3520562442837285</v>
@@ -6689,13 +6740,13 @@
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
 8 metre (capacity 22):
+8 (3) -&gt; 4 (2) -&gt; 5 (1) -&gt; 7 (3) -&gt; 11 (3) -&gt; 1 (1) -&gt; 2 (1)
 9 (1) -&gt; 14 (4) -&gt; 6 (2) -&gt; 3 (2) -&gt; 12 (3) -&gt; 15 (1) -&gt; 13 (2) -&gt; 10 (1)
-8 (3) -&gt; 4 (2) -&gt; 5 (1) -&gt; 7 (3) -&gt; 11 (3) -&gt; 1 (1) -&gt; 2 (1)
 </t>
         </is>
       </c>
       <c r="O29" t="n">
-        <v>512.5885275000001</v>
+        <v>453.0893558000002</v>
       </c>
       <c r="P29" t="n">
         <v>841.4299311216971</v>
@@ -6786,7 +6837,7 @@
         </is>
       </c>
       <c r="K30" t="n">
-        <v>1286.410260777525</v>
+        <v>1286.331534759897</v>
       </c>
       <c r="L30" s="4" t="n">
         <v>0.11181446591527</v>
@@ -6798,17 +6849,17 @@
       <c r="N30" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
-13 (3) -&gt; 6 (6) -&gt; 1 (3) -&gt; 8 (4) -&gt; 4 (2) -&gt; 12 (2) -&gt; 11 (2)
+2 (1) -&gt; 9 (6) -&gt; 15 (3) -&gt; 3 (2) -&gt; 12 (2) -&gt; 4 (2) -&gt; 8 (4) -&gt; 11 (2)
 11 metre (capacity 30):
-14 (1) -&gt; 10 (4) -&gt; 7 (6) -&gt; 5 (5) -&gt; 9 (6) -&gt; 3 (2) -&gt; 15 (3) -&gt; 2 (1)
+14 (1) -&gt; 5 (5) -&gt; 10 (4) -&gt; 7 (6) -&gt; 13 (3) -&gt; 6 (6) -&gt; 1 (3)
 </t>
         </is>
       </c>
       <c r="O30" t="n">
-        <v>868.0086797000004</v>
+        <v>598.4948423999999</v>
       </c>
       <c r="P30" t="n">
-        <v>1323.487054912182</v>
+        <v>1286.331534759897</v>
       </c>
       <c r="Q30" s="4">
         <f>(P30-G30)/G30</f>
@@ -6910,12 +6961,12 @@
           <t xml:space="preserve">8 metre (capacity 22):
 6 (1) -&gt; 15 (1) -&gt; 1 (1) -&gt; 12 (1) -&gt; 10 (2) -&gt; 5 (3) -&gt; 11 (1) -&gt; 7 (4) -&gt; 14 (2) -&gt; 9 (1)
 Rigid (capacity 16):
-8 (1) -&gt; 2 (4) -&gt; 3 (3) -&gt; 13 (3) -&gt; 4 (4)
+4 (4) -&gt; 13 (3) -&gt; 3 (3) -&gt; 2 (4) -&gt; 8 (1)
 </t>
         </is>
       </c>
       <c r="O31" t="n">
-        <v>463.1081634999991</v>
+        <v>495.8122725999997</v>
       </c>
       <c r="P31" t="n">
         <v>856.8045807289046</v>
@@ -6998,7 +7049,7 @@
         </is>
       </c>
       <c r="K32" t="n">
-        <v>724.4871132683159</v>
+        <v>724.4870426166991</v>
       </c>
       <c r="L32" s="4" t="n">
         <v>0.2664009757385997</v>
@@ -7010,17 +7061,19 @@
       <c r="N32" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
-5 (12) -&gt; 1 (7)
-6 (5) -&gt; 4 (8) -&gt; 2 (9)
+6 (5)
 7 (7) -&gt; 3 (5) -&gt; 9 (3) -&gt; 8 (4)
+1 (7) -&gt; 5 (12)
+4 (8) -&gt; 2 (9)
+11 metre (capacity 30):
 </t>
         </is>
       </c>
       <c r="O32" t="n">
-        <v>309.1472044</v>
+        <v>228.2156266000002</v>
       </c>
       <c r="P32" t="n">
-        <v>753.2358255285246</v>
+        <v>754.9499541567666</v>
       </c>
       <c r="Q32" s="4">
         <f>(P32-G32)/G32</f>
@@ -7110,18 +7163,19 @@
       <c r="N33" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
+4 (9) -&gt; 8 (8) -&gt; 3 (5)
 11 metre (capacity 30):
 7 (7) -&gt; 9 (11) -&gt; 1 (4) -&gt; 2 (5) -&gt; 6 (2)
-5 (8) -&gt; 4 (9) -&gt; 8 (8) -&gt; 3 (5)
 Rigid (capacity 16):
+5 (8)
 </t>
         </is>
       </c>
       <c r="O33" t="n">
-        <v>270.348945</v>
+        <v>228.8513993000006</v>
       </c>
       <c r="P33" t="n">
-        <v>1024.350870524725</v>
+        <v>1043.169111110342</v>
       </c>
       <c r="Q33" s="4">
         <f>(P33-G33)/G33</f>
@@ -7215,6 +7269,7 @@
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
 9 (14)
+8 metre (capacity 22):
 11 metre (capacity 30):
 6 (14) -&gt; 7 (15)
 2 (5) -&gt; 4 (14) -&gt; 1 (7)
@@ -7223,7 +7278,7 @@
         </is>
       </c>
       <c r="O34" t="n">
-        <v>420.5396387000001</v>
+        <v>281.7760601999998</v>
       </c>
       <c r="P34" t="n">
         <v>883.1390965570637</v>
@@ -7305,7 +7360,7 @@
         </is>
       </c>
       <c r="K35" t="n">
-        <v>931.9144711710784</v>
+        <v>931.8298593139458</v>
       </c>
       <c r="L35" s="4" t="n">
         <v>0.3415304796921158</v>
@@ -7316,7 +7371,8 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
+          <t xml:space="preserve">8 metre (capacity 22):
+Rigid (capacity 16):
 8 (8) -&gt; 3 (8)
 11 metre (capacity 30):
 9 (6) -&gt; 5 (4) -&gt; 6 (5) -&gt; 4 (3) -&gt; 7 (3) -&gt; 2 (2) -&gt; 1 (2)
@@ -7324,7 +7380,7 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>305.8699082000003</v>
+        <v>265.1643839999997</v>
       </c>
       <c r="P35" t="n">
         <v>854.4762539967021</v>
@@ -7418,19 +7474,19 @@
       <c r="N36" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
+11 metre (capacity 30):
 2 (3) -&gt; 7 (1) -&gt; 1 (8) -&gt; 3 (4)
-11 metre (capacity 30):
-5 (12) -&gt; 6 (10)
-8 (10) -&gt; 9 (3) -&gt; 4 (8)
+9 (3) -&gt; 5 (12) -&gt; 6 (10)
 8 metre (capacity 22):
+8 (10) -&gt; 4 (8)
 </t>
         </is>
       </c>
       <c r="O36" t="n">
-        <v>317.1145366</v>
+        <v>255.9975743000005</v>
       </c>
       <c r="P36" t="n">
-        <v>747.3232399828744</v>
+        <v>770.9518224366122</v>
       </c>
       <c r="Q36" s="4">
         <f>(P36-G36)/G36</f>
@@ -7510,7 +7566,7 @@
         </is>
       </c>
       <c r="K37" t="n">
-        <v>1326.10584170281</v>
+        <v>1326.047008496605</v>
       </c>
       <c r="L37" s="4" t="n">
         <v>0.2459067686438042</v>
@@ -7521,20 +7577,20 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 metre (capacity 22):
-2 (9) -&gt; 4 (8) -&gt; 9 (3)
-11 metre (capacity 30):
-7 (16) -&gt; 6 (11)
-3 (10) -&gt; 8 (16)
+          <t xml:space="preserve">11 metre (capacity 30):
+8 (16) -&gt; 3 (10)
 5 (12) -&gt; 1 (12)
+4 (8) -&gt; 9 (3) -&gt; 7 (16)
+8 metre (capacity 22):
+6 (11) -&gt; 2 (9)
 </t>
         </is>
       </c>
       <c r="O37" t="n">
-        <v>388.5819654999996</v>
+        <v>271.5002951999995</v>
       </c>
       <c r="P37" t="n">
-        <v>1401.748026361061</v>
+        <v>1326.047008496605</v>
       </c>
       <c r="Q37" s="4">
         <f>(P37-G37)/G37</f>
@@ -7625,14 +7681,14 @@
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
 11 metre (capacity 30):
+5 (1) -&gt; 2 (1) -&gt; 3 (12) -&gt; 6 (4)
 4 (4) -&gt; 7 (2) -&gt; 9 (7) -&gt; 8 (4) -&gt; 1 (11)
-6 (4) -&gt; 3 (12) -&gt; 2 (1) -&gt; 5 (1)
 8 metre (capacity 22):
 </t>
         </is>
       </c>
       <c r="O38" t="n">
-        <v>262.6094512</v>
+        <v>226.3959122000006</v>
       </c>
       <c r="P38" t="n">
         <v>622.2180764428056</v>
@@ -7726,17 +7782,18 @@
       <c r="N39" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
-3 (3) -&gt; 9 (8) -&gt; 6 (5)
+4 (1) -&gt; 5 (1) -&gt; 1 (2) -&gt; 2 (4) -&gt; 7 (4)
+8 (10) -&gt; 3 (3)
+6 (5) -&gt; 9 (8)
 11 metre (capacity 30):
-7 (4) -&gt; 8 (10) -&gt; 2 (4) -&gt; 1 (2) -&gt; 5 (1) -&gt; 4 (1)
 </t>
         </is>
       </c>
       <c r="O39" t="n">
-        <v>276.8129958999998</v>
+        <v>174.3911535999996</v>
       </c>
       <c r="P39" t="n">
-        <v>987.843110637234</v>
+        <v>1001.185311729765</v>
       </c>
       <c r="Q39" s="4">
         <f>(P39-G39)/G39</f>
@@ -7816,7 +7873,7 @@
         </is>
       </c>
       <c r="K40" t="n">
-        <v>1367.440463239961</v>
+        <v>1367.146728044428</v>
       </c>
       <c r="L40" s="4" t="n">
         <v>0.1881009902756456</v>
@@ -7828,9 +7885,9 @@
       <c r="N40" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
-2 (8) -&gt; 5 (10)
+1 (11) -&gt; 6 (5)
+5 (10) -&gt; 2 (8)
 Rigid (capacity 16):
-1 (11) -&gt; 6 (5)
 8 (7)
 11 metre (capacity 30):
 9 (5) -&gt; 7 (7) -&gt; 4 (12) -&gt; 3 (5)
@@ -7838,10 +7895,10 @@
         </is>
       </c>
       <c r="O40" t="n">
-        <v>292.5233773</v>
+        <v>413.8151592000004</v>
       </c>
       <c r="P40" t="n">
-        <v>1175.414901887981</v>
+        <v>1206.305074600059</v>
       </c>
       <c r="Q40" s="4">
         <f>(P40-G40)/G40</f>
@@ -7932,18 +7989,18 @@
       <c r="N41" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
-3 (12)
+9 (5) -&gt; 4 (4) -&gt; 3 (12)
 11 metre (capacity 30):
-5 (4) -&gt; 6 (13) -&gt; 7 (11)
-2 (14) -&gt; 1 (3) -&gt; 4 (4) -&gt; 9 (5) -&gt; 8 (4)
+1 (3) -&gt; 2 (14) -&gt; 7 (11)
+8 (4) -&gt; 5 (4) -&gt; 6 (13)
 </t>
         </is>
       </c>
       <c r="O41" t="n">
-        <v>293.2506680000006</v>
+        <v>249.4281912000006</v>
       </c>
       <c r="P41" t="n">
-        <v>1171.163514436588</v>
+        <v>1172.748196784024</v>
       </c>
       <c r="Q41" s="4">
         <f>(P41-G41)/G41</f>
@@ -8040,18 +8097,18 @@
       <c r="N42" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-3 (5) -&gt; 10 (2) -&gt; 2 (8) -&gt; 6 (11) -&gt; 8 (4)
+8 (4) -&gt; 6 (11) -&gt; 2 (8) -&gt; 10 (2)
 8 metre (capacity 22):
-12 (12) -&gt; 11 (3) -&gt; 7 (1)
+3 (5) -&gt; 7 (1) -&gt; 11 (3) -&gt; 12 (12)
 9 (7) -&gt; 4 (1) -&gt; 5 (2) -&gt; 1 (11)
 </t>
         </is>
       </c>
       <c r="O42" t="n">
-        <v>401.0180667999999</v>
+        <v>307.8755359999996</v>
       </c>
       <c r="P42" t="n">
-        <v>1149.08514985564</v>
+        <v>1191.432500031729</v>
       </c>
       <c r="Q42" s="4">
         <f>(P42-G42)/G42</f>
@@ -8149,19 +8206,20 @@
       <c r="N43" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
-11 (1) -&gt; 6 (5) -&gt; 5 (8) -&gt; 7 (4) -&gt; 3 (4)
+5 (8)
+7 (4) -&gt; 1 (7) -&gt; 3 (4)
 Rigid (capacity 16):
-9 (8) -&gt; 1 (7) -&gt; 8 (1)
+11 (1) -&gt; 6 (5) -&gt; 8 (1) -&gt; 9 (8)
 11 metre (capacity 30):
 2 (6) -&gt; 10 (10) -&gt; 4 (4) -&gt; 12 (9)
 </t>
         </is>
       </c>
       <c r="O43" t="n">
-        <v>446.5484197000005</v>
+        <v>525.2870451999997</v>
       </c>
       <c r="P43" t="n">
-        <v>1105.841482055037</v>
+        <v>1108.045048051991</v>
       </c>
       <c r="Q43" s="4">
         <f>(P43-G43)/G43</f>
@@ -8258,14 +8316,15 @@
       <c r="N44" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-5 (5) -&gt; 12 (11) -&gt; 7 (2)
+2 (1) -&gt; 6 (8) -&gt; 11 (6) -&gt; 4 (1)
 3 (8) -&gt; 1 (10) -&gt; 8 (3) -&gt; 10 (1) -&gt; 9 (1)
-2 (1) -&gt; 6 (8) -&gt; 11 (6) -&gt; 4 (1)
+7 (2) -&gt; 12 (11) -&gt; 5 (5)
+8 metre (capacity 22):
 </t>
         </is>
       </c>
       <c r="O44" t="n">
-        <v>415.2917458000011</v>
+        <v>265.1971490000005</v>
       </c>
       <c r="P44" t="n">
         <v>977.1735761910081</v>
@@ -8364,19 +8423,20 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 metre (capacity 30):
-11 (9) -&gt; 9 (3) -&gt; 1 (9) -&gt; 2 (7)
-10 (7) -&gt; 8 (10) -&gt; 12 (9) -&gt; 6 (1)
+          <t xml:space="preserve">Rigid (capacity 16):
 8 metre (capacity 22):
 3 (5) -&gt; 5 (4) -&gt; 4 (7) -&gt; 7 (5)
+11 metre (capacity 30):
+6 (1) -&gt; 12 (9) -&gt; 8 (10) -&gt; 10 (7)
+2 (7) -&gt; 1 (9) -&gt; 9 (3) -&gt; 11 (9)
 </t>
         </is>
       </c>
       <c r="O45" t="n">
-        <v>640.1704766000003</v>
+        <v>476.6016035999992</v>
       </c>
       <c r="P45" t="n">
-        <v>1012.611449136445</v>
+        <v>1012.611449136446</v>
       </c>
       <c r="Q45" s="4">
         <f>(P45-G45)/G45</f>
@@ -8475,8 +8535,8 @@
       <c r="N46" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
+7 (2) -&gt; 2 (6) -&gt; 8 (4) -&gt; 3 (6) -&gt; 4 (2)
 9 (4) -&gt; 10 (6)
-4 (2) -&gt; 3 (6) -&gt; 8 (4) -&gt; 2 (6) -&gt; 7 (2)
 11 metre (capacity 30):
 1 (5) -&gt; 6 (6) -&gt; 11 (2) -&gt; 12 (7) -&gt; 5 (10)
 Rigid (capacity 16):
@@ -8484,7 +8544,7 @@
         </is>
       </c>
       <c r="O46" t="n">
-        <v>537.6972268999998</v>
+        <v>349.1707250999989</v>
       </c>
       <c r="P46" t="n">
         <v>1207.078493999617</v>
@@ -8582,19 +8642,19 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
+          <t xml:space="preserve">11 metre (capacity 30):
+5 (9) -&gt; 10 (2) -&gt; 12 (8) -&gt; 2 (9)
+3 (2) -&gt; 9 (1) -&gt; 7 (7) -&gt; 4 (8) -&gt; 6 (1) -&gt; 11 (5) -&gt; 8 (3) -&gt; 1 (2)
 8 metre (capacity 22):
-11 metre (capacity 30):
-9 (1) -&gt; 7 (7) -&gt; 4 (8) -&gt; 6 (1) -&gt; 11 (5) -&gt; 8 (3) -&gt; 1 (2)
-2 (9) -&gt; 12 (8) -&gt; 3 (2) -&gt; 10 (2) -&gt; 5 (9)
+Rigid (capacity 16):
 </t>
         </is>
       </c>
       <c r="O47" t="n">
-        <v>405.3070793000006</v>
+        <v>377.6647546000004</v>
       </c>
       <c r="P47" t="n">
-        <v>799.1406234953578</v>
+        <v>811.6703400824063</v>
       </c>
       <c r="Q47" s="4">
         <f>(P47-G47)/G47</f>
@@ -8690,19 +8750,20 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 metre (capacity 22):
+          <t xml:space="preserve">11 metre (capacity 30):
+10 (6) -&gt; 7 (2) -&gt; 1 (9) -&gt; 12 (3)
+5 (6) -&gt; 11 (3) -&gt; 4 (2) -&gt; 9 (7) -&gt; 8 (10)
+Rigid (capacity 16):
+8 metre (capacity 22):
 6 (4) -&gt; 3 (8) -&gt; 2 (8)
-11 metre (capacity 30):
-5 (6) -&gt; 11 (3) -&gt; 4 (2) -&gt; 9 (7) -&gt; 8 (10)
-10 (6) -&gt; 7 (2) -&gt; 1 (9) -&gt; 12 (3)
 </t>
         </is>
       </c>
       <c r="O48" t="n">
-        <v>679.3504835999993</v>
+        <v>360.9418872999995</v>
       </c>
       <c r="P48" t="n">
-        <v>873.0560538038177</v>
+        <v>873.0560538038178</v>
       </c>
       <c r="Q48" s="4">
         <f>(P48-G48)/G48</f>
@@ -8799,21 +8860,21 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
+          <t xml:space="preserve">8 metre (capacity 22):
+9 (8) -&gt; 4 (5) -&gt; 3 (8)
+Rigid (capacity 16):
 11 (10)
 11 metre (capacity 30):
-5 (8) -&gt; 1 (7) -&gt; 7 (9) -&gt; 8 (6)
-4 (5) -&gt; 9 (8) -&gt; 12 (10)
-8 metre (capacity 22):
-3 (8) -&gt; 10 (8) -&gt; 6 (1) -&gt; 2 (5)
+8 (6) -&gt; 5 (8) -&gt; 6 (1) -&gt; 10 (8) -&gt; 2 (5)
+1 (7) -&gt; 7 (9) -&gt; 12 (10)
 </t>
         </is>
       </c>
       <c r="O49" t="n">
-        <v>449.0606509999998</v>
+        <v>439.4680506999994</v>
       </c>
       <c r="P49" t="n">
-        <v>1289.129827108421</v>
+        <v>1319.92653993926</v>
       </c>
       <c r="Q49" s="4">
         <f>(P49-G49)/G49</f>
@@ -8897,7 +8958,7 @@
         </is>
       </c>
       <c r="K50" t="n">
-        <v>1088.708858004286</v>
+        <v>1088.705961302745</v>
       </c>
       <c r="L50" s="4" t="n">
         <v>0.1356667398854045</v>
@@ -8908,18 +8969,19 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 metre (capacity 30):
-8 (1) -&gt; 2 (6) -&gt; 3 (2) -&gt; 9 (1) -&gt; 6 (4) -&gt; 1 (9) -&gt; 4 (1)
-8 metre (capacity 22):
-5 (4) -&gt; 7 (2) -&gt; 11 (3) -&gt; 12 (2) -&gt; 10 (9)
+          <t xml:space="preserve">8 metre (capacity 22):
+3 (2) -&gt; 9 (1) -&gt; 6 (4) -&gt; 1 (9) -&gt; 4 (1)
+11 metre (capacity 30):
+5 (4) -&gt; 7 (2) -&gt; 11 (3) -&gt; 12 (2) -&gt; 2 (6) -&gt; 10 (9) -&gt; 8 (1)
+Rigid (capacity 16):
 </t>
         </is>
       </c>
       <c r="O50" t="n">
-        <v>400.1393131000004</v>
+        <v>336.4328005000007</v>
       </c>
       <c r="P50" t="n">
-        <v>1132.241078906159</v>
+        <v>1088.705961302745</v>
       </c>
       <c r="Q50" s="4">
         <f>(P50-G50)/G50</f>
@@ -9016,21 +9078,21 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
-7 (4) -&gt; 11 (9) -&gt; 6 (2)
-11 metre (capacity 30):
+          <t xml:space="preserve">11 metre (capacity 30):
 5 (3) -&gt; 10 (9) -&gt; 12 (9) -&gt; 8 (9)
 8 metre (capacity 22):
-4 (10) -&gt; 1 (8) -&gt; 2 (4)
-9 (8) -&gt; 3 (8)
+4 (10) -&gt; 1 (8)
+2 (4) -&gt; 9 (8) -&gt; 3 (8)
+Rigid (capacity 16):
+6 (2) -&gt; 11 (9) -&gt; 7 (4)
 </t>
         </is>
       </c>
       <c r="O51" t="n">
-        <v>462.8972104999993</v>
+        <v>494.9195553999998</v>
       </c>
       <c r="P51" t="n">
-        <v>1230.788478416771</v>
+        <v>1355.94412226609</v>
       </c>
       <c r="Q51" s="4">
         <f>(P51-G51)/G51</f>
@@ -9132,17 +9194,17 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 metre (capacity 30):
-10 (5) -&gt; 9 (5) -&gt; 3 (3) -&gt; 15 (6) -&gt; 11 (1) -&gt; 4 (7) -&gt; 14 (3)
-Rigid (capacity 16):
-8 (5) -&gt; 2 (5) -&gt; 5 (2) -&gt; 1 (3)
+          <t xml:space="preserve">Rigid (capacity 16):
+1 (3) -&gt; 5 (2) -&gt; 2 (5) -&gt; 8 (5)
 8 metre (capacity 22):
 6 (8) -&gt; 7 (2) -&gt; 13 (4) -&gt; 12 (3)
+11 metre (capacity 30):
+14 (3) -&gt; 4 (7) -&gt; 11 (1) -&gt; 15 (6) -&gt; 3 (3) -&gt; 9 (5) -&gt; 10 (5)
 </t>
         </is>
       </c>
       <c r="O52" t="n">
-        <v>641.0992283999985</v>
+        <v>624.6711491000005</v>
       </c>
       <c r="P52" t="n">
         <v>962.3431591979642</v>
@@ -9249,20 +9311,19 @@
       <c r="N53" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
-13 (1) -&gt; 14 (6) -&gt; 6 (3) -&gt; 8 (4) -&gt; 7 (8)
-2 (2) -&gt; 10 (5) -&gt; 11 (3) -&gt; 4 (3) -&gt; 1 (6) -&gt; 12 (2)
+2 (2) -&gt; 3 (7) -&gt; 15 (5)
+10 (5) -&gt; 11 (3) -&gt; 4 (3) -&gt; 1 (6) -&gt; 9 (4)
 Rigid (capacity 16):
-15 (5) -&gt; 3 (7)
 11 metre (capacity 30):
-9 (4) -&gt; 5 (2)
+7 (8) -&gt; 8 (4) -&gt; 6 (3) -&gt; 14 (6) -&gt; 13 (1) -&gt; 12 (2) -&gt; 5 (2)
 </t>
         </is>
       </c>
       <c r="O53" t="n">
-        <v>590.9634501999999</v>
+        <v>507.9009951000007</v>
       </c>
       <c r="P53" t="n">
-        <v>1170.641417405643</v>
+        <v>1243.286364160106</v>
       </c>
       <c r="Q53" s="4">
         <f>(P53-G53)/G53</f>
@@ -9352,7 +9413,7 @@
         </is>
       </c>
       <c r="K54" t="n">
-        <v>975.4626174759479</v>
+        <v>975.462615638453</v>
       </c>
       <c r="L54" s="4" t="n">
         <v>0.1947723838441573</v>
@@ -9363,14 +9424,15 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 metre (capacity 22):
+          <t xml:space="preserve">Rigid (capacity 16):
+8 metre (capacity 22):
+9 (1) -&gt; 10 (2) -&gt; 11 (7) -&gt; 5 (1) -&gt; 13 (2) -&gt; 15 (2) -&gt; 14 (1) -&gt; 4 (2) -&gt; 7 (2)
 12 (6) -&gt; 2 (1) -&gt; 6 (3) -&gt; 3 (2) -&gt; 8 (3) -&gt; 1 (4)
-9 (1) -&gt; 10 (2) -&gt; 11 (7) -&gt; 5 (1) -&gt; 13 (2) -&gt; 15 (2) -&gt; 14 (1) -&gt; 4 (2) -&gt; 7 (2)
 </t>
         </is>
       </c>
       <c r="O54" t="n">
-        <v>589.6376583000019</v>
+        <v>479.1373138999988</v>
       </c>
       <c r="P54" t="n">
         <v>986.5123038407138</v>
@@ -9465,7 +9527,7 @@
         </is>
       </c>
       <c r="K55" t="n">
-        <v>1734.220435826672</v>
+        <v>1734.219878209735</v>
       </c>
       <c r="L55" s="4" t="n">
         <v>0.2983432419886213</v>
@@ -9477,20 +9539,20 @@
       <c r="N55" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-3 (8) -&gt; 11 (9) -&gt; 5 (7)
-13 (8) -&gt; 14 (4) -&gt; 15 (1) -&gt; 8 (1) -&gt; 12 (8) -&gt; 7 (7)
-6 (8) -&gt; 9 (8) -&gt; 10 (6) -&gt; 2 (5)
+14 (4) -&gt; 5 (7) -&gt; 15 (1) -&gt; 8 (1) -&gt; 12 (8) -&gt; 7 (7)
+2 (5) -&gt; 10 (6) -&gt; 9 (8) -&gt; 6 (8)
+13 (8) -&gt; 11 (9) -&gt; 3 (8)
 8 metre (capacity 22):
-4 (6) -&gt; 1 (5)
+1 (5) -&gt; 4 (6)
 Rigid (capacity 16):
 </t>
         </is>
       </c>
       <c r="O55" t="n">
-        <v>729.1322881999999</v>
+        <v>568.3130997999997</v>
       </c>
       <c r="P55" t="n">
-        <v>1479.107828259259</v>
+        <v>1487.738497108275</v>
       </c>
       <c r="Q55" s="4">
         <f>(P55-G55)/G55</f>
@@ -9581,7 +9643,7 @@
         </is>
       </c>
       <c r="K56" t="n">
-        <v>1490.656141002366</v>
+        <v>1490.655680771097</v>
       </c>
       <c r="L56" s="4" t="n">
         <v>0.2064845212800801</v>
@@ -9593,18 +9655,18 @@
       <c r="N56" t="inlineStr">
         <is>
           <t xml:space="preserve">Rigid (capacity 16):
-10 (5) -&gt; 12 (1) -&gt; 9 (6) -&gt; 15 (4)
-2 (1) -&gt; 11 (3) -&gt; 6 (7) -&gt; 5 (1) -&gt; 13 (3)
+3 (1) -&gt; 8 (5) -&gt; 4 (1) -&gt; 7 (3) -&gt; 1 (3)
+13 (3) -&gt; 5 (1) -&gt; 11 (3) -&gt; 6 (7) -&gt; 2 (1)
 11 metre (capacity 30):
-1 (3) -&gt; 7 (3) -&gt; 4 (1) -&gt; 14 (9) -&gt; 8 (5) -&gt; 3 (1)
+10 (5) -&gt; 12 (1) -&gt; 9 (6) -&gt; 15 (4) -&gt; 14 (9)
 </t>
         </is>
       </c>
       <c r="O56" t="n">
-        <v>754.2183009</v>
+        <v>432.1809078999995</v>
       </c>
       <c r="P56" t="n">
-        <v>1454.78404815136</v>
+        <v>1474.954967044446</v>
       </c>
       <c r="Q56" s="4">
         <f>(P56-G56)/G56</f>
@@ -9695,7 +9757,7 @@
         </is>
       </c>
       <c r="K57" t="n">
-        <v>875.6453824270292</v>
+        <v>875.6447806938481</v>
       </c>
       <c r="L57" s="4" t="n">
         <v>0.278597361211454</v>
@@ -9706,19 +9768,21 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rigid (capacity 16):
-5 (6) -&gt; 9 (2) -&gt; 15 (4) -&gt; 7 (2) -&gt; 6 (2)
-3 (6) -&gt; 14 (2) -&gt; 10 (2) -&gt; 13 (5)
-11 metre (capacity 30):
-8 (3) -&gt; 1 (7) -&gt; 11 (3) -&gt; 2 (5) -&gt; 4 (5) -&gt; 12 (7)
+          <t xml:space="preserve">11 metre (capacity 30):
+1 (7) -&gt; 13 (5) -&gt; 7 (2) -&gt; 15 (4) -&gt; 9 (2) -&gt; 5 (6) -&gt; 6 (2)
+8 metre (capacity 22):
+8 (3)
+Rigid (capacity 16):
+3 (6) -&gt; 14 (2) -&gt; 12 (7)
+11 (3) -&gt; 10 (2) -&gt; 2 (5) -&gt; 4 (5)
 </t>
         </is>
       </c>
       <c r="O57" t="n">
-        <v>843.4938672999997</v>
+        <v>857.4403509000003</v>
       </c>
       <c r="P57" t="n">
-        <v>834.377601210616</v>
+        <v>865.0512851856599</v>
       </c>
       <c r="Q57" s="4">
         <f>(P57-G57)/G57</f>
@@ -9809,7 +9873,7 @@
         </is>
       </c>
       <c r="K58" t="n">
-        <v>1287.259466421646</v>
+        <v>1286.194422943748</v>
       </c>
       <c r="L58" s="4" t="n">
         <v>0.2342084988856621</v>
@@ -9822,17 +9886,18 @@
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
 2 (6) -&gt; 8 (3) -&gt; 11 (4) -&gt; 14 (3)
-5 (2) -&gt; 4 (3) -&gt; 10 (4) -&gt; 3 (1) -&gt; 7 (6)
+4 (3) -&gt; 10 (4) -&gt; 3 (1) -&gt; 7 (6)
+Rigid (capacity 16):
 11 metre (capacity 30):
-13 (8) -&gt; 9 (8) -&gt; 12 (1) -&gt; 15 (3) -&gt; 1 (3) -&gt; 6 (4)
+6 (4) -&gt; 1 (3) -&gt; 15 (3) -&gt; 12 (1) -&gt; 9 (8) -&gt; 13 (8) -&gt; 5 (2)
 </t>
         </is>
       </c>
       <c r="O58" t="n">
-        <v>858.8470230000021</v>
+        <v>818.3367384000012</v>
       </c>
       <c r="P58" t="n">
-        <v>1275.382289345094</v>
+        <v>1277.933433799529</v>
       </c>
       <c r="Q58" s="4">
         <f>(P58-G58)/G58</f>
@@ -9937,16 +10002,16 @@
       <c r="N59" t="inlineStr">
         <is>
           <t xml:space="preserve">11 metre (capacity 30):
-6 (5) -&gt; 13 (7) -&gt; 2 (6) -&gt; 3 (8) -&gt; 9 (2)
-7 (8) -&gt; 5 (5) -&gt; 14 (5) -&gt; 8 (9)
+9 (2) -&gt; 3 (8) -&gt; 2 (6) -&gt; 13 (7) -&gt; 6 (5)
+8 (9) -&gt; 14 (5) -&gt; 5 (5) -&gt; 7 (8)
 8 metre (capacity 22):
-11 (1) -&gt; 12 (7) -&gt; 10 (4) -&gt; 15 (3) -&gt; 1 (4)
 4 (9)
+1 (4) -&gt; 15 (3) -&gt; 10 (4) -&gt; 12 (7) -&gt; 11 (1)
 </t>
         </is>
       </c>
       <c r="O59" t="n">
-        <v>815.1835444000001</v>
+        <v>717.4032890000017</v>
       </c>
       <c r="P59" t="n">
         <v>1025.97020552298</v>
@@ -10041,7 +10106,7 @@
         </is>
       </c>
       <c r="K60" t="n">
-        <v>928.1092174359235</v>
+        <v>928.1018042726959</v>
       </c>
       <c r="L60" s="4" t="n">
         <v>0.142310132540058</v>
@@ -10053,18 +10118,19 @@
       <c r="N60" t="inlineStr">
         <is>
           <t xml:space="preserve">8 metre (capacity 22):
+11 (8) -&gt; 6 (4)
 14 (7) -&gt; 9 (5) -&gt; 13 (9)
 11 metre (capacity 30):
-8 (1) -&gt; 15 (6) -&gt; 7 (8) -&gt; 3 (5) -&gt; 2 (6) -&gt; 6 (4)
-12 (6) -&gt; 1 (3) -&gt; 11 (8) -&gt; 5 (2) -&gt; 4 (6) -&gt; 10 (5)
+3 (5) -&gt; 7 (8) -&gt; 15 (6) -&gt; 8 (1)
+12 (6) -&gt; 1 (3) -&gt; 5 (2) -&gt; 4 (6) -&gt; 10 (5) -&gt; 2 (6)
 </t>
         </is>
       </c>
       <c r="O60" t="n">
-        <v>676.0706847999973</v>
+        <v>672.2648152000002</v>
       </c>
       <c r="P60" t="n">
-        <v>948.7054240947547</v>
+        <v>1035.824466025884</v>
       </c>
       <c r="Q60" s="4">
         <f>(P60-G60)/G60</f>
@@ -10169,21 +10235,22 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 metre (capacity 30):
-10 (5) -&gt; 12 (8) -&gt; 6 (6) -&gt; 14 (7) -&gt; 11 (4)
-3 (6) -&gt; 7 (6) -&gt; 1 (5) -&gt; 4 (4) -&gt; 2 (6)
+          <t xml:space="preserve">Rigid (capacity 16):
+15 (6) -&gt; 13 (6)
+10 (5) -&gt; 9 (2) -&gt; 8 (4)
 8 metre (capacity 22):
-Rigid (capacity 16):
-5 (8) -&gt; 8 (4) -&gt; 9 (2)
-15 (6) -&gt; 13 (6)
+2 (6)
+11 metre (capacity 30):
+4 (4) -&gt; 1 (5) -&gt; 7 (6) -&gt; 3 (6) -&gt; 5 (8)
+11 (4) -&gt; 14 (7) -&gt; 6 (6) -&gt; 12 (8)
 </t>
         </is>
       </c>
       <c r="O61" t="n">
-        <v>741.7026270000024</v>
+        <v>714.968768900002</v>
       </c>
       <c r="P61" t="n">
-        <v>1212.417268828427</v>
+        <v>1245.892684760786</v>
       </c>
       <c r="Q61" s="4">
         <f>(P61-G61)/G61</f>
@@ -11045,10 +11112,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -11124,7 +11191,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="16" t="n">
         <v>43745</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -11224,8 +11291,8 @@
         <v/>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="11" t="n">
+    <row r="3" ht="14.25" customHeight="1" s="2">
+      <c r="A3" s="17" t="n">
         <v>43768</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -11236,33 +11303,104 @@
       <c r="C3" t="n">
         <v>592286.4353333331</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>{"0": [[[74, 5], [48, 4], [33, 16], [9, 10], [121, 6], [95, 15], [182, 7], [28, 6], [19, 6], [81, 16], [94, 5], [83, 16], [119, 12], [154, 14], [93, 9], [2, 14], [83, 15], [70, 7], [68, 10], [18, 15], [171, 2], [126, 10], [117, 6], [209, 9], [193, 3], [75, 7], [17, 16], [125, 14], [98, 16], [35, 16], [66, 16], [188, 15]]], "1": [[[144, 3], [4, 19], [55, 22], [39, 1], [134, 10], [88, 22], [101, 10], [25, 22], [37, 10], [186, 15], [34, 16], [104, 22], [57, 15], [62, 1], [123, 2], [151, 15], [176, 16], [15, 22], [72, 22], [8, 0], [139, 15], [15, 0], [159, 22], [152, 4], [135, 5], [33, 22], [8, 0], [38, 22], [96, 16], [198, 7], [174, 5], [40, 22], [194, 22], [41, 22], [40, 22], [187, 8], [194, 16], [40, 1], [104, 14], [196, 13], [207, 20], [153, 22], [108, 9], [33, 17], [131, 12], [199, 10], [91, 13], [81, 22], [168, 8], [156, 12], [72, 8], [200, 15], [1, 4], [192, 21], [191, 2], [157, 22], [97, 0], [46, 15], [4, 0], [110, 19], [3, 0], [163, 17], [157, 2], [153, 22], [82, 22], [159, 2], [3, 0], [53, 13]]], "2": [[[42, 12], [120, 16], [197, 25], [32, 27], [6, 14], [41, 30], [132, 10], [16, 30], [172, 20], [79, 30], [148, 6], [44, 30], [77, 30], [150, 8], [24, 25], [66, 30], [25, 5], [172, 20], [79, 0], [149, 30], [77, 0], [165, 30], [149, 24], [140, 30], [35, 5], [97, 21], [59, 28], [92, 30], [55, 30], [49, 24], [143, 5], [208, 24], [63, 16], [100, 30], [29, 29]]]}</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Rigid (capacity 16):
-74-G (5) -&gt; 48-D (4) -&gt; 33-C (16) -&gt; 9-B (10) -&gt; 121-O (6) -&gt; 95-K (15) -&gt; 182-U (7) -&gt; 28-C (6) -&gt; 19-B (6) -&gt; 81-H (16) -&gt; 94-K (5) -&gt; 83-H (16) -&gt; 119-O (12) -&gt; 154-S (14) -&gt; 93-K (9) -&gt; 2-A (14) -&gt; 83-H (15) -&gt; 70-G (7) -&gt; 68-G (10) -&gt; 18-B (15) -&gt; 171-S (2) -&gt; 126-P (10) -&gt; 117-N (6) -&gt; 209-Z (9) -&gt; 193-V (3) -&gt; 75-H (7) -&gt; 17-B (16) -&gt; 125-P (14) -&gt; 98-L (16) -&gt; 35-C (16) -&gt; 66-G (16) -&gt; 188-V (15)
+      <c r="F3" s="11" t="inlineStr">
+        <is>
+          <t>Rigid (capacity 16):
+199-W (10)
+168-S (8)
+91-K (13)
+156-S (12)
+25-C (16)
+2-A (14)
+39-C (1) -&gt; 188-V (15)
+176-T (16)
+120-O (16)
+63-G (16)
 8 Metre (capacity 22):
-144-Q (3) -&gt; 4-A (19) -&gt; 55-E (22) -&gt; 39-C (1) -&gt; 134-P (10) -&gt; 88-K (22) -&gt; 101-L (10) -&gt; 25-C (22) -&gt; 37-C (10) -&gt; 186-V (15) -&gt; 34-C (16) -&gt; 104-M (22) -&gt; 57-F (15) -&gt; 62-G (1) -&gt; 123-O (2) -&gt; 151-R (15) -&gt; 176-T (16) -&gt; 15-B (22) -&gt; 72-G (22) -&gt; 8-B (0) -&gt; 139-P (15) -&gt; 15-B (0) -&gt; 159-S (22) -&gt; 152-R (4) -&gt; 135-P (5) -&gt; 33-C (22) -&gt; 8-B (0) -&gt; 38-C (22) -&gt; 96-K (16) -&gt; 198-W (7) -&gt; 174-T (5) -&gt; 40-C (22) -&gt; 194-V (22) -&gt; 41-C (22) -&gt; 40-C (22) -&gt; 187-V (8) -&gt; 194-V (16) -&gt; 40-C (1) -&gt; 104-M (14) -&gt; 196-W (13) -&gt; 207-Y (20) -&gt; 153-S (22) -&gt; 108-M (9) -&gt; 33-C (17) -&gt; 131-P (12) -&gt; 199-W (10) -&gt; 91-K (13) -&gt; 81-H (22) -&gt; 168-S (8) -&gt; 156-S (12) -&gt; 72-G (8) -&gt; 200-W (15) -&gt; 1-A (4) -&gt; 192-V (21) -&gt; 191-V (2) -&gt; 157-S (22) -&gt; 97-K (0) -&gt; 46-D (15) -&gt; 4-A (0) -&gt; 110-M (19) -&gt; 3-A (0) -&gt; 163-S (17) -&gt; 157-S (2) -&gt; 153-S (22) -&gt; 82-H (22) -&gt; 159-S (2) -&gt; 3-A (0) -&gt; 53-E (13)
+196-W (13) -&gt; 171-S (2)
+82-H (22)
+172-S (22)
+35-C (22)
+131-P (12)
+25-C (22)
+35-C (13) -&gt; 48-D (4)
+33-C (22)
+34-C (16)
+83-H (22)
+132-P (10) -&gt; 198-W (7)
+33-C (17)
+152-R (4) -&gt; 98-L (16)
+207-Y (20)
+77-H (22) -&gt; 79-H (22) -&gt; 148-R (6)
+150-R (8)
 11 Metre (capacity 30):
-42-C (12) -&gt; 120-O (16) -&gt; 197-W (25) -&gt; 32-C (27) -&gt; 6-B (14) -&gt; 41-C (30) -&gt; 132-P (10) -&gt; 16-B (30) -&gt; 172-S (20) -&gt; 79-H (30) -&gt; 148-R (6) -&gt; 44-D (30) -&gt; 77-H (30) -&gt; 150-R (8) -&gt; 24-B (25) -&gt; 66-G (30) -&gt; 25-C (5) -&gt; 172-S (20) -&gt; 79-H (0) -&gt; 149-R (30) -&gt; 77-H (0) -&gt; 165-S (30) -&gt; 149-R (24) -&gt; 140-P (30) -&gt; 35-C (5) -&gt; 97-K (21) -&gt; 59-G (28) -&gt; 92-K (30) -&gt; 55-E (30) -&gt; 49-D (24) -&gt; 143-P (5) -&gt; 208-Z (24) -&gt; 63-G (16) -&gt; 100-L (30) -&gt; 29-C (29)
-</t>
+29-C (29)
+1-A (4) -&gt; 68-G (10)
+135-P (5) -&gt; 88-K (22)
+97-K (30)
+55-E (30)
+157-S (24) -&gt; 193-V (3)
+81-H (2) -&gt; 38-C (22)
+97-K (7) -&gt; 101-L (10)
+46-D (15) -&gt; 126-P (10)
+209-Z (9) -&gt; 117-N (6) -&gt; 125-P (14)
+194-V (30)
+28-C (6) -&gt; 49-D (24)
+77-H (30)
+151-R (15) -&gt; 186-V (15)
+59-G (28)
+16-B (30)
+149-R (30)
+72-G (30)
+208-Z (24)
+81-H (30)
+194-V (8) -&gt; 187-V (8) -&gt; 6-B (14)
+153-S (30)
+143-P (5) -&gt; 75-H (7) -&gt; 17-B (16)
+8-B (30)
+53-E (13) -&gt; 134-P (10)
+32-C (27)
+100-L (30)
+110-M (19) -&gt; 104-M (6)
+95-K (15) -&gt; 182-U (7)
+108-M (9) -&gt; 154-S (14) -&gt; 70-G (7)
+140-P (30)
+96-K (16) -&gt; 42-C (12)
+4-A (30)
+93-K (9) -&gt; 192-V (21)
+92-K (30)
+8-B (4) -&gt; 9-B (10) -&gt; 121-O (6) -&gt; 19-B (6)
+66-G (30)
+200-W (15) -&gt; 18-B (15)
+149-R (24) -&gt; 144-Q (3)
+172-S (30)
+174-T (5) -&gt; 139-P (15) -&gt; 41-C (6)
+57-F (15) -&gt; 94-K (5) -&gt; 62-G (1) -&gt; 123-O (2)
+15-B (28)
+104-M (30)
+40-C (30)
+3-A (27)
+83-H (9) -&gt; 119-O (12)
+79-H (30)
+197-W (25) -&gt; 191-V (2)
+163-S (17) -&gt; 4-A (11)
+37-C (10) -&gt; 74-G (5)
+41-C (30)
+159-S (24)
+24-B (25) -&gt; 66-G (4)
+44-D (30)
+165-S (30)
+40-C (15) -&gt; 153-S (14)</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>3601.575652</v>
+        <v>3600.6243162</v>
       </c>
       <c r="H3" t="n">
-        <v>266390.1040000001</v>
-      </c>
-      <c r="I3" t="n">
-        <v>72648.50251580951</v>
+        <v>609208.492333333</v>
       </c>
       <c r="J3">
-        <f>C3-(H3+I3*10)</f>
+        <f>C3-H3</f>
         <v/>
       </c>
       <c r="K3" s="4">
@@ -11271,11 +11409,648 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="n">
+      <c r="A4" s="15" t="n">
         <v>43775</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>{"0": [[[108, 14]], [[56, 9], [118, 7]], [[105, 7], [199, 9]], [[9, 5], [196, 10], [74, 1]], [[192, 16]], [[154, 16]], [[63, 16]], [[48, 13]], [[70, 14], [192, 2]], [[197, 13]], [[37, 1]], [[34, 15]], [[186, 16]], [[93, 10]], [[38, 14], [178, 2]], [[37, 1]], [[4, 10], [53, 6]], [[131, 13]], [[16, 6], [149, 8]], [[207, 16]], [[120, 16]], [[12, 7], [198, 6]], [[151, 1], [12, 7]], [[184, 16]], [[9, 13]], [[166, 10], [101, 2]], [[168, 8], [7, 4], [115, 4]], [[186, 14]], [[37, 2], [81, 1], [91, 13]], [[95, 16]], [[83, 16]], [[75, 9], [135, 6]], [[188, 12], [39, 1]], [[101, 7], [19, 6], [143, 1], [193, 2]], [[46, 16]]], "2": [[[123, 27], [151, 1]], [[55, 30]], [[81, 30]], [[151, 27]], [[44, 30]], [[77, 21], [44, 6]], [[194, 30]], [[159, 24], [6, 1], [187, 2], [194, 3]], [[100, 30]], [[110, 21], [17, 8], [164, 1]], [[68, 15], [200, 10], [72, 5]], [[72, 30]], [[149, 29], [148, 1]], [[165, 27]], [[15, 30]], [[35, 30]], [[41, 30]], [[172, 28]], [[79, 30]], [[208, 30]], [[40, 29], [41, 1]], [[117, 5], [126, 12], [125, 13]], [[119, 14], [2, 13]], [[19, 10], [28, 20]], [[110, 2], [15, 28]], [[91, 30]], [[32, 30]], [[151, 30]], [[28, 3], [182, 15], [95, 9]]], "1": [[[132, 20]], [[33, 22]], [[8, 20], [33, 2]], [[104, 11], [174, 11]], [[176, 17], [35, 5]], [[153, 12], [82, 1], [100, 9]], [[25, 20], [52, 2]], [[144, 20]], [[139, 20]], [[130, 22]], [[83, 22]], [[59, 22]], [[62, 22]], [[96, 17], [184, 2], [74, 2]], [[152, 22]], [[29, 18], [154, 4]], [[208, 22]], [[97, 21], [4, 1]], [[57, 21]], [[185, 2], [3, 9], [88, 6], [208, 3]], [[178, 21], [115, 1]], [[193, 9], [143, 3], [121, 10]], [[121, 4], [163, 12], [51, 1], [135, 4]], [[66, 22]]]}</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>471229.1394000001</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>{"0": [[[208, 3], [17, 8]], [[6, 1], [41, 15]], [[96, 16]], [[19, 16]], [[149, 16]], [[34, 15]], [[207, 16]], [[81, 16]], [[83, 16]], [[166, 10], [74, 3]], [[72, 16]], [[82, 1], [194, 11], [187, 2]], [[41, 16]], [[12, 14]], [[48, 13]], [[53, 6], [196, 10]], [[163, 12]], [[105, 7]], [[108, 14]], [[200, 10]], [[120, 16]]], "1": [[[66, 22]], [[25, 20]], [[57, 21]], [[39, 1], [188, 12], [168, 8]], [[153, 12], [100, 9], [96, 1]], [[149, 21]], [[139, 20]], [[97, 21]], [[154, 20]], [[152, 22]], [[192, 18]], [[83, 22]], [[62, 22]], [[208, 22]], [[101, 9], [56, 9]], [[184, 18]], [[104, 11], [174, 11]], [[194, 22]]], "2": [[[117, 5], [118, 7], [135, 10], [198, 6]], [[100, 30]], [[35, 5], [144, 20]], [[9, 18], [4, 11]], [[55, 30]], [[208, 30]], [[165, 27]], [[159, 24]], [[178, 23], [7, 4]], [[72, 19]], [[130, 22], [173, 1]], [[79, 30]], [[15, 28]], [[151, 29]], [[88, 6], [75, 9], [193, 11]], [[93, 10], [29, 18]], [[95, 25], [143, 4]], [[91, 30]], [[38, 14], [46, 16]], [[18, 23]], [[164, 1], [115, 5], [132, 20]], [[44, 6], [77, 21], [148, 1]], [[37, 4], [185, 2], [110, 23]], [[151, 30]], [[44, 30]], [[70, 14], [68, 15]], [[16, 6], [52, 2], [59, 22]], [[32, 30]], [[33, 24]], [[8, 20]], [[81, 15], [91, 13]], [[186, 30]], [[35, 30]], [[197, 13], [125, 13]], [[176, 17], [126, 12]], [[123, 27]], [[15, 30]], [[172, 28]], [[28, 23]], [[182, 15], [199, 9]], [[119, 14], [2, 13]], [[40, 29]], [[51, 1], [3, 9], [121, 14]], [[63, 16], [131, 13]]]}</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rigid (capacity 16):
+208-Z (3) -&gt; 17-B (8)
+6-B (1) -&gt; 41-C (15)
+96-K (16)
+19-B (16)
+149-R (16)
+34-C (15)
+207-Y (16)
+81-H (16)
+83-H (16)
+166-S (10) -&gt; 74-G (3)
+72-G (16)
+82-H (1) -&gt; 194-V (11) -&gt; 187-V (2)
+41-C (16)
+12-B (14)
+48-D (13)
+53-E (6) -&gt; 196-W (10)
+163-S (12)
+105-M (7)
+108-M (14)
+200-W (10)
+120-O (16)
+8 Metre (capacity 22):
+66-G (22)
+25-C (20)
+57-F (21)
+39-C (1) -&gt; 188-V (12) -&gt; 168-S (8)
+153-S (12) -&gt; 100-L (9) -&gt; 96-K (1)
+149-R (21)
+139-P (20)
+97-K (21)
+154-S (20)
+152-R (22)
+192-V (18)
+83-H (22)
+62-G (22)
+208-Z (22)
+101-L (9) -&gt; 56-F (9)
+184-V (18)
+104-M (11) -&gt; 174-T (11)
+194-V (22)
+11 Metre (capacity 30):
+117-N (5) -&gt; 118-N (7) -&gt; 135-P (10) -&gt; 198-W (6)
+100-L (30)
+35-C (5) -&gt; 144-Q (20)
+9-B (18) -&gt; 4-A (11)
+55-E (30)
+208-Z (30)
+165-S (27)
+159-S (24)
+178-T (23) -&gt; 7-B (4)
+72-G (19)
+130-P (22) -&gt; 173-T (1)
+79-H (30)
+15-B (28)
+151-R (29)
+88-K (6) -&gt; 75-H (9) -&gt; 193-V (11)
+93-K (10) -&gt; 29-C (18)
+95-K (25) -&gt; 143-P (4)
+91-K (30)
+38-C (14) -&gt; 46-D (16)
+18-B (23)
+164-S (1) -&gt; 115-N (5) -&gt; 132-P (20)
+44-D (6) -&gt; 77-H (21) -&gt; 148-R (1)
+37-C (4) -&gt; 185-V (2) -&gt; 110-M (23)
+151-R (30)
+44-D (30)
+70-G (14) -&gt; 68-G (15)
+16-B (6) -&gt; 52-E (2) -&gt; 59-G (22)
+32-C (30)
+33-C (24)
+8-B (20)
+81-H (15) -&gt; 91-K (13)
+186-V (30)
+35-C (30)
+197-W (13) -&gt; 125-P (13)
+176-T (17) -&gt; 126-P (12)
+123-O (27)
+15-B (30)
+172-S (28)
+28-C (23)
+182-U (15) -&gt; 199-W (9)
+119-O (14) -&gt; 2-A (13)
+40-C (29)
+51-D (1) -&gt; 3-A (9) -&gt; 121-O (14)
+63-G (16) -&gt; 131-P (13)
+</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>3893.4923676</v>
+      </c>
+      <c r="H4" t="n">
+        <v>468885.1420666666</v>
+      </c>
+      <c r="J4">
+        <f>C4-(H4+I4*10)</f>
+        <v/>
+      </c>
+      <c r="K4" s="4">
+        <f>J4/C4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="15" t="n">
+        <v>43775</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>{"1": [[[123, 21]], [[192, 20]], [[196, 20]], [[38, 22]], [[91, 22]], [[63, 22]], [[93, 15]], [[97, 22]], [[207, 20]], [[159, 20], [153, 2]], [[40, 11], [41, 9]], [[156, 6], [168, 10], [132, 6]], [[157, 12], [152, 8], [4, 2]], [[121, 6], [143, 7], [193, 3], [19, 6]], [[66, 22]], [[163, 16], [3, 4]], [[189, 22]], [[140, 20]], [[17, 19], [164, 2]], [[49, 14], [197, 7]], [[8, 15], [208, 6]], [[81, 7], [91, 15]], [[15, 22]], [[59, 21], [161, 1]], [[93, 14]], [[97, 22]], [[207, 20]], [[159, 20], [153, 2]], [[40, 11], [41, 9]], [[156, 6], [168, 10], [132, 6]], [[157, 12], [152, 8], [4, 2]], [[121, 6], [143, 7], [193, 3], [19, 6]], [[66, 22]], [[163, 16], [3, 4]], [[189, 22]], [[140, 20]], [[17, 19], [164, 2]], [[49, 14], [197, 7]], [[8, 15], [208, 6]], [[81, 7], [91, 15]], [[15, 22]], [[59, 21], [161, 1]]], "0": [[[70, 12]], [[199, 11], [74, 1]], [[34, 15]], [[9, 7], [48, 6], [181, 3]], [[154, 16]], [[81, 13], [8, 3]], [[108, 10], [120, 5]], [[131, 12], [151, 4]], [[53, 16]], [[197, 16]], [[166, 6], [66, 10]], [[83, 16]], [[3, 16]], [[75, 5]], [[24, 15]], [[83, 14]], [[120, 9], [198, 6]], [[28, 5], [135, 11]], [[149, 12], [111, 2]], [[68, 6], [1, 6], [112, 4]], [[46, 16]], [[151, 11], [186, 2]], [[7, 8], [39, 3]], [[62, 1], [57, 13]], [[47, 9], [166, 7]], [[158, 5], [137, 8]], [[134, 15], [171, 1]], [[92, 16]], [[158, 5], [137, 8]], [[131, 12], [151, 4]], [[53, 16]], [[197, 16]], [[166, 6], [66, 10]], [[83, 16]], [[3, 16]], [[75, 5]], [[24, 15]], [[83, 14]], [[120, 9], [198, 6]], [[28, 5], [135, 11]], [[149, 12], [111, 2]], [[68, 6], [1, 6], [112, 4]], [[46, 16]], [[151, 11], [186, 2]], [[7, 8], [39, 3]], [[62, 1], [57, 13]], [[47, 9], [166, 7]], [[158, 5], [137, 8]], [[134, 15], [171, 1]], [[92, 16]]], "2": [[[33, 30]], [[8, 30]], [[186, 8], [95, 22]], [[37, 28]], [[193, 4], [143, 5], [19, 9], [101, 5], [121, 5]], [[149, 28], [148, 2]], [[165, 27], [79, 3]], [[172, 30]], [[41, 30]], [[208, 30]], [[117, 7], [126, 9], [125, 11]], [[44, 25], [77, 5]], [[77, 30]], [[6, 16], [187, 10], [194, 4]], [[150, 14], [172, 16]], [[194, 30]], [[153, 30]], [[104, 22], [174, 6]], [[100, 30]], [[110, 22], [209, 7]], [[16, 30]], [[82, 27]], [[72, 30]], [[18, 16], [200, 14]], [[182, 16], [95, 7], [101, 7]], [[138, 1], [137, 29]], [], [[31, 28]], [[176, 21], [35, 6]], [[29, 28]], [[35, 30]], [[79, 30]], [[25, 27]], [[119, 13], [2, 15]], [], [[37, 28]], [[193, 4], [143, 5], [19, 9], [101, 5], [121, 5]], [[149, 28], [148, 2]], [[165, 27], [79, 3]], [[172, 30]], [[41, 30]], [[208, 30]], [[117, 7], [126, 9], [125, 11]], [[44, 25], [77, 5]], [[77, 30]], [[6, 16], [187, 10], [194, 4]], [[150, 14], [172, 16]], [[194, 30]], [[153, 30]], [[104, 22], [174, 6]], [[100, 30]], [[110, 22], [209, 7]], [[16, 30]], [[82, 27]], [[72, 30]], [[18, 16], [200, 14]], [[182, 16], [95, 7], [101, 7]], [[138, 1], [137, 29]], [], [[31, 28]], [[176, 21], [35, 6]], [[29, 28]], [[35, 30]], [[79, 30]], [[25, 27]], [[119, 13], [2, 15]], []], "3": [[[55, 36]], [[40, 38]], [[40, 38]]]}</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1428685.831666667</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>{"0": [[[1, 12]], [[59, 2], [161, 2], [148, 4], [150, 6]], [[70, 12]]], "1": [[[149, 22]], [[172, 22]], [[126, 18]], [[29, 16]], [[150, 22]], [[31, 16], [189, 4]], [[91, 22]], [[137, 22]], [[62, 2], [192, 20]], [[196, 20]], [[164, 4], [132, 12]]], "2": [[[7, 16]], [[37, 30]], [[72, 30]], [[143, 24]], [[193, 14]], [[149, 30]], [[19, 30]], [[152, 16], [108, 10]], [[208, 30]], [[49, 28]], [[149, 28]], [[172, 30]], [[123, 21]], [[198, 12], [112, 8]], [[15, 4], [187, 20]], [[137, 30]], [[158, 20]], [[16, 30]], [[200, 28]], [[16, 30]], [[24, 30]], [[33, 30]], [[37, 26]], [[91, 30]], [[25, 24]], [[81, 27]], [[57, 26]], [[119, 26]], [[83, 30]], [[8, 23]], [[9, 7], [97, 4], [174, 12]], [[40, 30]], [[72, 30]], [[120, 23]], [[63, 22]], [[154, 16], [68, 12]], [[104, 30]], [[39, 6], [168, 20]], [[66, 30]], [[165, 30]], [[153, 30]], [[131, 24]], [[172, 30]], [[166, 26]], [[93, 29]], [[25, 30]], [[151, 30]], [[79, 30]], [[28, 10]]], "3": [[[82, 40]], [[47, 18], [82, 14]], [[176, 40]], [[35, 40]], [[41, 40]], [[186, 12], [40, 28]], [[181, 3], [135, 22]], [[100, 20], [34, 15]], [[77, 40]], [[8, 40]], [[3, 40]], [[55, 36]], [[110, 4], [194, 28], [176, 2]], [[182, 32]], [[208, 40]], [[38, 22]], [[79, 36]], [[83, 30]], [[44, 40]], [[15, 40]], [[199, 11]], [[29, 40]], [[40, 40]], [[46, 32]], [[197, 6], [209, 14]], [[95, 36]], [[101, 24], [156, 12]], [[208, 2], [17, 38]], [[189, 40]], [[100, 40]], [[6, 32], [48, 6]], [[140, 40]], [[165, 24], [111, 4], [172, 10]], [[59, 40]], [[2, 30]], [[197, 40]], [[77, 30], [44, 10]], [[31, 40]], [[41, 38]], [[159, 40]], [[137, 38], [138, 2]], [[125, 22], [117, 14], [74, 1]], [[53, 32]], [[207, 40]], [[35, 32]], [[18, 32]], [[121, 22], [75, 10]], [[97, 40]], [[92, 32]], [[153, 34]], [[66, 34]], [[134, 30], [171, 2]], [[194, 40]], [[110, 40]], [[163, 32], [4, 4]], [[157, 24], [104, 14]]]}</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rigid (capacity 16):
+1-A (12)
+59-G (2) -&gt; 161-S (2) -&gt; 148-R (4) -&gt; 150-R (6)
+70-G (12)
+8 Metre (capacity 22):
+149-R (22)
+172-S (22)
+126-P (18)
+29-C (16)
+150-R (22)
+31-C (16) -&gt; 189-V (4)
+91-K (22)
+137-P (22)
+62-G (2) -&gt; 192-V (20)
+196-W (20)
+164-S (4) -&gt; 132-P (12)
+11 Metre (capacity 30):
+7-B (16)
+37-C (30)
+72-G (30)
+143-P (24)
+193-V (14)
+149-R (30)
+19-B (30)
+152-R (16) -&gt; 108-M (10)
+208-Z (30)
+49-D (28)
+149-R (28)
+172-S (30)
+123-O (21)
+198-W (12) -&gt; 112-M (8)
+15-B (4) -&gt; 187-V (20)
+137-P (30)
+158-S (20)
+16-B (30)
+200-W (28)
+16-B (30)
+24-B (30)
+33-C (30)
+37-C (26)
+91-K (30)
+25-C (24)
+81-H (27)
+57-F (26)
+119-O (26)
+83-H (30)
+8-B (23)
+9-B (7) -&gt; 97-K (4) -&gt; 174-T (12)
+40-C (30)
+72-G (30)
+120-O (23)
+63-G (22)
+154-S (16) -&gt; 68-G (12)
+104-M (30)
+39-C (6) -&gt; 168-S (20)
+66-G (30)
+165-S (30)
+153-S (30)
+131-P (24)
+172-S (30)
+166-S (26)
+93-K (29)
+25-C (30)
+151-R (30)
+79-H (30)
+28-C (10)
+Link (capacity 40):
+82-H (40)
+47-D (18) -&gt; 82-H (14)
+176-T (40)
+35-C (40)
+41-C (40)
+186-V (12) -&gt; 40-C (28)
+181-T (3) -&gt; 135-P (22)
+100-L (20) -&gt; 34-C (15)
+77-H (40)
+8-B (40)
+3-A (40)
+55-E (36)
+110-M (4) -&gt; 194-V (28) -&gt; 176-T (2)
+182-U (32)
+208-Z (40)
+38-C (22)
+79-H (36)
+83-H (30)
+44-D (40)
+15-B (40)
+199-W (11)
+29-C (40)
+40-C (40)
+46-D (32)
+197-W (6) -&gt; 209-Z (14)
+95-K (36)
+101-L (24) -&gt; 156-S (12)
+208-Z (2) -&gt; 17-B (38)
+189-V (40)
+100-L (40)
+6-B (32) -&gt; 48-D (6)
+140-P (40)
+165-S (24) -&gt; 111-M (4) -&gt; 172-S (10)
+59-G (40)
+2-A (30)
+197-W (40)
+77-H (30) -&gt; 44-D (10)
+31-C (40)
+41-C (38)
+159-S (40)
+137-P (38) -&gt; 138-P (2)
+125-P (22) -&gt; 117-N (14) -&gt; 74-G (1)
+53-E (32)
+207-Y (40)
+35-C (32)
+18-B (32)
+121-O (22) -&gt; 75-H (10)
+97-K (40)
+92-K (32)
+153-S (34)
+66-G (34)
+134-P (30) -&gt; 171-S (2)
+194-V (40)
+110-M (40)
+163-S (32) -&gt; 4-A (4)
+157-S (24) -&gt; 104-M (14)
+</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>3661.454996</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1267130.2462</v>
+      </c>
+      <c r="J5">
+        <f>C5-(H5+I5*10)</f>
+        <v/>
+      </c>
+      <c r="K5" s="4">
+        <f>J5/C5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="17" t="n">
+        <v>43768</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>{"0": [[[37, 10], [123, 1]], [[9, 10], [48, 4]], [[196, 13], [157, 3]], [[154, 14]], [[144, 3], [49, 3]], [[34, 16]], [[63, 16]], [[108, 9], [120, 7]], [[199, 10], [74, 5]], [[93, 9], [70, 7]], [[186, 14], [151, 1]], [[91, 13], [81, 2]], [[53, 13], [95, 3]], [[197, 16]], [[131, 12], [8, 4]], [[66, 12]], [[83, 13]], [[79, 7], [77, 7]], [[120, 9], [198, 7]], [[96, 16]], [[46, 15]], [[188, 15], [39, 1]], [[151, 14], [123, 1]], [[17, 16]], [[42, 12]], [[134, 10], [171, 2]], [[62, 1], [57, 15]], [[191, 2], [94, 5]]], "1": [[[192, 21]], [[38, 22]], [[33, 9], [4, 11]], [[88, 22]], [[82, 22]], [[68, 10], [1, 4], [18, 8]], [[207, 20]], [[83, 18], [2, 4]], [[119, 12], [2, 10]], [[18, 7], [200, 15]], [[3, 22]], [[157, 21]], [[163, 17], [3, 5]], [[66, 22]]], "2": [[[33, 30]], [[4, 30]], [[32, 27]], [[81, 30]], [[8, 30]], [[55, 30]], [[44, 30]], [[77, 30]], [[159, 24], [41, 6]], [[150, 8], [172, 20]], [[98, 16], [153, 14]], [[149, 24], [148, 6]], [[149, 30]], [[165, 30]], [[172, 30]], [[15, 28]], [[6, 14], [187, 8], [194, 8]], [[176, 16], [35, 5], [209, 9]], [[153, 30]], [[104, 30]], [[100, 30]], [[110, 19], [174, 5], [104, 6]], [[16, 30]], [[156, 12], [168, 8], [132, 10]], [[72, 30]], [[29, 29]], [[35, 30]], [[41, 30]], [[194, 30]], [[79, 30]], [[208, 24], [152, 4]], [[24, 25], [25, 5]], [[25, 30]], [[117, 6], [126, 10], [125, 14]], [[40, 30]], [[59, 28]], [[92, 30]], [[139, 15], [40, 15]], [[121, 6], [143, 5], [193, 3], [19, 6], [97, 10]], [[97, 27]], [[186, 1], [95, 12], [182, 7], [101, 10]], [[49, 21], [197, 9]], [[140, 30]]]}</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>592286.4353333331</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>{"0": [[[66, 16]], [[79, 16]], [[96, 16]], [[66, 16]], [[40, 15]], [[144, 3], [117, 6], [174, 5]], [[131, 12]], [[151, 15]]], "1": [[[207, 20], [123, 2]], [[150, 8], [148, 6], [66, 2]], [[38, 22]], [[4, 11], [48, 4]]], "2": [[[208, 24]], [[4, 30]], [[165, 30]], [[81, 30]], [[104, 30]], [[53, 13], [63, 16]], [[32, 27]], [[140, 30]], [[149, 30]], [[70, 7], [154, 14], [1, 4]], [[3, 27], [193, 3]], [[24, 25], [74, 5]], [[97, 30]], [[44, 30]], [[6, 14], [139, 15]], [[121, 6], [163, 17], [182, 7]], [[15, 28]], [[16, 30]], [[92, 30]], [[100, 30]], [[77, 30]], [[59, 28]], [[104, 6], [176, 16]], [[25, 30]], [[101, 10], [9, 10], [33, 9]], [[194, 8], [187, 8], [41, 6]], [[197, 25]], [[72, 30]], [[125, 14], [126, 10]], [[134, 10], [42, 12]], [[88, 22], [75, 7]], [[188, 15], [39, 1], [132, 10]], [[17, 16], [143, 5], [19, 6]], [[81, 2], [91, 13], [199, 10]], [[186, 15]], [[152, 4], [108, 9], [18, 15]], [[2, 14], [119, 12], [83, 1]], [[49, 24]], [[172, 20], [25, 5]], [[168, 8], [120, 16]], [[200, 15], [37, 10]], [[156, 12], [46, 15]], [[29, 29]], [[83, 30]], [[57, 15], [94, 5], [62, 1]], [[82, 22]], [[34, 16], [171, 2]], [[97, 7], [28, 6], [95, 15]], [[192, 21], [198, 7]], [[55, 30]], [[153, 14], [98, 16]], [[77, 7], [79, 21]], [[33, 30]], [[35, 30]], [[209, 9], [196, 13]], [[35, 5], [149, 24]], [[172, 30]], [[110, 19]], [[153, 30]], [[41, 30]], [[194, 30]], [[159, 24], [135, 5]], [[8, 4], [157, 24], [191, 2]], [[8, 30]], [[68, 10], [93, 9]], [[40, 30]]]}</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rigid (capacity 16):
+66-G (16)
+79-H (16)
+96-K (16)
+66-G (16)
+40-C (15)
+144-Q (3) -&gt; 117-N (6) -&gt; 174-T (5)
+131-P (12)
+151-R (15)
+8 Metre (capacity 22):
+207-Y (20) -&gt; 123-O (2)
+150-R (8) -&gt; 148-R (6) -&gt; 66-G (2)
+38-C (22)
+4-A (11) -&gt; 48-D (4)
+11 Metre (capacity 30):
+208-Z (24)
+4-A (30)
+165-S (30)
+81-H (30)
+104-M (30)
+53-E (13) -&gt; 63-G (16)
+32-C (27)
+140-P (30)
+149-R (30)
+70-G (7) -&gt; 154-S (14) -&gt; 1-A (4)
+3-A (27) -&gt; 193-V (3)
+24-B (25) -&gt; 74-G (5)
+97-K (30)
+44-D (30)
+6-B (14) -&gt; 139-P (15)
+121-O (6) -&gt; 163-S (17) -&gt; 182-U (7)
+15-B (28)
+16-B (30)
+92-K (30)
+100-L (30)
+77-H (30)
+59-G (28)
+104-M (6) -&gt; 176-T (16)
+25-C (30)
+101-L (10) -&gt; 9-B (10) -&gt; 33-C (9)
+194-V (8) -&gt; 187-V (8) -&gt; 41-C (6)
+197-W (25)
+72-G (30)
+125-P (14) -&gt; 126-P (10)
+134-P (10) -&gt; 42-C (12)
+88-K (22) -&gt; 75-H (7)
+188-V (15) -&gt; 39-C (1) -&gt; 132-P (10)
+17-B (16) -&gt; 143-P (5) -&gt; 19-B (6)
+81-H (2) -&gt; 91-K (13) -&gt; 199-W (10)
+186-V (15)
+152-R (4) -&gt; 108-M (9) -&gt; 18-B (15)
+2-A (14) -&gt; 119-O (12) -&gt; 83-H (1)
+49-D (24)
+172-S (20) -&gt; 25-C (5)
+168-S (8) -&gt; 120-O (16)
+200-W (15) -&gt; 37-C (10)
+156-S (12) -&gt; 46-D (15)
+29-C (29)
+83-H (30)
+57-F (15) -&gt; 94-K (5) -&gt; 62-G (1)
+82-H (22)
+34-C (16) -&gt; 171-S (2)
+97-K (7) -&gt; 28-C (6) -&gt; 95-K (15)
+192-V (21) -&gt; 198-W (7)
+55-E (30)
+153-S (14) -&gt; 98-L (16)
+77-H (7) -&gt; 79-H (21)
+33-C (30)
+35-C (30)
+209-Z (9) -&gt; 196-W (13)
+35-C (5) -&gt; 149-R (24)
+172-S (30)
+110-M (19)
+153-S (30)
+41-C (30)
+194-V (30)
+159-S (24) -&gt; 135-P (5)
+8-B (4) -&gt; 157-S (24) -&gt; 191-V (2)
+8-B (30)
+68-G (10) -&gt; 93-K (9)
+40-C (30)
+</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>3786.4904318</v>
+      </c>
+      <c r="H6" t="n">
+        <v>611931.9450000001</v>
+      </c>
+      <c r="J6">
+        <f>C6-(H6+I6*10)</f>
+        <v/>
+      </c>
+      <c r="K6" s="4">
+        <f>J6/C6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="16" t="n">
+        <v>43745</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>{"2": [[[17, 24], [164, 4]], [[44, 30]], [[111, 3], [77, 27]], [[149, 28], [148, 2]], [[165, 30]], [[159, 19], [194, 11]], [[41, 30]], [[172, 30]], [[79, 30]], [[104, 30]], [[6, 23], [187, 7]], [[176, 30]], [[153, 30]], [[208, 30]], [[35, 30]], [[100, 30]], [[83, 20]], [[40, 30]], [[117, 7], [126, 14], [125, 9]], [[121, 12], [143, 11], [193, 7]], [[80, 20], [168, 9]], [[135, 5], [182, 15], [95, 10]], [[81, 30]], [[193, 12], [143, 18]], [[121, 19], [135, 10]]], "1": [[[75, 18]], [[149, 22]], [[24, 8], [25, 14]], [[207, 21]], [[72, 22]], [[119, 10], [2, 12]], [[157, 22]], [[46, 20]], [[188, 22]], [[186, 9], [53, 12]], [[130, 22]], [[83, 20]], [[116, 10], [177, 11], [203, 1]], [[27, 22]]], "0": [[[194, 16]], [[16, 10], [165, 4]], [[156, 16]], [[77, 11]], [[120, 11], [198, 5]], [[151, 16]], [[196, 8], [48, 5]], [[34, 14]], [[9, 15]], [[154, 13]], [[8, 16]], [[108, 11]], [[152, 15]], [[120, 12]], [[199, 1], [91, 6], [81, 6]], [[197, 14]], [[131, 16]], [[151, 9], [173, 7]], [[144, 12]], [[166, 6], [28, 2], [3, 8]], [[97, 13]], [[66, 15]]]}</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>469154.8897999998</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>{"0": [[]], "1": [[]], "2": [[[97, 13], [9, 15]], [[100, 30]], [[198, 5], [120, 23]], [[35, 30]], [[153, 30]], [[194, 27]], [[116, 10], [203, 1], [177, 11]], [[165, 30]], [[6, 23]], [[53, 12], [186, 9]], [[81, 30]], [[41, 30]], [[77, 30]], [[151, 25]], [[2, 12], [119, 10]], [[176, 30]], [[168, 9], [46, 20]], [[79, 30]], [[125, 9], [197, 14], [117, 7]], [[135, 15], [196, 8]], [[208, 30]], [[81, 6], [154, 13], [83, 10]], [[121, 30]], [[193, 19], [19, 10], [121, 1]], [[166, 6], [80, 20]], [[104, 30]], [[40, 30]], [[159, 19], [108, 11]], [[48, 5], [182, 15], [95, 10]], [[188, 22], [91, 6], [199, 1]], [[157, 22], [3, 8]], [[130, 22]], [[172, 30]], [[16, 10], [148, 2], [165, 4], [77, 8], [111, 3]], [[83, 30]], [[27, 22], [187, 7]], [[72, 22]], [[66, 15], [25, 14]], [[156, 16]], [[164, 4], [17, 24]], [[143, 29]], [[75, 18], [101, 6]], [[8, 16]], [[28, 2], [149, 20], [24, 8]], [[149, 30]], [[126, 14], [144, 12]], [[131, 16]], [[44, 30]], [[152, 15], [34, 14]], [[207, 21], [173, 7]]]}</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rigid (capacity 16):
+8 Metre (capacity 22):
+11 Metre (capacity 30):
+97-K (13) -&gt; 9-B (15)
+100-L (30)
+198-W (5) -&gt; 120-O (23)
+35-C (30)
+153-S (30)
+194-V (27)
+116-N (10) -&gt; 203-W (1) -&gt; 177-T (11)
+165-S (30)
+6-B (23)
+53-E (12) -&gt; 186-V (9)
+81-H (30)
+41-C (30)
+77-H (30)
+151-R (25)
+2-A (12) -&gt; 119-O (10)
+176-T (30)
+168-S (9) -&gt; 46-D (20)
+79-H (30)
+125-P (9) -&gt; 197-W (14) -&gt; 117-N (7)
+135-P (15) -&gt; 196-W (8)
+208-Z (30)
+81-H (6) -&gt; 154-S (13) -&gt; 83-H (10)
+121-O (30)
+193-V (19) -&gt; 19-B (10) -&gt; 121-O (1)
+166-S (6) -&gt; 80-H (20)
+104-M (30)
+40-C (30)
+159-S (19) -&gt; 108-M (11)
+48-D (5) -&gt; 182-U (15) -&gt; 95-K (10)
+188-V (22) -&gt; 91-K (6) -&gt; 199-W (1)
+157-S (22) -&gt; 3-A (8)
+130-P (22)
+172-S (30)
+16-B (10) -&gt; 148-R (2) -&gt; 165-S (4) -&gt; 77-H (8) -&gt; 111-M (3)
+83-H (30)
+27-C (22) -&gt; 187-V (7)
+72-G (22)
+66-G (15) -&gt; 25-C (14)
+156-S (16)
+164-S (4) -&gt; 17-B (24)
+143-P (29)
+75-H (18) -&gt; 101-L (6)
+8-B (16)
+28-C (2) -&gt; 149-R (20) -&gt; 24-B (8)
+149-R (30)
+126-P (14) -&gt; 144-Q (12)
+131-P (16)
+44-D (30)
+152-R (15) -&gt; 34-C (14)
+207-Y (21) -&gt; 173-T (7)
+</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>3601.0539597</v>
+      </c>
+      <c r="H7" t="n">
+        <v>412483.5701333333</v>
+      </c>
+      <c r="J7">
+        <f>C7-(H7+I7*10)</f>
+        <v/>
+      </c>
+      <c r="K7" s="4">
+        <f>J7/C7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="15" t="n">
+        <v>43795</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>{"3": [[[22, 36]], [[41, 39]], [[23, 40]], [[85, 30]], []], "1": [[[156, 17], [132, 5]], [[17, 10], [164, 1], [197, 11]], [[207, 22]], [[83, 22]], [[119, 12], [2, 10]], [[46, 20]], [[188, 20]], [[151, 20]], [[56, 11], [118, 9]], [[72, 15], [18, 7]], [[58, 15], [22, 7]], [[142, 22]], [[50, 2], [78, 6], [113, 4], [94, 6], [102, 4]], [[35, 21]], [[168, 13], [17, 7]], [[163, 19], [3, 3]], [[186, 22]], [[205, 9], [45, 6], [206, 7]], [[144, 21]], [[157, 10], [28, 12]], [[121, 4], [143, 6], [193, 7], [185, 5]], [[135, 10], [95, 3], [182, 7]], [[151, 22]], [[173, 13], [131, 7]], [[40, 22]], [[57, 21]], [[89, 22]], [[158, 22]], [[84, 22]]], "2": [[[59, 30]], [[68, 9], [1, 21]], [[72, 30]], [[29, 30]], [[18, 18], [200, 12]], [[96, 27]], [[152, 4], [15, 26]], [[139, 30]], [[24, 9], [25, 7], [59, 11]], [[40, 30]], [[117, 2], [126, 14], [125, 14]], [[157, 15], [95, 15]], [[135, 15], [33, 5], [182, 10]], [[121, 14], [143, 15]], [[66, 19], [168, 11]], [[69, 30]], [[153, 30]], [[91, 27]], [[49, 30]], [[208, 30]], [[29, 10], [1, 20]], [[12, 20]], [[81, 5], [91, 23]], [[193, 5], [19, 12], [101, 10]], [[104, 12], [100, 15], [153, 3]], [[95, 30]], [[201, 30]], [[111, 30]], [[99, 30]], [[124, 30]], [[150, 30]], [[109, 30]], [[104, 30]], [[15, 30]], [[98, 30]], [[99, 10], [26, 20]], [[149, 30]], [[150, 19], [149, 7], [165, 4]], [[110, 7], [176, 8], [174, 15]], [[172, 19], [111, 11]], [[109, 28]], [[156, 20], [132, 10]], [[10, 30]], [[76, 20], [10, 10]], [[17, 29], [164, 1]], [[53, 14], [130, 16]], [[3, 25], [51, 4]], [[29, 27]], [[154, 30]], [[11, 2], [208, 11], [97, 14]], [[69, 30]], [[157, 1], [193, 7], [143, 11], [121, 11]], [[178, 28], [61, 2]], [[45, 7], [175, 23]], [[185, 17]], [[19, 2], [28, 17], [101, 11]], [[69, 30]], [], [[147, 7]], [[85, 30]], [[20, 30]], [[84, 30]], [[116, 5], [85, 23]], [[20, 18]]], "0": [[[7, 4], [188, 6], [39, 5]], [[120, 9], [198, 6]], [[80, 16]], [[69, 15]], [[134, 13]], [[92, 16]], [[112, 2], [198, 7], [42, 1]], [[51, 12]], [[62, 13], [87, 2]], [[47, 12], [166, 4]], [[128, 14]], [[105, 5], [46, 4], [115, 7]], [[191, 4], [48, 10], [96, 2]], [[186, 16]], [[134, 8], [171, 5]], [[93, 10], [151, 6]], [[8, 5], [33, 5]], [[142, 4], [12, 11]], [[130, 3], [53, 13]], [[13, 16]], [[9, 11]], [[97, 15]], [[75, 3], [135, 5]], [[90, 16]], [], [], [], [[195, 1]], [[83, 16]], [[69, 7]], [[158, 13]]]}</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1275847.080066667</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>{"3": [[[85, 40]], [[72, 40]], [[12, 31]], [[120, 9], [98, 30]], [[153, 33], [131, 7]], [[84, 40]], [[20, 40]], [[115, 7], [47, 12], [126, 14]], [[22, 40]], [[49, 30], [166, 4]], [[150, 40]], [[15, 40]], [[45, 13], [22, 3]], [[116, 5], [84, 12], [147, 7], [110, 7], [42, 1]], [[91, 10], [58, 15]], [[33, 10], [135, 30]], [[35, 21], [125, 14], [11, 2]], [[178, 28], [56, 11]], [[158, 35]], [[10, 40]], [[157, 26], [117, 2], [61, 2], [39, 5], [164, 2]], [[95, 40]], [[69, 40]], [[205, 9]], [[111, 40]], [[124, 30]], [[85, 40]], [[92, 40]], [[59, 1], [92, 8], [66, 19]], [[175, 23]], [[91, 40]], [[40, 40]], [[96, 29]], [[9, 11], [28, 29]], [[163, 19]], [[23, 40]], [[185, 22], [176, 8]], [[101, 21], [200, 12]], [[2, 10], [142, 26]], [[69, 40]], [[207, 22], [198, 13]], [[50, 2], [78, 6], [113, 4], [182, 17], [191, 4]], [[17, 40]], [[134, 21], [171, 5]], [[69, 32]], [[83, 38]], [[130, 19], [13, 16]], [[29, 40]], [[97, 29], [87, 2], [94, 6]], [[72, 5], [195, 1], [154, 30]], [[104, 40]], [[208, 40]], [[118, 9], [19, 14]], [[186, 38]], [[1, 40]], [[144, 21], [206, 7]], [[128, 14]], [[149, 37], [111, 1]], [[165, 4], [201, 30]], [[99, 40]], [[90, 16]], [[197, 11], [76, 20]], [[132, 15]], [[109, 40]], [[102, 4], [57, 21], [119, 12]], [[17, 6], [81, 5], [80, 16], [152, 4]], [[59, 40]], [[168, 24], [7, 4]], [[41, 39]], [[100, 15]], [[3, 28], [48, 10]], [[18, 25], [93, 10], [1, 1]], [[150, 9], [172, 19]], [[151, 40]], [[188, 26], [24, 9], [105, 5]], [[20, 8], [89, 22], [85, 3]], [[139, 30]], [[40, 12], [173, 13]], [[62, 13], [151, 8]], [[156, 37]], [[121, 29], [8, 5]], [[53, 27]], [[26, 20], [109, 18]], [[68, 9], [29, 27], [112, 2]], [[193, 19], [51, 16], [208, 1]], [[25, 7], [46, 24]], [[174, 15], [15, 16], [104, 2], [75, 3]], [[95, 8], [143, 32]]]}</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Link (capacity 40):
+85-K (40)
+72-G (40)
+12-B (31)
+120-O (9) -&gt; 98-L (30)
+153-S (33) -&gt; 131-P (7)
+84-K (40)
+20-B (40)
+115-N (7) -&gt; 47-D (12) -&gt; 126-P (14)
+22-B (40)
+49-D (30) -&gt; 166-S (4)
+150-R (40)
+15-B (40)
+45-D (13) -&gt; 22-B (3)
+116-N (5) -&gt; 84-K (12) -&gt; 147-R (7) -&gt; 110-M (7) -&gt; 42-C (1)
+91-K (10) -&gt; 58-G (15)
+33-C (10) -&gt; 135-P (30)
+35-C (21) -&gt; 125-P (14) -&gt; 11-B (2)
+178-T (28) -&gt; 56-F (11)
+158-S (35)
+10-B (40)
+157-S (26) -&gt; 117-N (2) -&gt; 61-G (2) -&gt; 39-C (5) -&gt; 164-S (2)
+95-K (40)
+69-G (40)
+205-W (9)
+111-M (40)
+124-O (30)
+85-K (40)
+92-K (40)
+59-G (1) -&gt; 92-K (8) -&gt; 66-G (19)
+175-T (23)
+91-K (40)
+40-C (40)
+96-K (29)
+9-B (11) -&gt; 28-C (29)
+163-S (19)
+23-B (40)
+185-V (22) -&gt; 176-T (8)
+101-L (21) -&gt; 200-W (12)
+2-A (10) -&gt; 142-P (26)
+69-G (40)
+207-Y (22) -&gt; 198-W (13)
+50-D (2) -&gt; 78-H (6) -&gt; 113-M (4) -&gt; 182-U (17) -&gt; 191-V (4)
+17-B (40)
+134-P (21) -&gt; 171-S (5)
+69-G (32)
+83-H (38)
+130-P (19) -&gt; 13-B (16)
+29-C (40)
+97-K (29) -&gt; 87-K (2) -&gt; 94-K (6)
+72-G (5) -&gt; 195-W (1) -&gt; 154-S (30)
+104-M (40)
+208-Z (40)
+118-N (9) -&gt; 19-B (14)
+186-V (38)
+1-A (40)
+144-Q (21) -&gt; 206-W (7)
+128-P (14)
+149-R (37) -&gt; 111-M (1)
+165-S (4) -&gt; 201-W (30)
+99-L (40)
+90-K (16)
+197-W (11) -&gt; 76-H (20)
+132-P (15)
+109-M (40)
+102-L (4) -&gt; 57-F (21) -&gt; 119-O (12)
+17-B (6) -&gt; 81-H (5) -&gt; 80-H (16) -&gt; 152-R (4)
+59-G (40)
+168-S (24) -&gt; 7-B (4)
+41-C (39)
+100-L (15)
+3-A (28) -&gt; 48-D (10)
+18-B (25) -&gt; 93-K (10) -&gt; 1-A (1)
+150-R (9) -&gt; 172-S (19)
+151-R (40)
+188-V (26) -&gt; 24-B (9) -&gt; 105-M (5)
+20-B (8) -&gt; 89-K (22) -&gt; 85-K (3)
+139-P (30)
+40-C (12) -&gt; 173-T (13)
+62-G (13) -&gt; 151-R (8)
+156-S (37)
+121-O (29) -&gt; 8-B (5)
+53-E (27)
+26-C (20) -&gt; 109-M (18)
+68-G (9) -&gt; 29-C (27) -&gt; 112-M (2)
+193-V (19) -&gt; 51-D (16) -&gt; 208-Z (1)
+25-C (7) -&gt; 46-D (24)
+174-T (15) -&gt; 15-B (16) -&gt; 104-M (2) -&gt; 75-H (3)
+95-K (8) -&gt; 143-P (32)
+</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>3902.6114637</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1140670.6408</v>
+      </c>
+      <c r="J8">
+        <f>C8-(H8+I8*10)</f>
+        <v/>
+      </c>
+      <c r="K8" s="4">
+        <f>J8/C8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="17" t="n">
+        <v>43768</v>
+      </c>
+      <c r="J9">
+        <f>C9-(H9+I9*10)</f>
+        <v/>
+      </c>
+      <c r="K9" s="4">
+        <f>J9/C9</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added cost for hiring extra vehicles Moved solution reconstruction method Archive stops without loads are now given a load of 1 so that they are not ignored
</commit_message>
<xml_diff>
--- a/vrp_dss/Solve Times Summary.xlsx
+++ b/vrp_dss/Solve Times Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Aaron\Documents\Git Repositories\VRP-DSS\vrp_dss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23664A35-128B-481D-8FF4-71464225EF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D33A313-095B-456D-97EC-21427FEBA19E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="248">
   <si>
     <t># Customers</t>
   </si>
@@ -3908,6 +3908,21 @@
 140-P (30)
 41-C (6) -&gt; 194-V (8) -&gt; 187-V (8) -&gt; 35-C (5)
 </t>
+  </si>
+  <si>
+    <t>Excess vehicles used have increased costs</t>
+  </si>
+  <si>
+    <t>Seeding solutions</t>
+  </si>
+  <si>
+    <t>Unlimited fleets</t>
+  </si>
+  <si>
+    <t>Aspects added</t>
+  </si>
+  <si>
+    <t>Performance Optimisations</t>
   </si>
 </sst>
 </file>
@@ -7302,7 +7317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -7679,7 +7694,7 @@
   <dimension ref="A1:V208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="O29" sqref="O29"/>
@@ -12427,10 +12442,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12446,9 +12461,10 @@
     <col min="9" max="9" width="12.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>208</v>
       </c>
@@ -12482,8 +12498,11 @@
       <c r="K1" s="5" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>43745</v>
       </c>
@@ -12511,7 +12530,7 @@
         <v>2.9036620164271349E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>43768</v>
       </c>
@@ -12538,8 +12557,11 @@
         <f t="shared" si="0"/>
         <v>-2.8570731981184649E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>43775</v>
       </c>
@@ -12570,7 +12592,7 @@
         <v>4.974219837758781E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>43775</v>
       </c>
@@ -12600,8 +12622,11 @@
         <f t="shared" si="0"/>
         <v>0.11307985414694049</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>43768</v>
       </c>
@@ -12632,7 +12657,7 @@
         <v>-3.3168933972986682E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>43745</v>
       </c>
@@ -12663,7 +12688,7 @@
         <v>0.12079447725851343</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>43795</v>
       </c>
@@ -12694,7 +12719,7 @@
         <v>0.105950345757427</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>43768</v>
       </c>
@@ -12725,7 +12750,7 @@
         <v>-1.9547239268025863E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>43745</v>
       </c>
@@ -12755,8 +12780,11 @@
         <f t="shared" ref="K10:K11" si="3">J10/C10</f>
         <v>0.12671645898302314</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>43768</v>
       </c>
@@ -12787,8 +12815,26 @@
         <v>-1.4481975484296224E-2</v>
       </c>
     </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>43745</v>
+      </c>
+      <c r="L12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>43768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>43795</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K1:K1048576">
+  <conditionalFormatting sqref="K1:K1048576 L1">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Fixed bug in unlimited split algorithm. More testing done. Need to properly verify archive routes versus the model data.
</commit_message>
<xml_diff>
--- a/vrp_dss/Solve Times Summary.xlsx
+++ b/vrp_dss/Solve Times Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Aaron\Documents\Git Repositories\VRP-DSS\vrp_dss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D33A313-095B-456D-97EC-21427FEBA19E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140A615A-C713-4823-8019-A1535E71DA7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="270">
   <si>
     <t># Customers</t>
   </si>
@@ -3035,6 +3035,9 @@
   </si>
   <si>
     <t>Difference (%)</t>
+  </si>
+  <si>
+    <t>Aspects added</t>
   </si>
   <si>
     <t>{"2": [[[17, 24], [164, 4]], [[44, 30]], [[111, 3], [77, 27]], [[149, 28], [148, 2]], [[165, 30]], [[159, 19], [194, 11]], [[41, 30]], [[172, 30]], [[79, 30]], [[104, 30]], [[6, 23], [187, 7]], [[176, 30]], [[153, 30]], [[208, 30]], [[35, 30]], [[100, 30]], [[83, 20]], [[40, 30]], [[117, 7], [126, 14], [125, 9]], [[121, 12], [143, 11], [193, 7]], [[80, 20], [168, 9]], [[135, 5], [182, 15], [95, 10]], [[81, 30]], [[193, 12], [143, 18]], [[121, 19], [135, 10]]], "1": [[[75, 18]], [[149, 22]], [[24, 8], [25, 14]], [[207, 21]], [[72, 22]], [[119, 10], [2, 12]], [[157, 22]], [[46, 20]], [[188, 22]], [[186, 9], [53, 12]], [[130, 22]], [[83, 20]], [[116, 10], [177, 11], [203, 1]], [[27, 22]]], "0": [[[194, 16]], [[16, 10], [165, 4]], [[156, 16]], [[77, 11]], [[120, 11], [198, 5]], [[151, 16]], [[196, 8], [48, 5]], [[34, 14]], [[9, 15]], [[154, 13]], [[8, 16]], [[108, 11]], [[152, 15]], [[120, 12]], [[199, 1], [91, 6], [81, 6]], [[197, 14]], [[131, 16]], [[151, 9], [173, 7]], [[144, 12]], [[166, 6], [28, 2], [3, 8]], [[97, 13]], [[66, 15]]]}</t>
@@ -3201,6 +3204,9 @@
 44-D (30)
 165-S (30)
 40-C (15) -&gt; 153-S (14)</t>
+  </si>
+  <si>
+    <t>Unlimited fleets</t>
   </si>
   <si>
     <t>{"0": [[[108, 14]], [[56, 9], [118, 7]], [[105, 7], [199, 9]], [[9, 5], [196, 10], [74, 1]], [[192, 16]], [[154, 16]], [[63, 16]], [[48, 13]], [[70, 14], [192, 2]], [[197, 13]], [[37, 1]], [[34, 15]], [[186, 16]], [[93, 10]], [[38, 14], [178, 2]], [[37, 1]], [[4, 10], [53, 6]], [[131, 13]], [[16, 6], [149, 8]], [[207, 16]], [[120, 16]], [[12, 7], [198, 6]], [[151, 1], [12, 7]], [[184, 16]], [[9, 13]], [[166, 10], [101, 2]], [[168, 8], [7, 4], [115, 4]], [[186, 14]], [[37, 2], [81, 1], [91, 13]], [[95, 16]], [[83, 16]], [[75, 9], [135, 6]], [[188, 12], [39, 1]], [[101, 7], [19, 6], [143, 1], [193, 2]], [[46, 16]]], "2": [[[123, 27], [151, 1]], [[55, 30]], [[81, 30]], [[151, 27]], [[44, 30]], [[77, 21], [44, 6]], [[194, 30]], [[159, 24], [6, 1], [187, 2], [194, 3]], [[100, 30]], [[110, 21], [17, 8], [164, 1]], [[68, 15], [200, 10], [72, 5]], [[72, 30]], [[149, 29], [148, 1]], [[165, 27]], [[15, 30]], [[35, 30]], [[41, 30]], [[172, 28]], [[79, 30]], [[208, 30]], [[40, 29], [41, 1]], [[117, 5], [126, 12], [125, 13]], [[119, 14], [2, 13]], [[19, 10], [28, 20]], [[110, 2], [15, 28]], [[91, 30]], [[32, 30]], [[151, 30]], [[28, 3], [182, 15], [95, 9]]], "1": [[[132, 20]], [[33, 22]], [[8, 20], [33, 2]], [[104, 11], [174, 11]], [[176, 17], [35, 5]], [[153, 12], [82, 1], [100, 9]], [[25, 20], [52, 2]], [[144, 20]], [[139, 20]], [[130, 22]], [[83, 22]], [[59, 22]], [[62, 22]], [[96, 17], [184, 2], [74, 2]], [[152, 22]], [[29, 18], [154, 4]], [[208, 22]], [[97, 21], [4, 1]], [[57, 21]], [[185, 2], [3, 9], [88, 6], [208, 3]], [[178, 21], [115, 1]], [[193, 9], [143, 3], [121, 10]], [[121, 4], [163, 12], [51, 1], [135, 4]], [[66, 22]]]}</t>
@@ -3430,6 +3436,9 @@
 </t>
   </si>
   <si>
+    <t>Performance Optimisations</t>
+  </si>
+  <si>
     <t>{"0": [[[66, 16]], [[79, 16]], [[96, 16]], [[66, 16]], [[40, 15]], [[144, 3], [117, 6], [174, 5]], [[131, 12]], [[151, 15]]], "1": [[[207, 20], [123, 2]], [[150, 8], [148, 6], [66, 2]], [[38, 22]], [[4, 11], [48, 4]]], "2": [[[208, 24]], [[4, 30]], [[165, 30]], [[81, 30]], [[104, 30]], [[53, 13], [63, 16]], [[32, 27]], [[140, 30]], [[149, 30]], [[70, 7], [154, 14], [1, 4]], [[3, 27], [193, 3]], [[24, 25], [74, 5]], [[97, 30]], [[44, 30]], [[6, 14], [139, 15]], [[121, 6], [163, 17], [182, 7]], [[15, 28]], [[16, 30]], [[92, 30]], [[100, 30]], [[77, 30]], [[59, 28]], [[104, 6], [176, 16]], [[25, 30]], [[101, 10], [9, 10], [33, 9]], [[194, 8], [187, 8], [41, 6]], [[197, 25]], [[72, 30]], [[125, 14], [126, 10]], [[134, 10], [42, 12]], [[88, 22], [75, 7]], [[188, 15], [39, 1], [132, 10]], [[17, 16], [143, 5], [19, 6]], [[81, 2], [91, 13], [199, 10]], [[186, 15]], [[152, 4], [108, 9], [18, 15]], [[2, 14], [119, 12], [83, 1]], [[49, 24]], [[172, 20], [25, 5]], [[168, 8], [120, 16]], [[200, 15], [37, 10]], [[156, 12], [46, 15]], [[29, 29]], [[83, 30]], [[57, 15], [94, 5], [62, 1]], [[82, 22]], [[34, 16], [171, 2]], [[97, 7], [28, 6], [95, 15]], [[192, 21], [198, 7]], [[55, 30]], [[153, 14], [98, 16]], [[77, 7], [79, 21]], [[33, 30]], [[35, 30]], [[209, 9], [196, 13]], [[35, 5], [149, 24]], [[172, 30]], [[110, 19]], [[153, 30]], [[41, 30]], [[194, 30]], [[159, 24], [135, 5]], [[8, 4], [157, 24], [191, 2]], [[8, 30]], [[68, 10], [93, 9]], [[40, 30]]]}</t>
   </si>
   <si>
@@ -3819,6 +3828,9 @@
 </t>
   </si>
   <si>
+    <t>Seeding solutions</t>
+  </si>
+  <si>
     <t>{"0": [[[37, 10], [123, 2]], [[9, 10], [48, 4]], [[196, 13], [157, 2]], [[154, 14]], [[144, 3]], [[34, 16]], [[63, 16]], [[108, 9]], [[120, 16]], [[199, 10], [74, 5]], [[93, 9], [70, 7]], [[151, 15]], [[91, 13], [81, 2]], [[53, 13]], [[197, 16]], [[131, 12], [8, 4]], [[66, 12]], [[83, 9]], [[79, 7], [77, 7]], [[198, 7]], [[96, 16]], [[46, 15]], [[188, 15], [39, 1]], [[17, 16]], [[42, 12]], [[134, 10], [171, 2]], [[62, 1], [57, 15]], [[191, 2], [94, 5]]], "1": [[[192, 21]], [[38, 22]], [[33, 9], [4, 11]], [[88, 22]], [[82, 22]], [[68, 10], [135, 5], [1, 4]], [[28, 6], [18, 15]], [[207, 20]], [[83, 22]], [[2, 14]], [[119, 12]], [[200, 15]], [[3, 22]], [[157, 22]], [[163, 17], [3, 5]], [[66, 22]]], "2": [[[33, 30]], [[4, 30]], [[32, 27]], [[81, 30]], [[8, 30]], [[55, 30]], [[44, 30]], [[77, 30]], [[159, 24], [41, 6]], [[150, 8], [172, 20]], [[98, 16], [153, 14]], [[149, 24], [148, 6]], [[149, 30]], [[165, 30]], [[172, 30]], [[15, 28]], [[6, 14], [187, 8], [194, 8]], [[176, 16], [35, 5], [209, 9]], [[153, 30]], [[104, 30]], [[100, 30]], [[110, 19], [174, 5], [104, 6]], [[16, 30]], [[156, 12], [168, 8], [132, 10]], [[72, 30]], [[29, 29]], [[35, 30]], [[41, 30]], [[194, 30]], [[79, 30]], [[208, 24], [152, 4]], [[24, 25], [25, 5]], [[25, 30]], [[117, 6], [126, 10], [125, 14]], [[40, 30]], [[59, 28]], [[92, 30]], [[139, 15], [40, 15]], [[75, 7], [121, 6], [143, 5], [193, 3], [19, 6]], [[97, 30]], [[97, 7], [186, 15]], [[95, 15], [182, 7]], [[101, 10]], [[49, 24]], [[197, 9]], [[140, 30]]]}</t>
   </si>
   <si>
@@ -3910,19 +3922,771 @@
 </t>
   </si>
   <si>
+    <t>{"2": [[[17, 24], [164, 4]], [[44, 30]], [[111, 2], [77, 30]], [[149, 27], [148, 3]], [[165, 30]], [[159, 19], [194, 11]], [[41, 30]], [[172, 30]], [[79, 30]], [[104, 30]], [[6, 23], [187, 7]], [[176, 30]], [[153, 30]], [[208, 30]], [[35, 30]], [[100, 30]], [[83, 18]], [[40, 30]], [[117, 7], [126, 14], [125, 9]], [[121, 30], [143, 29], [193, 19]], [[80, 20], [168, 9]], [[135, 15], [182, 15], [95, 10]], [[81, 30]], [[193, 0], [143, 0]], [[121, 1], [135, 0]]], "1": [[[75, 19]], [[149, 22]], [[24, 8], [25, 14]], [[207, 21]], [[72, 22]], [[119, 10], [2, 12]], [[157, 22]], [[46, 20]], [[188, 22]], [[186, 9], [53, 12]], [[130, 22]], [[83, 22]], [[116, 10], [177, 11], [203, 1]], [[27, 22]]], "0": [[[194, 16]], [[16, 10], [165, 4]], [[156, 15], [39, 1]], [[77, 9]], [[120, 16], [198, 5]], [[151, 16]], [[196, 8], [48, 5]], [[34, 14]], [[9, 15]], [[154, 14]], [[8, 16]], [[108, 11]], [[152, 15]], [[120, 7]], [[199, 1], [91, 6], [81, 6]], [[197, 14]], [[131, 16]], [[151, 9], [173, 7]], [[144, 12]], [[166, 6], [28, 2], [3, 8]], [[97, 13]], [[66, 15]]]}</t>
+  </si>
+  <si>
+    <t>{"0": [[[197, 14]], [[135, 15]], [[196, 8], [48, 5]], [[131, 16]], [[9, 15]], [[97, 13]], [[95, 10], [199, 1]], [[173, 7]], [[53, 12]], [[2, 12]], [[198, 5], [120, 1]], [[19, 11]], [[8, 16]], [[81, 16]], [[154, 14]], [[119, 10]], [[186, 9]], [[156, 15]], [[34, 14]], [[108, 11]], [[152, 15]]], "1": [[[27, 22]], [[72, 22]], [[120, 22]], [[144, 12], [16, 10]], [[188, 22]], [[91, 6]], [[81, 22]], [[46, 20]], [[159, 19]], [[207, 21]], [[130, 22]], [[80, 20]], [[25, 14], [24, 8]], [[166, 6]], [[182, 15], [28, 2]]], "2": [[[172, 30]], [[157, 22], [3, 8]], [[17, 24], [101, 6]], [[77, 30]], [[176, 30]], [[100, 30]], [[187, 7], [203, 1], [177, 11], [116, 10]], [[153, 30]], [[104, 30]], [[35, 30]], [[151, 25]], [[149, 30]], [[44, 30]], [[208, 30]], [[168, 9], [66, 15], [39, 1], [164, 4]], [[40, 30]], [[143, 29]], [[79, 30]], [[111, 2], [77, 9], [149, 19]], [[41, 30]], [[125, 9], [117, 7], [126, 14]], [[6, 23]], [[194, 27]]], "3": [[[165, 34], [148, 3]], [[193, 19], [75, 19]], [[121, 31]], [[83, 40]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+197-W (14)
+135-P (15)
+196-W (8) -&gt; 48-D (5)
+131-P (16)
+9-B (15)
+97-K (13)
+95-K (10) -&gt; 199-W (1)
+173-T (7)
+53-E (12)
+2-A (12)
+198-W (5) -&gt; 120-O (1)
+19-B (11)
+8-B (16)
+81-H (16)
+154-S (14)
+119-O (10)
+186-V (9)
+156-S (15)
+34-C (14)
+108-M (11)
+152-R (15)
+8 Metre (capacity 22):
+27-C (22)
+72-G (22)
+120-O (22)
+144-Q (12) -&gt; 16-B (10)
+188-V (22)
+91-K (6)
+81-H (22)
+46-D (20)
+159-S (19)
+207-Y (21)
+130-P (22)
+80-H (20)
+25-C (14) -&gt; 24-B (8)
+166-S (6)
+182-U (15) -&gt; 28-C (2)
+11 Metre (capacity 30):
+172-S (30)
+157-S (22) -&gt; 3-A (8)
+17-B (24) -&gt; 101-L (6)
+77-H (30)
+176-T (30)
+100-L (30)
+187-V (7) -&gt; 203-W (1) -&gt; 177-T (11) -&gt; 116-N (10)
+153-S (30)
+104-M (30)
+35-C (30)
+151-R (25)
+149-R (30)
+44-D (30)
+208-Z (30)
+168-S (9) -&gt; 66-G (15) -&gt; 39-C (1) -&gt; 164-S (4)
+40-C (30)
+143-P (29)
+79-H (30)
+111-M (2) -&gt; 77-H (9) -&gt; 149-R (19)
+41-C (30)
+125-P (9) -&gt; 117-N (7) -&gt; 126-P (14)
+6-B (23)
+194-V (27)
+Link (capacity 40):
+165-S (34) -&gt; 148-R (3)
+193-V (19) -&gt; 75-H (19)
+121-O (31)
+83-H (40)
+</t>
+  </si>
+  <si>
     <t>Excess vehicles used have increased costs</t>
   </si>
   <si>
-    <t>Seeding solutions</t>
-  </si>
-  <si>
-    <t>Unlimited fleets</t>
-  </si>
-  <si>
-    <t>Aspects added</t>
-  </si>
-  <si>
-    <t>Performance Optimisations</t>
+    <t>{"2": [[[149, 30]], [[172, 30]], [[165, 30]], [[44, 30]], [[149, 24], [148, 6]], [[159, 24], [41, 6]], [[77, 30]], [[15, 28]], [[150, 8], [172, 20]], [[98, 16], [153, 14]], [[194, 30]], [[79, 30]], [[6, 14], [187, 8], [194, 8]], [[104, 30]], [[41, 30]], [[153, 30]], [[176, 16], [35, 5], [209, 9]], [[100, 30]], [[208, 24], [152, 4]], [[16, 30]], [[24, 25], [25, 4], [66, 0]], [[110, 19], [174, 5], [104, 6]], [[35, 30]], [[156, 11], [168, 9], [132, 10]], [[25, 30]], [[59, 28]], [[117, 6], [126, 10], [125, 14]], [[40, 30]], [[92, 30]], [[72, 30]], [[29, 29]], [[139, 15], [40, 15]], [[121, 6], [143, 5], [193, 4], [19, 6], [97, 30]], [[186, 0], [95, 0], [182, 6], [101, 10], [75, 8]], [[33, 30]], [[4, 30]], [[49, 8], [197, 9]], [[32, 27]], [[81, 30]], [[8, 30]], [[55, 30]], [[97, 7]], [[140, 30]]], "0": [[[79, 7], [77, 7]], [[120, 16], [198, 6]], [[96, 16]], [[188, 15], [39, 1]], [[151, 15], [123, 2]], [[46, 16]], [[17, 15], [164, 1]], [[42, 12]], [[134, 10], [171, 2]], [[37, 10], [123, 0]], [[9, 10], [48, 5]], [[62, 1], [155, 1], [87, 1], [57, 13]], [[191, 2], [94, 5]], [[196, 13], [157, 2]], [[34, 16]], [[154, 15]], [[144, 3], [49, 16]], [[63, 16]], [[108, 9], [120, 1]], [[199, 10], [74, 5]], [[93, 9], [70, 7]], [[186, 15], [151, 0]], [[91, 13], [81, 2]], [[53, 13], [95, 15]], [[197, 16]], [[66, 13]], [[131, 12], [8, 4]], [[83, 9]]], "1": [[[207, 20]], [[83, 22], [2, 14]], [[82, 22]], [[119, 12], [2, 0]], [[68, 10], [1, 3], [18, 15], [112, 1]], [[18, 0], [200, 15]], [[157, 22]], [[163, 17], [3, 5]], [[192, 22]], [[66, 22]], [[38, 22]], [[33, 9], [4, 11]], [[88, 22]], [[3, 22]]]}</t>
+  </si>
+  <si>
+    <t>{"2": [[[149, 24]], [[172, 30]], [[165, 30]], [[44, 30]], [[149, 24], [148, 6]], [[159, 24], [41, 0]], [[77, 30]], [[15, 28]], [[150, 8], [172, 0]], [[98, 16], [153, 30]], [[194, 8]], [[79, 30]], [[6, 14], [187, 8], [194, 8]], [[104, 6]], [[41, 6]], [[153, 14]], [[176, 16], [35, 30], [209, 9]], [[100, 30]], [[208, 24], [152, 4]], [[16, 30]], [[24, 25], [25, 30], [66, 5]], [[110, 19], [174, 5], [104, 6]], [[35, 5]], [[156, 11], [168, 9], [132, 10]], [[25, 4]], [[59, 28]], [[117, 6], [126, 10], [125, 14]], [[40, 30]], [[92, 30]], [[72, 30]], [[29, 29]], [[139, 15], [40, 0]], [[121, 6], [143, 5], [193, 4], [19, 6], [97, 30]], [[186, 15], [95, 15], [182, 6], [101, 10], [75, 8]], [[33, 30]], [[4, 30]], [[49, 24], [197, 25]], [[32, 27]], [[81, 30]], [[8, 18]], [[55, 30]], [[97, 7]], [[140, 30]]], "0": [[[79, 16], [77, 16]], [[120, 16], [198, 6]], [[96, 16]], [[188, 15], [39, 1]], [[151, 15], [123, 2]], [[46, 16]], [[17, 15], [164, 1]], [[42, 12]], [[134, 10], [171, 2]], [[37, 10], [123, 0]], [[9, 10], [48, 5]], [[62, 1], [155, 1], [87, 1], [57, 13]], [[191, 2], [94, 5]], [[196, 13], [157, 16]], [[34, 16]], [[154, 15]], [[144, 3], [49, 0]], [[63, 16]], [[108, 9], [120, 1]], [[199, 10], [74, 5]], [[93, 9], [70, 7]], [[186, 0], [151, 0]], [[91, 13], [81, 16]], [[53, 13], [95, 0]], [[197, 16]], [[66, 0]], [[131, 12], [8, 16]], [[83, 16]]], "1": [[[207, 20]], [[83, 22], [2, 14]], [[82, 22]], [[119, 12], [2, 0]], [[68, 10], [1, 3], [18, 15], [112, 1]], [[18, 0], [200, 15]], [[157, 22]], [[163, 17], [3, 5]], [[192, 22]], [[66, 22]], [[38, 22]], [[33, 22], [4, 22]], [[88, 22]], [[3, 22]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 Metre (capacity 30):
+149-R (24)
+172-S (30)
+165-S (30)
+44-D (30)
+149-R (24) -&gt; 148-R (6)
+159-S (24) -&gt; 41-C (0)
+77-H (30)
+15-B (28)
+150-R (8) -&gt; 172-S (0)
+98-L (16) -&gt; 153-S (30)
+194-V (8)
+79-H (30)
+6-B (14) -&gt; 187-V (8) -&gt; 194-V (8)
+104-M (6)
+41-C (6)
+153-S (14)
+176-T (16) -&gt; 35-C (30) -&gt; 209-Z (9)
+100-L (30)
+208-Z (24) -&gt; 152-R (4)
+16-B (30)
+24-B (25) -&gt; 25-C (30) -&gt; 66-G (5)
+110-M (19) -&gt; 174-T (5) -&gt; 104-M (6)
+35-C (5)
+156-S (11) -&gt; 168-S (9) -&gt; 132-P (10)
+25-C (4)
+59-G (28)
+117-N (6) -&gt; 126-P (10) -&gt; 125-P (14)
+40-C (30)
+92-K (30)
+72-G (30)
+29-C (29)
+139-P (15) -&gt; 40-C (0)
+121-O (6) -&gt; 143-P (5) -&gt; 193-V (4) -&gt; 19-B (6) -&gt; 97-K (30)
+186-V (15) -&gt; 95-K (15) -&gt; 182-U (6) -&gt; 101-L (10) -&gt; 75-H (8)
+33-C (30)
+4-A (30)
+49-D (24) -&gt; 197-W (25)
+32-C (27)
+81-H (30)
+8-B (18)
+55-E (30)
+97-K (7)
+140-P (30)
+Rigid (capacity 16):
+79-H (16) -&gt; 77-H (16)
+120-O (16) -&gt; 198-W (6)
+96-K (16)
+188-V (15) -&gt; 39-C (1)
+151-R (15) -&gt; 123-O (2)
+46-D (16)
+17-B (15) -&gt; 164-S (1)
+42-C (12)
+134-P (10) -&gt; 171-S (2)
+37-C (10) -&gt; 123-O (0)
+9-B (10) -&gt; 48-D (5)
+62-G (1) -&gt; 155-S (1) -&gt; 87-K (1) -&gt; 57-F (13)
+191-V (2) -&gt; 94-K (5)
+196-W (13) -&gt; 157-S (16)
+34-C (16)
+154-S (15)
+144-Q (3) -&gt; 49-D (0)
+63-G (16)
+108-M (9) -&gt; 120-O (1)
+199-W (10) -&gt; 74-G (5)
+93-K (9) -&gt; 70-G (7)
+186-V (0) -&gt; 151-R (0)
+91-K (13) -&gt; 81-H (16)
+53-E (13) -&gt; 95-K (0)
+197-W (16)
+66-G (0)
+131-P (12) -&gt; 8-B (16)
+83-H (16)
+8 Metre (capacity 22):
+207-Y (20)
+83-H (22) -&gt; 2-A (14)
+82-H (22)
+119-O (12) -&gt; 2-A (0)
+68-G (10) -&gt; 1-A (3) -&gt; 18-B (15) -&gt; 112-M (1)
+18-B (0) -&gt; 200-W (15)
+157-S (22)
+163-S (17) -&gt; 3-A (5)
+192-V (22)
+66-G (22)
+38-C (22)
+33-C (22) -&gt; 4-A (22)
+88-K (22)
+3-A (22)
+</t>
+  </si>
+  <si>
+    <t>{"3": [[[22, 21]], [[41, 39]], [[23, 40]], [[85, 23]], []], "1": [[[156, 22], [132, 15]], [[17, 22], [164, 2], [197, 11]], [[207, 22]], [[83, 22]], [[119, 12], [2, 10]], [[46, 22]], [[188, 22]], [[151, 22]], [[56, 11], [118, 9]], [[72, 15], [18, 22]], [[58, 15], [22, 22]], [[142, 22]], [[50, 2], [78, 6], [113, 4], [94, 6], [102, 4]], [[35, 21]], [[168, 22], [17, 22]], [[163, 18], [3, 22]], [[186, 22]], [[205, 9], [45, 13], [206, 7]], [[144, 21], [106, 1]], [[157, 22], [28, 22], [11, 3]], [[121, 22], [143, 22], [193, 19], [185, 22]], [[135, 22], [95, 18], [182, 17]], [[151, 22]], [[173, 13], [131, 7]], [[40, 22]], [[57, 21]], [[89, 22]], [[158, 22]], [[84, 22]]], "2": [[[59, 30]], [[154, 1], [68, 8], [1, 30]], [[72, 30]], [[29, 30]], [[18, 2], [200, 13]], [[96, 29]], [[152, 4], [15, 26]], [[139, 30]], [[24, 9], [25, 7], [59, 11]], [[40, 30]], [[117, 2], [126, 14], [125, 14]], [[157, 4], [95, 0]], [[135, 10], [33, 10], [182, 0]], [[121, 7], [143, 11]], [[66, 19], [168, 2]], [[69, 30]], [[153, 30]], [[91, 30]], [[49, 30]], [[208, 30]], [[29, 30], [1, 11]], [[12, 30]], [[81, 5], [91, 20]], [[193, 0], [19, 14], [101, 21]], [[104, 12], [100, 15], [153, 3]], [[95, 30]], [[201, 30]], [[111, 30]], [[99, 30]], [[124, 30]], [[150, 30]], [[109, 30]], [[104, 30]], [[15, 30]], [[98, 30]], [[99, 10], [26, 20]], [[149, 30]], [[150, 19], [149, 7], [165, 4]], [[110, 7], [176, 8], [174, 14], [60, 1]], [[172, 20], [111, 10]], [[109, 28]], [[156, 15], [132, 0]], [[10, 30]], [[76, 20], [10, 10]], [[17, 2], [164, 0]], [[53, 27], [130, 19]], [[3, 8], [51, 16]], [[29, 8]], [[154, 30]], [[11, 0], [208, 11], [97, 29]], [[69, 30]], [[157, 0], [193, 0], [143, 0], [121, 0]], [[178, 28], [61, 2]], [[45, 0], [175, 23]], [[185, 0]], [[19, 0], [28, 6], [101, 0]], [[69, 30]], [], [[147, 7]], [[85, 30]], [[20, 30]], [[84, 30]], [[116, 5], [85, 30]], [[20, 18]]], "0": [[[7, 4], [188, 4], [39, 5]], [[120, 9], [198, 13]], [[80, 16]], [[69, 16]], [[134, 16]], [[92, 16]], [[112, 2], [198, 0], [42, 1]], [[51, 0]], [[62, 13], [155, 1], [87, 2]], [[47, 12], [166, 4]], [[128, 16]], [[105, 5], [46, 2], [115, 7]], [[191, 4], [48, 10], [96, 0]], [[186, 16]], [[134, 5], [171, 5]], [[93, 10], [151, 4]], [[8, 5], [33, 0]], [[142, 4], [12, 1]], [[130, 0], [53, 0]], [[13, 16]], [[9, 11]], [[97, 0]], [[75, 3], [135, 0]], [[90, 16]], [[128, 1]], [[128, 0]], [[128, 0]], [[195, 1]], [[83, 16]], [[69, 6]], [[158, 13]]]}</t>
+  </si>
+  <si>
+    <t>{"0": [[[115, 7]], [[2, 10]], [[132, 15]], [[24, 9], [25, 7]], [[113, 4]], [[119, 12]], [[135, 16]], [[198, 13]], [[39, 5]], [[17, 16]], [[84, 16]], [[72, 16]], [[105, 5]], [[154, 16]], [[83, 16], [102, 4]], [[72, 13]], [[62, 13]], [[56, 11]], [[80, 16]], [[174, 14]], [[48, 10]], [[90, 16]], [[135, 16]], [[112, 2]], [[78, 6]], [[154, 15], [195, 1]], [[164, 2], [47, 12]], [[66, 16]], [[9, 11]], [[33, 10]], [[100, 15]], [[13, 16]], [[143, 16]], [[171, 5]], [[173, 13]], [[72, 0]], [[45, 13], [11, 3]], [[120, 9]], [[1, 16]], [[22, 16]], [[68, 8]], [[59, 16]], [[208, 16]], [[19, 14]], [[200, 13]], [[58, 15]], [[93, 10]], [[165, 4], [75, 3]], [[118, 9]], [[7, 4]], [[51, 16]], [[191, 4]], [[205, 9]]], "1": [[[172, 20]], [[208, 22]], [[104, 22]], [[12, 22]], [[57, 21]], [[69, 22]], [[193, 19]], [[89, 22]], [[128, 17]], [[207, 22]]], "2": [[[97, 29]], [[206, 7], [175, 23]], [[49, 30]], [[17, 30]], [[121, 29]], [[28, 28]], [[22, 30], [66, 19]], [[59, 30]], [[92, 30]], [[178, 28]], [[201, 30]], [[149, 30]], [[109, 30]], [[23, 30]], [[15, 30]], [[176, 8], [117, 2], [8, 5]], [[186, 30]], [[151, 30]], [[35, 21]], [[163, 18]], [[46, 24]], [[41, 30]], [[83, 30]], [[85, 30], [147, 7]], [[84, 30], [20, 30]], [[53, 27]], [[92, 18]], [[94, 6], [155, 1], [87, 2]], [[153, 30]], [[3, 30]], [[139, 30]], [[149, 0]], [[85, 23]], [[130, 19]], [[91, 30], [81, 5]], [[188, 26]], [[26, 20], [99, 30]], [[150, 30]], [[69, 30]], [[96, 29]], [[186, 0]], [[185, 22], [131, 7]], [[134, 21]], [[142, 26]], [[151, 18]], [[10, 30]], [[20, 18]], [[15, 26]], [[41, 9], [144, 21]], [[166, 4]], [[91, 20]], [[126, 14], [197, 11]], [[168, 24]], [[101, 21]], [[60, 1], [116, 5], [40, 30], [42, 1]], [[182, 17], [152, 4]], [[98, 30]], [[12, 30]], [[29, 30]], [[110, 7], [153, 3]], [[109, 28], [106, 1]], [[40, 22]], [[143, 30]], [[157, 26]], [[18, 24]], [[10, 10], [76, 20]], [[23, 10], [150, 19]], [[99, 10]], [[69, 8]], [[125, 14], [61, 2], [208, 30]], [[104, 30], [95, 30]], [[84, 22]], [[50, 2]], [[85, 30]], [[124, 30]], [[69, 30]]], "3": [[[111, 40]], [[29, 28]], [[158, 35]], [[95, 40]], [[1, 25]], [[156, 37]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+115-N (7)
+2-A (10)
+132-P (15)
+24-B (9) -&gt; 25-C (7)
+113-M (4)
+119-O (12)
+135-P (16)
+198-W (13)
+39-C (5)
+17-B (16)
+84-K (16)
+72-G (16)
+105-M (5)
+154-S (16)
+83-H (16) -&gt; 102-L (4)
+72-G (13)
+62-G (13)
+56-F (11)
+80-H (16)
+174-T (14)
+48-D (10)
+90-K (16)
+135-P (16)
+112-M (2)
+78-H (6)
+154-S (15) -&gt; 195-W (1)
+164-S (2) -&gt; 47-D (12)
+66-G (16)
+9-B (11)
+33-C (10)
+100-L (15)
+13-B (16)
+143-P (16)
+171-S (5)
+173-T (13)
+72-G (0)
+45-D (13) -&gt; 11-B (3)
+120-O (9)
+1-A (16)
+22-B (16)
+68-G (8)
+59-G (16)
+208-Z (16)
+19-B (14)
+200-W (13)
+58-G (15)
+93-K (10)
+165-S (4) -&gt; 75-H (3)
+118-N (9)
+7-B (4)
+51-D (16)
+191-V (4)
+205-W (9)
+8 Metre (capacity 22):
+172-S (20)
+208-Z (22)
+104-M (22)
+12-B (22)
+57-F (21)
+69-G (22)
+193-V (19)
+89-K (22)
+128-P (17)
+207-Y (22)
+11 Metre (capacity 30):
+97-K (29)
+206-W (7) -&gt; 175-T (23)
+49-D (30)
+17-B (30)
+121-O (29)
+28-C (28)
+22-B (30) -&gt; 66-G (19)
+59-G (30)
+92-K (30)
+178-T (28)
+201-W (30)
+149-R (30)
+109-M (30)
+23-B (30)
+15-B (30)
+176-T (8) -&gt; 117-N (2) -&gt; 8-B (5)
+186-V (30)
+151-R (30)
+35-C (21)
+163-S (18)
+46-D (24)
+41-C (30)
+83-H (30)
+85-K (30) -&gt; 147-R (7)
+84-K (30) -&gt; 20-B (30)
+53-E (27)
+92-K (18)
+94-K (6) -&gt; 155-S (1) -&gt; 87-K (2)
+153-S (30)
+3-A (30)
+139-P (30)
+149-R (0)
+85-K (23)
+130-P (19)
+91-K (30) -&gt; 81-H (5)
+188-V (26)
+26-C (20) -&gt; 99-L (30)
+150-R (30)
+69-G (30)
+96-K (29)
+186-V (0)
+185-V (22) -&gt; 131-P (7)
+134-P (21)
+142-P (26)
+151-R (18)
+10-B (30)
+20-B (18)
+15-B (26)
+41-C (9) -&gt; 144-Q (21)
+166-S (4)
+91-K (20)
+126-P (14) -&gt; 197-W (11)
+168-S (24)
+101-L (21)
+60-G (1) -&gt; 116-N (5) -&gt; 40-C (30) -&gt; 42-C (1)
+182-U (17) -&gt; 152-R (4)
+98-L (30)
+12-B (30)
+29-C (30)
+110-M (7) -&gt; 153-S (3)
+109-M (28) -&gt; 106-M (1)
+40-C (22)
+143-P (30)
+157-S (26)
+18-B (24)
+10-B (10) -&gt; 76-H (20)
+23-B (10) -&gt; 150-R (19)
+99-L (10)
+69-G (8)
+125-P (14) -&gt; 61-G (2) -&gt; 208-Z (30)
+104-M (30) -&gt; 95-K (30)
+84-K (22)
+50-D (2)
+85-K (30)
+124-O (30)
+69-G (30)
+Link (capacity 40):
+111-M (40)
+29-C (28)
+158-S (35)
+95-K (40)
+1-A (25)
+156-S (37)
+</t>
+  </si>
+  <si>
+    <t>{"1": [[[192, 22]], [[123, 19], [2, 18]], [[154, 22]], [[32, 21]], [[186, 15], [53, 14]], [[95, 15], [197, 22]], [[44, 22]], [[98, 22]], [[110, 11], [174, 11]], [[156, 8], [168, 8], [132, 7]], [[25, 22]], [[153, 22]], [[207, 22]], [[18, 11], [200, 10]], [[59, 22]], [[68, 7], [1, 6], [112, 9]], [[62, 7], [155, 1], [87, 1], [57, 15]], [[17, 20], [164, 1]], [[101, 14], [95, 0], [75, 5]], [[4, 1], [8, 22], [55, 1]], [[3, 15], [19, 19]]], "0": [[[9, 7], [48, 5]], [[34, 14]], [[196, 16]], [[199, 6], [74, 7], [192, 2]], [[63, 16]], [[38, 16]], [[93, 2], [131, 14]], [[83, 15]], [[66, 10]], [[97, 16]], [[92, 13], [66, 0]], [[7, 13]], [[83, 16]], [[120, 13], [198, 6]], [[96, 15]], [[46, 16]], [[188, 14], [39, 2]], [[151, 16]], [[108, 11], [120, 0], [62, 0]], [[168, 0], [19, 0]], [[166, 9]], [[151, 8]], [[75, 0]]], "2": [[[81, 28], [91, 8]], [[55, 30]], [[77, 30]], [[187, 8], [6, 22]], [[159, 15], [40, 30], [194, 8]], [[150, 10], [172, 4], [149, 30]], [[194, 30]], [[176, 24], [35, 6]], [[153, 30]], [[16, 30]], [[149, 15], [148, 1]], [[165, 30]], [[172, 30]], [[15, 27]], [[41, 30]], [[79, 30]], [[35, 30]], [[100, 28]], [[208, 30]], [[24, 20], [209, 10]], [[104, 27]], [[139, 15], [41, 12]], [[82, 17], [197, 8]], [[29, 28]], [[157, 17], [182, 12], [88, 1]], [[117, 5], [126, 14], [125, 11]], [[119, 12], [2, 0]], [[121, 13], [143, 12], [193, 18], [19, 0]], [[66, 30]], [[152, 12], [186, 0], [81, 0], [91, 0]], [[163, 15], [51, 8], [3, 0]], [[189, 17], [140, 20]], [[8, 25]], [[193, 0], [143, 0], [101, 0], [121, 0], [135, 5]]], "3": [[[40, 16]], [[138, 1], [137, 38]]]}</t>
+  </si>
+  <si>
+    <t>{"1": [[[192, 22]], [[123, 19], [2, 18]], [[154, 22]], [[32, 21]], [[186, 15], [53, 14]], [[95, 15], [197, 22]], [[44, 22]], [[98, 22]], [[110, 11], [174, 11]], [[156, 8], [168, 8], [132, 7]], [[25, 22]], [[153, 22]], [[207, 22]], [[18, 11], [200, 10]], [[59, 22]], [[68, 7], [1, 6], [112, 9]], [[62, 7], [155, 1], [87, 1], [57, 15]], [[17, 20], [164, 1]], [[101, 14], [95, 0], [75, 5]], [[4, 1], [8, 22], [55, 22]], [[3, 15], [19, 19]]], "0": [[[9, 7], [48, 5]], [[34, 14]], [[196, 16]], [[199, 6], [74, 7], [192, 16]], [[63, 16]], [[38, 16]], [[93, 2], [131, 14]], [[83, 15]], [[66, 16]], [[97, 16]], [[92, 13], [66, 16]], [[7, 13]], [[83, 0]], [[120, 13], [198, 6]], [[96, 15]], [[46, 16]], [[188, 14], [39, 2]], [[151, 16]], [[108, 11], [120, 0], [62, 0]], [[168, 0], [19, 0]], [[166, 9]], [[151, 8]], [[75, 0]]], "2": [[[81, 28], [91, 8]], [[55, 15]], [[77, 30]], [[187, 8], [6, 22]], [[159, 15], [40, 16], [194, 30]], [[150, 10], [172, 4], [149, 30]], [[194, 8]], [[176, 24], [35, 30]], [[153, 22]], [[16, 30]], [[149, 15], [148, 1]], [[165, 30]], [[172, 4]], [[15, 27]], [[41, 30]], [[79, 30]], [[35, 6]], [[100, 28]], [[208, 30]], [[24, 20], [209, 10]], [[104, 27]], [[139, 15], [41, 12]], [[82, 17], [197, 30]], [[29, 28]], [[157, 17], [182, 12], [88, 1]], [[117, 5], [126, 14], [125, 11]], [[119, 12], [2, 0]], [[121, 13], [143, 12], [193, 18], [19, 0]], [[66, 30]], [[152, 12], [186, 0], [81, 0], [91, 0]], [[163, 15], [51, 8], [3, 0]], [[189, 17], [140, 20]], [[8, 17]], [[193, 0], [143, 0], [101, 0], [121, 0], [135, 5]]], "3": [[[40, 40]], [[138, 1], [137, 38]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Metre (capacity 22):
+192-V (22)
+123-O (19) -&gt; 2-A (18)
+154-S (22)
+32-C (21)
+186-V (15) -&gt; 53-E (14)
+95-K (15) -&gt; 197-W (22)
+44-D (22)
+98-L (22)
+110-M (11) -&gt; 174-T (11)
+156-S (8) -&gt; 168-S (8) -&gt; 132-P (7)
+25-C (22)
+153-S (22)
+207-Y (22)
+18-B (11) -&gt; 200-W (10)
+59-G (22)
+68-G (7) -&gt; 1-A (6) -&gt; 112-M (9)
+62-G (7) -&gt; 155-S (1) -&gt; 87-K (1) -&gt; 57-F (15)
+17-B (20) -&gt; 164-S (1)
+101-L (14) -&gt; 95-K (0) -&gt; 75-H (5)
+4-A (1) -&gt; 8-B (22) -&gt; 55-E (22)
+3-A (15) -&gt; 19-B (19)
+Rigid (capacity 16):
+9-B (7) -&gt; 48-D (5)
+34-C (14)
+196-W (16)
+199-W (6) -&gt; 74-G (7) -&gt; 192-V (16)
+63-G (16)
+38-C (16)
+93-K (2) -&gt; 131-P (14)
+83-H (15)
+66-G (16)
+97-K (16)
+92-K (13) -&gt; 66-G (16)
+7-B (13)
+83-H (0)
+120-O (13) -&gt; 198-W (6)
+96-K (15)
+46-D (16)
+188-V (14) -&gt; 39-C (2)
+151-R (16)
+108-M (11) -&gt; 120-O (0) -&gt; 62-G (0)
+168-S (0) -&gt; 19-B (0)
+166-S (9)
+151-R (8)
+75-H (0)
+11 Metre (capacity 30):
+81-H (28) -&gt; 91-K (8)
+55-E (15)
+77-H (30)
+187-V (8) -&gt; 6-B (22)
+159-S (15) -&gt; 40-C (16) -&gt; 194-V (30)
+150-R (10) -&gt; 172-S (4) -&gt; 149-R (30)
+194-V (8)
+176-T (24) -&gt; 35-C (30)
+153-S (22)
+16-B (30)
+149-R (15) -&gt; 148-R (1)
+165-S (30)
+172-S (4)
+15-B (27)
+41-C (30)
+79-H (30)
+35-C (6)
+100-L (28)
+208-Z (30)
+24-B (20) -&gt; 209-Z (10)
+104-M (27)
+139-P (15) -&gt; 41-C (12)
+82-H (17) -&gt; 197-W (30)
+29-C (28)
+157-S (17) -&gt; 182-U (12) -&gt; 88-K (1)
+117-N (5) -&gt; 126-P (14) -&gt; 125-P (11)
+119-O (12) -&gt; 2-A (0)
+121-O (13) -&gt; 143-P (12) -&gt; 193-V (18) -&gt; 19-B (0)
+66-G (30)
+152-R (12) -&gt; 186-V (0) -&gt; 81-H (0) -&gt; 91-K (0)
+163-S (15) -&gt; 51-D (8) -&gt; 3-A (0)
+189-V (17) -&gt; 140-P (20)
+8-B (17)
+193-V (0) -&gt; 143-P (0) -&gt; 101-L (0) -&gt; 121-O (0) -&gt; 135-P (5)
+Link (capacity 40):
+40-C (40)
+138-P (1) -&gt; 137-P (38)
+</t>
+  </si>
+  <si>
+    <t>{"2": [[[17, 24], [164, 4]], [[44, 30]], [[111, 2]], [[77, 30]], [[149, 27], [148, 3]], [[165, 30]], [[159, 19], [194, 11]], [[41, 30]], [[172, 30]], [[79, 30]], [[104, 30]], [[6, 23], [187, 7]], [[176, 30]], [[153, 30]], [[208, 30]], [[35, 30]], [[100, 30]], [[19, 11]], [[83, 30]], [[40, 30]], [[117, 7], [126, 14], [125, 9]], [[121, 30]], [[143, 29]], [[193, 19]], [[80, 20]], [[168, 9]], [[135, 15]], [[182, 15]], [[95, 10]], [[81, 30]], [[121, 1]]], "1": [[[75, 19]], [[149, 22]], [[24, 8]], [[25, 14]], [[207, 21]], [[72, 22]], [[119, 10]], [[2, 12]], [[157, 22]], [[46, 20]], [[188, 22]], [[186, 9]], [[53, 12]], [[130, 22]], [[83, 10]], [[116, 10], [177, 11], [203, 1]], [[27, 22]]], "0": [[[194, 16]], [[16, 10], [165, 4]], [[156, 15], [39, 1]], [[77, 9]], [[120, 16]], [[198, 5]], [[151, 16]], [[196, 8], [48, 5]], [[34, 14]], [[9, 15]], [[154, 14]], [[8, 16]], [[108, 11]], [[152, 15]], [[120, 7]], [[101, 6], [199, 1]], [[91, 6], [81, 6]], [[197, 14]], [[131, 16]], [[151, 9]], [[173, 7]], [[144, 12]], [[166, 6], [28, 2], [3, 8]], [[97, 13]], [[66, 15]]]}</t>
+  </si>
+  <si>
+    <t>{"0": [[[182, 15]], [[197, 14]], [[34, 14]], [[19, 11]], [[2, 12]], [[8, 16]], [[131, 16]], [[154, 14]], [[108, 11]], [[196, 8], [48, 5]], [[9, 15]], [[119, 10]], [[66, 15]]], "1": [[[188, 22]], [[16, 10], [144, 12]], [[27, 22]], [[81, 14], [199, 1]], [[81, 22]], [[91, 6]], [[198, 5]], [[75, 19]], [[72, 22]], [[207, 21]], [[97, 13], [121, 22]], [[157, 22]], [[83, 22]], [[149, 22]], [[83, 18]], [[46, 20]], [[152, 15]], [[186, 9]]], "2": [[[35, 30]], [[79, 30]], [[95, 10], [28, 2]], [[208, 30]], [[135, 15], [53, 12]], [[151, 25]], [[6, 23]], [[159, 19], [173, 7]], [[101, 6], [17, 24]], [[172, 30]], [[25, 14], [24, 8], [166, 6]], [[126, 14], [117, 7], [125, 9]], [[153, 30]], [[100, 30]], [[176, 30]], [[120, 23]], [[41, 30]], [[104, 30]], [[193, 19], [3, 8]], [[168, 9], [80, 20]], [[156, 15], [39, 1], [164, 4]], [[40, 30]], [[44, 30]], [[187, 7], [116, 10], [203, 1], [177, 11]], [[194, 27]], [[130, 22]], [[149, 30], [111, 2]], [[121, 30]], [[143, 29]]], "3": [[[77, 39]], [[148, 3], [165, 34]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+182-U (15)
+197-W (14)
+34-C (14)
+19-B (11)
+2-A (12)
+8-B (16)
+131-P (16)
+154-S (14)
+108-M (11)
+196-W (8) -&gt; 48-D (5)
+9-B (15)
+119-O (10)
+66-G (15)
+8 Metre (capacity 22):
+188-V (22)
+16-B (10) -&gt; 144-Q (12)
+27-C (22)
+81-H (14) -&gt; 199-W (1)
+81-H (22)
+91-K (6)
+198-W (5)
+75-H (19)
+72-G (22)
+207-Y (21)
+97-K (13) -&gt; 121-O (22)
+157-S (22)
+83-H (22)
+149-R (22)
+83-H (18)
+46-D (20)
+152-R (15)
+186-V (9)
+11 Metre (capacity 30):
+35-C (30)
+79-H (30)
+95-K (10) -&gt; 28-C (2)
+208-Z (30)
+135-P (15) -&gt; 53-E (12)
+151-R (25)
+6-B (23)
+159-S (19) -&gt; 173-T (7)
+101-L (6) -&gt; 17-B (24)
+172-S (30)
+25-C (14) -&gt; 24-B (8) -&gt; 166-S (6)
+126-P (14) -&gt; 117-N (7) -&gt; 125-P (9)
+153-S (30)
+100-L (30)
+176-T (30)
+120-O (23)
+41-C (30)
+104-M (30)
+193-V (19) -&gt; 3-A (8)
+168-S (9) -&gt; 80-H (20)
+156-S (15) -&gt; 39-C (1) -&gt; 164-S (4)
+40-C (30)
+44-D (30)
+187-V (7) -&gt; 116-N (10) -&gt; 203-W (1) -&gt; 177-T (11)
+194-V (27)
+130-P (22)
+149-R (30) -&gt; 111-M (2)
+121-O (30)
+143-P (29)
+Link (capacity 40):
+77-H (39)
+148-R (3) -&gt; 165-S (34)
+</t>
+  </si>
+  <si>
+    <t>{"2": [[[149, 30]], [[172, 30]], [[165, 30]], [[44, 30]], [[149, 24], [148, 6]], [[159, 24], [41, 6]], [[77, 30]], [[15, 28]], [[150, 8], [172, 20]], [[98, 16], [153, 14]], [[194, 30]], [[79, 30]], [[6, 14], [135, 6]], [[187, 8], [194, 8]], [[104, 30]], [[41, 30]], [[153, 30]], [[176, 16], [35, 5], [209, 9]], [[100, 30]], [[208, 24], [152, 4]], [[16, 30]], [[24, 25], [25, 4]], [[110, 19], [174, 5], [104, 6]], [[35, 30]], [[156, 11]], [[168, 9]], [[132, 10]], [[25, 30]], [[59, 28]], [[117, 6], [126, 10], [125, 14]], [[40, 30]], [[92, 30]], [[72, 30]], [[29, 29]], [[139, 15], [40, 15]], [[121, 6], [143, 5], [193, 4], [19, 6]], [[97, 30]], [[182, 6]], [[101, 10], [75, 8]], [[33, 30]], [[4, 30]], [[49, 8]], [[197, 9]], [[32, 27]], [[81, 30]], [[8, 30]], [[55, 30]], [[97, 7]], [[140, 30]]], "0": [[[79, 7], [77, 7]], [[120, 16]], [[198, 6]], [[96, 16]], [[188, 15], [39, 1]], [[151, 15]], [[123, 2]], [[46, 16]], [[17, 15], [164, 1]], [[42, 12]], [[134, 10], [171, 2]], [[37, 10]], [[9, 10]], [[48, 5], [62, 1], [155, 1], [87, 1]], [[57, 13]], [[191, 2]], [[94, 5]], [[196, 13]], [[157, 16]], [[34, 16]], [[154, 15]], [[144, 3]], [[49, 16]], [[63, 16]], [[108, 9]], [[120, 1]], [[199, 10]], [[74, 5]], [[93, 9]], [[70, 7]], [[186, 15]], [[91, 13], [81, 2]], [[53, 13]], [[95, 15]], [[197, 16]], [[66, 13]], [[28, 7]], [[131, 12], [8, 4]], [[83, 16]]], "1": [[[207, 20]], [[83, 15]], [[2, 14]], [[82, 22]], [[119, 12]], [[68, 10]], [[1, 3]], [[18, 15], [112, 1]], [[200, 15]], [[157, 8]], [[163, 17], [3, 5]], [[192, 22]], [[66, 22]], [[38, 22]], [[33, 9]], [[4, 11]], [[88, 22]], [[3, 22]]]}</t>
+  </si>
+  <si>
+    <t>{"0": [[[143, 5], [28, 7]], [[168, 9], [39, 1]], [[156, 11]], [[200, 15]], [[95, 15]], [[134, 10]], [[37, 10]], [[93, 9]], [[196, 13]], [[154, 15]], [[74, 5]], [[151, 15]], [[2, 14]], [[63, 16]], [[70, 7]], [[66, 16]], [[186, 15]], [[91, 13]], [[121, 6], [48, 5]], [[18, 15]], [[19, 6]], [[139, 15]], [[123, 2]], [[96, 16]], [[42, 12]], [[83, 15]], [[199, 10]], [[198, 6]], [[1, 3]]], "1": [[[82, 22]], [[4, 22]], [[110, 19]], [[125, 14], [97, 22]], [[119, 12]]], "2": [[[92, 30]], [[16, 30]], [[194, 30]], [[49, 24], [164, 1]], [[132, 10], [101, 10]], [[150, 8], [172, 30]], [[104, 0]], [[35, 30]], [[25, 30]], [[149, 30]], [[172, 20]], [[159, 24]], [[97, 30]], [[41, 30]], [[35, 5], [144, 3], [176, 16]], [[100, 30]], [[87, 1], [57, 13], [94, 5], [62, 1], [155, 1]], [[34, 16], [112, 1]], [[59, 28]], [[108, 9], [152, 4]], [[209, 9], [117, 6], [126, 10]], [[40, 30]], [[197, 25]], [[165, 30]], [[104, 0], [41, 6], [40, 15]], [[120, 17]], [[9, 10], [17, 15]], [[188, 15]], [[157, 24], [182, 6]], [[38, 22], [81, 30]], [[33, 9], [53, 13]], [[131, 12], [83, 30]], [[208, 24]], [[68, 10]], [[33, 30]], [[29, 29]], [[153, 30]], [[207, 20], [135, 6]], [[24, 25], [25, 4]], [[4, 30]], [[8, 30]], [[192, 22], [171, 2]], [[81, 2]], [[153, 14], [98, 16]], [[72, 30]], [[3, 27]], [[75, 8], [163, 17], [8, 4]], [[6, 14], [194, 8], [187, 8]], [[174, 5]], [[15, 28]], [[88, 22], [191, 2], [193, 4]], [[44, 30]], [[148, 6], [149, 24]], [[140, 30]], [[32, 27]], [[55, 30]]], "3": [[[46, 16], [66, 35]], [[77, 37]], [[79, 37]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+143-P (5) -&gt; 28-C (7)
+168-S (9) -&gt; 39-C (1)
+156-S (11)
+200-W (15)
+95-K (15)
+134-P (10)
+37-C (10)
+93-K (9)
+196-W (13)
+154-S (15)
+74-G (5)
+151-R (15)
+2-A (14)
+63-G (16)
+70-G (7)
+66-G (16)
+186-V (15)
+91-K (13)
+121-O (6) -&gt; 48-D (5)
+18-B (15)
+19-B (6)
+139-P (15)
+123-O (2)
+96-K (16)
+42-C (12)
+83-H (15)
+199-W (10)
+198-W (6)
+1-A (3)
+8 Metre (capacity 22):
+82-H (22)
+4-A (22)
+110-M (19)
+125-P (14) -&gt; 97-K (22)
+119-O (12)
+11 Metre (capacity 30):
+92-K (30)
+16-B (30)
+194-V (30)
+49-D (24) -&gt; 164-S (1)
+132-P (10) -&gt; 101-L (10)
+150-R (8) -&gt; 172-S (30)
+104-M (0)
+35-C (30)
+25-C (30)
+149-R (30)
+172-S (20)
+159-S (24)
+97-K (30)
+41-C (30)
+35-C (5) -&gt; 144-Q (3) -&gt; 176-T (16)
+100-L (30)
+87-K (1) -&gt; 57-F (13) -&gt; 94-K (5) -&gt; 62-G (1) -&gt; 155-S (1)
+34-C (16) -&gt; 112-M (1)
+59-G (28)
+108-M (9) -&gt; 152-R (4)
+209-Z (9) -&gt; 117-N (6) -&gt; 126-P (10)
+40-C (30)
+197-W (25)
+165-S (30)
+104-M (0) -&gt; 41-C (6) -&gt; 40-C (15)
+120-O (17)
+9-B (10) -&gt; 17-B (15)
+188-V (15)
+157-S (24) -&gt; 182-U (6)
+38-C (22) -&gt; 81-H (30)
+33-C (9) -&gt; 53-E (13)
+131-P (12) -&gt; 83-H (30)
+208-Z (24)
+68-G (10)
+33-C (30)
+29-C (29)
+153-S (30)
+207-Y (20) -&gt; 135-P (6)
+24-B (25) -&gt; 25-C (4)
+4-A (30)
+8-B (30)
+192-V (22) -&gt; 171-S (2)
+81-H (2)
+153-S (14) -&gt; 98-L (16)
+72-G (30)
+3-A (27)
+75-H (8) -&gt; 163-S (17) -&gt; 8-B (4)
+6-B (14) -&gt; 194-V (8) -&gt; 187-V (8)
+174-T (5)
+15-B (28)
+88-K (22) -&gt; 191-V (2) -&gt; 193-V (4)
+44-D (30)
+148-R (6) -&gt; 149-R (24)
+140-P (30)
+32-C (27)
+55-E (30)
+Link (capacity 40):
+46-D (16) -&gt; 66-G (35)
+77-H (37)
+79-H (37)
+</t>
+  </si>
+  <si>
+    <t>{"3": [[[92, 32]], [[22, 40]], [[41, 39]], [[23, 40]], [[85, 23]]], "1": [[[156, 7]], [[17, 16]], [[197, 11]], [[207, 22]], [[83, 22]], [[119, 12]], [[2, 10]], [[46, 22]], [[188, 22]], [[151, 22]], [[56, 11]], [[118, 9]], [[72, 15]], [[58, 15], [22, 3]], [[142, 22]], [[50, 2]], [[78, 6]], [[113, 4]], [[94, 6], [102, 4]], [[35, 21]], [[163, 18]], [[186, 22]], [[205, 9], [206, 7]], [[144, 21], [106, 1]], [[135, 2]], [[151, 22]], [[173, 13], [131, 7]], [[40, 22]], [[57, 21]], [[89, 22]], [[158, 22]], [[84, 22]]], "2": [[[59, 30]], [[154, 1]], [[68, 8]], [[1, 30]], [[72, 30]], [[29, 30]], [[18, 24]], [[200, 13]], [[96, 29]], [[152, 4]], [[15, 26]], [[139, 30]], [[24, 9], [25, 7], [59, 11]], [[40, 30]], [[117, 2], [126, 14], [125, 14]], [[157, 26]], [[95, 18]], [[135, 30]], [[33, 10]], [[182, 17]], [[121, 29]], [[143, 30]], [[66, 19]], [[168, 24]], [[69, 30]], [[153, 30]], [[91, 30]], [[49, 30]], [[208, 30]], [[29, 30]], [[1, 11]], [[12, 30]], [[81, 5]], [[91, 20]], [[193, 19]], [[19, 14]], [[101, 21]], [[104, 12], [100, 15], [153, 3]], [[95, 30]], [[201, 30]], [[111, 30]], [[99, 30]], [[124, 30]], [[150, 30]], [[109, 30]], [[104, 30]], [[15, 30]], [[98, 30]], [[99, 10], [26, 20]], [[149, 30]], [[150, 19], [149, 7], [165, 4]], [[110, 7], [176, 8], [174, 14], [60, 1]], [[172, 20], [111, 10]], [[109, 28]], [[156, 30]], [[132, 15]], [[10, 30]], [[76, 20], [10, 10]], [[17, 30]], [[164, 2]], [[53, 27]], [[130, 19]], [[3, 30]], [[51, 16]], [[29, 8]], [[154, 30]], [[11, 3]], [[208, 11]], [[97, 29]], [[69, 30]], [[143, 3]], [[178, 28]], [[61, 2], [45, 13]], [[175, 23]], [[185, 22]], [[28, 28]], [[69, 30]], [[147, 7]], [[85, 30]], [[20, 30]], [[84, 30]], [[116, 5]], [[85, 30]], [[20, 18]]], "0": [[[7, 4], [188, 4], [39, 5]], [[120, 9]], [[198, 13]], [[80, 16]], [[69, 16]], [[134, 16]], [[92, 16]], [[112, 2], [42, 1]], [[62, 13], [155, 1], [87, 2]], [[47, 12], [166, 4]], [[128, 16]], [[105, 5], [46, 2]], [[115, 7]], [[191, 4]], [[48, 10]], [[186, 16]], [[134, 5]], [[171, 5]], [[93, 10]], [[151, 4]], [[8, 5]], [[142, 4]], [[12, 1]], [[13, 16]], [[9, 11], [75, 3]], [[90, 16]], [[128, 1], [195, 1]], [[83, 16]], [[69, 6]], [[158, 13]]]}</t>
+  </si>
+  <si>
+    <t>{"0": [[[151, 16]], [[1, 16]], [[154, 15]], [[100, 15]], [[157, 16]], [[24, 9]], [[50, 2]], [[83, 16]], [[131, 7]], [[125, 14]], [[173, 13]], [[29, 16]], [[130, 3]], [[2, 10]], [[119, 12]], [[151, 16]], [[105, 5]], [[29, 16]], [[156, 15]], [[19, 14]], [[29, 4]], [[48, 10], [164, 2]], [[154, 15], [195, 1]], [[7, 4], [39, 5]], [[93, 10]], [[174, 14]], [[8, 5], [130, 3]], [[117, 2], [126, 14]], [[47, 12]], [[113, 4]], [[33, 10]], [[186, 6]], [[151, 16]], [[78, 6]], [[120, 9]], [[17, 16]], [[68, 8]], [[1, 16]], [[198, 13]], [[15, 16]], [[72, 16]], [[200, 13]], [[13, 16]], [[153, 1]], [[90, 16]], [[171, 5]], [[69, 16]], [[56, 11]], [[152, 4]], [[197, 11]]], "1": [[[69, 22]], [[15, 22]], [[153, 22]], [[91, 22]], [[156, 22]], [[80, 16]], [[15, 18]], [[157, 22]], [[69, 22]], [[57, 21], [12, 1]], [[92, 22]], [[95, 22]], [[185, 22]], [[193, 19]], [[134, 21]], [[69, 22]]], "2": [[[208, 30]], [[49, 30]], [[158, 5], [84, 22], [60, 1]], [[3, 30]], [[9, 11], [51, 16]], [[29, 20]], [[168, 24]], [[142, 26]], [[104, 30]], [[207, 22]], [[188, 26]], [[62, 13], [155, 1], [102, 4], [94, 6]], [[46, 24]], [[59, 11], [58, 15]], [[149, 30]], [[201, 30]], [[85, 30]], [[158, 30]], [[89, 22], [112, 2]], [[40, 30]], [[109, 28]], [[84, 30]], [[95, 30], [11, 3]], [[17, 30]], [[97, 29]], [[66, 19], [81, 5]], [[186, 22]], [[20, 30]], [[1, 9]], [[10, 10], [76, 20]], [[96, 29]], [[144, 21]], [[85, 30]], [[40, 22], [42, 1]], [[98, 30]], [[205, 9], [150, 19], [61, 2]], [[191, 4], [128, 17]], [[135, 30]], [[85, 23], [147, 7]], [[12, 30]], [[92, 30]], [[22, 30]], [[59, 30]], [[132, 15]], [[104, 12], [110, 7]], [[10, 30]], [[69, 30]], [[182, 17]], [[35, 21], [176, 8]], [[139, 30]], [[91, 30]], [[18, 24]], [[72, 29]], [[118, 9], [143, 3], [163, 18]], [[87, 2]], [[115, 7]], [[124, 30]], [[109, 30]], [[106, 1], [22, 13]], [[28, 28]], [[101, 21]], [[178, 28]], [[166, 4], [175, 23]], [[45, 13], [25, 7]], [[83, 22]], [[143, 30]], [[150, 30]], [[20, 18], [116, 5]], [[149, 7], [26, 20]], [[135, 2], [53, 27]], [[121, 29]]], "3": [[[206, 7], [165, 4], [172, 20]], [[208, 11], [75, 3]], [[111, 40]], [[99, 40]], [[23, 40]], [[41, 39]]]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid (capacity 16):
+151-R (16)
+1-A (16)
+154-S (15)
+100-L (15)
+157-S (16)
+24-B (9)
+50-D (2)
+83-H (16)
+131-P (7)
+125-P (14)
+173-T (13)
+29-C (16)
+130-P (3)
+2-A (10)
+119-O (12)
+151-R (16)
+105-M (5)
+29-C (16)
+156-S (15)
+19-B (14)
+29-C (4)
+48-D (10) -&gt; 164-S (2)
+154-S (15) -&gt; 195-W (1)
+7-B (4) -&gt; 39-C (5)
+93-K (10)
+174-T (14)
+8-B (5) -&gt; 130-P (3)
+117-N (2) -&gt; 126-P (14)
+47-D (12)
+113-M (4)
+33-C (10)
+186-V (6)
+151-R (16)
+78-H (6)
+120-O (9)
+17-B (16)
+68-G (8)
+1-A (16)
+198-W (13)
+15-B (16)
+72-G (16)
+200-W (13)
+13-B (16)
+153-S (1)
+90-K (16)
+171-S (5)
+69-G (16)
+56-F (11)
+152-R (4)
+197-W (11)
+8 Metre (capacity 22):
+69-G (22)
+15-B (22)
+153-S (22)
+91-K (22)
+156-S (22)
+80-H (16)
+15-B (18)
+157-S (22)
+69-G (22)
+57-F (21) -&gt; 12-B (1)
+92-K (22)
+95-K (22)
+185-V (22)
+193-V (19)
+134-P (21)
+69-G (22)
+11 Metre (capacity 30):
+208-Z (30)
+49-D (30)
+158-S (5) -&gt; 84-K (22) -&gt; 60-G (1)
+3-A (30)
+9-B (11) -&gt; 51-D (16)
+29-C (20)
+168-S (24)
+142-P (26)
+104-M (30)
+207-Y (22)
+188-V (26)
+62-G (13) -&gt; 155-S (1) -&gt; 102-L (4) -&gt; 94-K (6)
+46-D (24)
+59-G (11) -&gt; 58-G (15)
+149-R (30)
+201-W (30)
+85-K (30)
+158-S (30)
+89-K (22) -&gt; 112-M (2)
+40-C (30)
+109-M (28)
+84-K (30)
+95-K (30) -&gt; 11-B (3)
+17-B (30)
+97-K (29)
+66-G (19) -&gt; 81-H (5)
+186-V (22)
+20-B (30)
+1-A (9)
+10-B (10) -&gt; 76-H (20)
+96-K (29)
+144-Q (21)
+85-K (30)
+40-C (22) -&gt; 42-C (1)
+98-L (30)
+205-W (9) -&gt; 150-R (19) -&gt; 61-G (2)
+191-V (4) -&gt; 128-P (17)
+135-P (30)
+85-K (23) -&gt; 147-R (7)
+12-B (30)
+92-K (30)
+22-B (30)
+59-G (30)
+132-P (15)
+104-M (12) -&gt; 110-M (7)
+10-B (30)
+69-G (30)
+182-U (17)
+35-C (21) -&gt; 176-T (8)
+139-P (30)
+91-K (30)
+18-B (24)
+72-G (29)
+118-N (9) -&gt; 143-P (3) -&gt; 163-S (18)
+87-K (2)
+115-N (7)
+124-O (30)
+109-M (30)
+106-M (1) -&gt; 22-B (13)
+28-C (28)
+101-L (21)
+178-T (28)
+166-S (4) -&gt; 175-T (23)
+45-D (13) -&gt; 25-C (7)
+83-H (22)
+143-P (30)
+150-R (30)
+20-B (18) -&gt; 116-N (5)
+149-R (7) -&gt; 26-C (20)
+135-P (2) -&gt; 53-E (27)
+121-O (29)
+Link (capacity 40):
+206-W (7) -&gt; 165-S (4) -&gt; 172-S (20)
+208-Z (11) -&gt; 75-H (3)
+111-M (40)
+99-L (40)
+23-B (40)
+41-C (39)
+</t>
+  </si>
+  <si>
+    <t>Seeded solutions will be split again if customer completion changed their chromosomes (I am also regenerating the model data sheets just in case of errors).</t>
   </si>
 </sst>
 </file>
@@ -4332,7 +5096,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6705-486E-A71D-F6CCB68D3CE8}"/>
+              <c16:uniqueId val="{00000000-2D52-4DF8-A7CD-61A1A5E857FE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4405,7 +5169,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6705-486E-A71D-F6CCB68D3CE8}"/>
+              <c16:uniqueId val="{00000001-2D52-4DF8-A7CD-61A1A5E857FE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4743,7 +5507,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0B1D-43EA-B535-E58CBDCA2CA1}"/>
+              <c16:uniqueId val="{00000000-CF65-42E6-B8A5-AE907BBEF5B2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4816,7 +5580,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0B1D-43EA-B535-E58CBDCA2CA1}"/>
+              <c16:uniqueId val="{00000001-CF65-42E6-B8A5-AE907BBEF5B2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5155,7 +5919,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C73E-4D2F-9410-5BA422F19426}"/>
+              <c16:uniqueId val="{00000000-2BB3-4E34-914F-FAB19C30DA6C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5228,7 +5992,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C73E-4D2F-9410-5BA422F19426}"/>
+              <c16:uniqueId val="{00000001-2BB3-4E34-914F-FAB19C30DA6C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5552,7 +6316,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E006-472A-801A-EE9D1860B66A}"/>
+              <c16:uniqueId val="{00000000-2B3E-4C8A-BF0E-0649C35ADAFA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5611,7 +6375,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E006-472A-801A-EE9D1860B66A}"/>
+              <c16:uniqueId val="{00000001-2B3E-4C8A-BF0E-0649C35ADAFA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5948,7 +6712,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DFC2-4D3C-9D65-4FB52F68F248}"/>
+              <c16:uniqueId val="{00000000-8D9C-4A93-B830-DD2A0ADF47BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6021,7 +6785,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DFC2-4D3C-9D65-4FB52F68F248}"/>
+              <c16:uniqueId val="{00000001-8D9C-4A93-B830-DD2A0ADF47BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6358,7 +7122,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0790-494B-8661-29D8889F656B}"/>
+              <c16:uniqueId val="{00000000-31AB-4365-9847-D4C31E726078}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6431,7 +7195,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0790-494B-8661-29D8889F656B}"/>
+              <c16:uniqueId val="{00000001-31AB-4365-9847-D4C31E726078}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6485,7 +7249,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0790-494B-8661-29D8889F656B}"/>
+              <c16:uniqueId val="{00000002-31AB-4365-9847-D4C31E726078}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6539,7 +7303,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0790-494B-8661-29D8889F656B}"/>
+              <c16:uniqueId val="{00000003-31AB-4365-9847-D4C31E726078}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7694,7 +8458,7 @@
   <dimension ref="A1:V208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="O29" sqref="O29"/>
@@ -12442,10 +13206,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12461,7 +13225,7 @@
     <col min="9" max="9" width="12.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.7109375" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -12499,7 +13263,7 @@
         <v>217</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -12507,13 +13271,13 @@
         <v>43745</v>
       </c>
       <c r="B2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C2">
         <v>469154.88979999977</v>
       </c>
       <c r="F2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G2">
         <v>3603.7618333999999</v>
@@ -12526,7 +13290,7 @@
         <v>13622.672333333176</v>
       </c>
       <c r="K2" s="12">
-        <f t="shared" ref="K2:K9" si="0">J2/C2</f>
+        <f t="shared" ref="K2:K18" si="0">J2/C2</f>
         <v>2.9036620164271349E-2</v>
       </c>
     </row>
@@ -12535,13 +13299,13 @@
         <v>43768</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C3">
         <v>592286.43533333309</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G3">
         <v>3600.6243162000001</v>
@@ -12558,7 +13322,7 @@
         <v>-2.8570731981184649E-2</v>
       </c>
       <c r="L3" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -12566,16 +13330,16 @@
         <v>43775</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C4">
         <v>471229.1394000001</v>
       </c>
       <c r="E4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G4">
         <v>3893.4923675999999</v>
@@ -12584,7 +13348,7 @@
         <v>468885.14206666662</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J9" si="1">C4-(H4+I4*10)</f>
+        <f t="shared" ref="J4:J18" si="1">C4-(H4+I4*10)</f>
         <v>2343.9973333334783</v>
       </c>
       <c r="K4" s="12">
@@ -12597,16 +13361,16 @@
         <v>43775</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C5">
         <v>1428685.831666667</v>
       </c>
       <c r="E5" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G5">
         <v>3661.4549959999999</v>
@@ -12623,7 +13387,7 @@
         <v>0.11307985414694049</v>
       </c>
       <c r="L5" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -12631,16 +13395,16 @@
         <v>43768</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C6">
         <v>592286.43533333309</v>
       </c>
       <c r="E6" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F6" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G6">
         <v>3786.4904317999999</v>
@@ -12662,16 +13426,16 @@
         <v>43745</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C7">
         <v>469154.88979999977</v>
       </c>
       <c r="E7" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F7" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G7">
         <v>3601.0539597000002</v>
@@ -12693,16 +13457,16 @@
         <v>43795</v>
       </c>
       <c r="B8" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C8">
         <v>1275847.0800666669</v>
       </c>
       <c r="E8" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="G8">
         <v>3902.6114637000001</v>
@@ -12724,16 +13488,16 @@
         <v>43768</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C9">
         <v>592286.43533333309</v>
       </c>
       <c r="E9" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="G9">
         <v>7200.1489792000002</v>
@@ -12755,16 +13519,16 @@
         <v>43745</v>
       </c>
       <c r="B10" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C10">
         <v>475403.35446666653</v>
       </c>
       <c r="E10" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F10" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="G10">
         <v>3601.0659418</v>
@@ -12772,16 +13536,16 @@
       <c r="H10">
         <v>415161.92479999957</v>
       </c>
-      <c r="J10" s="11">
-        <f t="shared" ref="J10:J11" si="2">C10-(H10+I10*10)</f>
+      <c r="J10">
+        <f t="shared" si="1"/>
         <v>60241.429666666954</v>
       </c>
       <c r="K10" s="12">
-        <f t="shared" ref="K10:K11" si="3">J10/C10</f>
+        <f t="shared" si="0"/>
         <v>0.12671645898302314</v>
       </c>
       <c r="L10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -12789,16 +13553,16 @@
         <v>43768</v>
       </c>
       <c r="B11" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C11">
         <v>600912.63166666601</v>
       </c>
       <c r="E11" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="F11" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G11">
         <v>3600.2064667</v>
@@ -12806,12 +13570,12 @@
       <c r="H11">
         <v>609615.0336666666</v>
       </c>
-      <c r="J11" s="11">
-        <f t="shared" si="2"/>
+      <c r="J11">
+        <f t="shared" si="1"/>
         <v>-8702.4020000005839</v>
       </c>
       <c r="K11" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>-1.4481975484296224E-2</v>
       </c>
     </row>
@@ -12819,18 +13583,223 @@
       <c r="A12" s="9">
         <v>43745</v>
       </c>
+      <c r="B12" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12">
+        <v>494345.58179999999</v>
+      </c>
+      <c r="E12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F12" t="s">
+        <v>249</v>
+      </c>
+      <c r="G12">
+        <v>7170.8296077000005</v>
+      </c>
+      <c r="H12">
+        <v>462138.49680000002</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>32207.084999999963</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="0"/>
+        <v>6.5150951451266648E-2</v>
+      </c>
       <c r="L12" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>43768</v>
       </c>
+      <c r="B13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13">
+        <v>593149.57433333329</v>
+      </c>
+      <c r="E13" t="s">
+        <v>252</v>
+      </c>
+      <c r="F13" t="s">
+        <v>253</v>
+      </c>
+      <c r="G13">
+        <v>5056.3446751000001</v>
+      </c>
+      <c r="H13">
+        <v>593149.57433333329</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>43795</v>
+      </c>
+      <c r="B14" t="s">
+        <v>254</v>
+      </c>
+      <c r="C14">
+        <v>1372973.317933334</v>
+      </c>
+      <c r="E14" t="s">
+        <v>255</v>
+      </c>
+      <c r="F14" t="s">
+        <v>256</v>
+      </c>
+      <c r="G14">
+        <v>7318.0830248000002</v>
+      </c>
+      <c r="H14">
+        <v>1254723.0476333329</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>118250.27030000114</v>
+      </c>
+      <c r="K14" s="12">
+        <f t="shared" si="0"/>
+        <v>8.6127143736483655E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>43754</v>
+      </c>
+      <c r="B15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15">
+        <v>636315.92813333333</v>
+      </c>
+      <c r="E15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F15" t="s">
+        <v>259</v>
+      </c>
+      <c r="G15">
+        <v>4347.3198690999998</v>
+      </c>
+      <c r="H15">
+        <v>636315.92813333333</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>43745</v>
+      </c>
+      <c r="B16" t="s">
+        <v>260</v>
+      </c>
+      <c r="C16">
+        <v>538213.87013333349</v>
+      </c>
+      <c r="E16" t="s">
+        <v>261</v>
+      </c>
+      <c r="F16" t="s">
+        <v>262</v>
+      </c>
+      <c r="G16">
+        <v>7527.1272962000003</v>
+      </c>
+      <c r="H16">
+        <v>464391.88160000002</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>73821.988533333468</v>
+      </c>
+      <c r="K16" s="12">
+        <f t="shared" si="0"/>
+        <v>0.13716106668719871</v>
+      </c>
+      <c r="L16" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>43768</v>
+      </c>
+      <c r="B17" t="s">
+        <v>263</v>
+      </c>
+      <c r="C17">
+        <v>632705.85299999989</v>
+      </c>
+      <c r="E17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F17" t="s">
+        <v>265</v>
+      </c>
+      <c r="G17">
+        <v>6666.2375192999998</v>
+      </c>
+      <c r="H17">
+        <v>590658.45699999982</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>42047.396000000066</v>
+      </c>
+      <c r="K17" s="12">
+        <f t="shared" si="0"/>
+        <v>6.6456467568034458E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>43795</v>
+      </c>
+      <c r="B18" t="s">
+        <v>266</v>
+      </c>
+      <c r="C18">
+        <v>1432583.6294</v>
+      </c>
+      <c r="E18" t="s">
+        <v>267</v>
+      </c>
+      <c r="F18" t="s">
+        <v>268</v>
+      </c>
+      <c r="G18">
+        <v>7733.803919</v>
+      </c>
+      <c r="H18">
+        <v>1254822.7691666661</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>177760.86023333389</v>
+      </c>
+      <c r="K18" s="12">
+        <f t="shared" si="0"/>
+        <v>0.12408410691373345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>